<commit_message>
fix link & faq saving issue
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Customers.xlsx
+++ b/EDI/Web/wwwroot/Upload/Customers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>School Name</t>
   </si>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB628"/>
+  <dimension ref="A1:AB636"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1116,36 +1116,6 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="20">
-        <v>42299</v>
-      </c>
-      <c r="K12" s="21">
-        <v>200122609501901</v>
-      </c>
       <c r="Q12"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -1158,36 +1128,6 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="20">
-        <v>41876</v>
-      </c>
-      <c r="K13" s="21">
-        <v>200122604903901</v>
-      </c>
       <c r="Q13"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -1199,37 +1139,7 @@
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="20">
-        <v>42113</v>
-      </c>
-      <c r="K14" s="21">
-        <v>200122699902901</v>
-      </c>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Q14"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1399,7 +1309,6 @@
     </row>
     <row r="28" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q28"/>
-      <c r="R28" s="12"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -1496,6 +1405,7 @@
     </row>
     <row r="36" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q36"/>
+      <c r="R36" s="12"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -1687,9 +1597,7 @@
       <c r="AB51" s="4"/>
     </row>
     <row r="52" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P52" s="3"/>
       <c r="Q52"/>
-      <c r="R52" s="12"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -1785,7 +1693,9 @@
       <c r="AB59" s="4"/>
     </row>
     <row r="60" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P60" s="3"/>
       <c r="Q60"/>
+      <c r="R60" s="12"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="3"/>
@@ -1929,9 +1839,7 @@
       <c r="AB71" s="4"/>
     </row>
     <row r="72" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P72" s="3"/>
       <c r="Q72"/>
-      <c r="R72" s="12"/>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
@@ -2016,7 +1924,6 @@
     </row>
     <row r="79" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q79"/>
-      <c r="R79" s="12"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
@@ -2028,7 +1935,9 @@
       <c r="AB79" s="4"/>
     </row>
     <row r="80" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P80" s="3"/>
       <c r="Q80"/>
+      <c r="R80" s="12"/>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
@@ -2112,7 +2021,6 @@
       <c r="AB86" s="4"/>
     </row>
     <row r="87" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P87" s="3"/>
       <c r="Q87"/>
       <c r="R87" s="12"/>
       <c r="T87" s="3"/>
@@ -2210,7 +2118,9 @@
       <c r="AB94" s="4"/>
     </row>
     <row r="95" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P95" s="3"/>
       <c r="Q95"/>
+      <c r="R95" s="12"/>
       <c r="T95" s="3"/>
       <c r="U95" s="3"/>
       <c r="V95" s="3"/>
@@ -2233,7 +2143,7 @@
       <c r="AA96" s="4"/>
       <c r="AB96" s="4"/>
     </row>
-    <row r="97" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q97"/>
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
@@ -2245,7 +2155,7 @@
       <c r="AA97" s="4"/>
       <c r="AB97" s="4"/>
     </row>
-    <row r="98" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q98"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -2257,7 +2167,7 @@
       <c r="AA98" s="4"/>
       <c r="AB98" s="4"/>
     </row>
-    <row r="99" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q99"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -2269,9 +2179,8 @@
       <c r="AA99" s="4"/>
       <c r="AB99" s="4"/>
     </row>
-    <row r="100" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="100" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q100"/>
-      <c r="R100" s="12"/>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
       <c r="V100" s="3"/>
@@ -2282,7 +2191,7 @@
       <c r="AA100" s="4"/>
       <c r="AB100" s="4"/>
     </row>
-    <row r="101" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q101"/>
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
@@ -2294,7 +2203,7 @@
       <c r="AA101" s="4"/>
       <c r="AB101" s="4"/>
     </row>
-    <row r="102" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q102"/>
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
@@ -2306,7 +2215,7 @@
       <c r="AA102" s="4"/>
       <c r="AB102" s="4"/>
     </row>
-    <row r="103" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q103"/>
       <c r="T103" s="3"/>
       <c r="U103" s="3"/>
@@ -2318,7 +2227,7 @@
       <c r="AA103" s="4"/>
       <c r="AB103" s="4"/>
     </row>
-    <row r="104" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q104"/>
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
@@ -2330,7 +2239,7 @@
       <c r="AA104" s="4"/>
       <c r="AB104" s="4"/>
     </row>
-    <row r="105" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q105"/>
       <c r="T105" s="3"/>
       <c r="U105" s="3"/>
@@ -2342,7 +2251,7 @@
       <c r="AA105" s="4"/>
       <c r="AB105" s="4"/>
     </row>
-    <row r="106" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q106"/>
       <c r="T106" s="3"/>
       <c r="U106" s="3"/>
@@ -2354,7 +2263,7 @@
       <c r="AA106" s="4"/>
       <c r="AB106" s="4"/>
     </row>
-    <row r="107" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q107"/>
       <c r="T107" s="3"/>
       <c r="U107" s="3"/>
@@ -2366,8 +2275,7 @@
       <c r="AA107" s="4"/>
       <c r="AB107" s="4"/>
     </row>
-    <row r="108" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P108" s="3"/>
+    <row r="108" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q108"/>
       <c r="R108" s="12"/>
       <c r="T108" s="3"/>
@@ -2380,7 +2288,7 @@
       <c r="AA108" s="4"/>
       <c r="AB108" s="4"/>
     </row>
-    <row r="109" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q109"/>
       <c r="T109" s="3"/>
       <c r="U109" s="3"/>
@@ -2392,7 +2300,7 @@
       <c r="AA109" s="4"/>
       <c r="AB109" s="4"/>
     </row>
-    <row r="110" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q110"/>
       <c r="T110" s="3"/>
       <c r="U110" s="3"/>
@@ -2404,7 +2312,7 @@
       <c r="AA110" s="4"/>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q111"/>
       <c r="T111" s="3"/>
       <c r="U111" s="3"/>
@@ -2416,7 +2324,7 @@
       <c r="AA111" s="4"/>
       <c r="AB111" s="4"/>
     </row>
-    <row r="112" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q112"/>
       <c r="T112" s="3"/>
       <c r="U112" s="3"/>
@@ -2428,7 +2336,7 @@
       <c r="AA112" s="4"/>
       <c r="AB112" s="4"/>
     </row>
-    <row r="113" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q113"/>
       <c r="T113" s="3"/>
       <c r="U113" s="3"/>
@@ -2440,7 +2348,7 @@
       <c r="AA113" s="4"/>
       <c r="AB113" s="4"/>
     </row>
-    <row r="114" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q114"/>
       <c r="T114" s="3"/>
       <c r="U114" s="3"/>
@@ -2452,7 +2360,7 @@
       <c r="AA114" s="4"/>
       <c r="AB114" s="4"/>
     </row>
-    <row r="115" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q115"/>
       <c r="T115" s="3"/>
       <c r="U115" s="3"/>
@@ -2464,8 +2372,10 @@
       <c r="AA115" s="4"/>
       <c r="AB115" s="4"/>
     </row>
-    <row r="116" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P116" s="3"/>
       <c r="Q116"/>
+      <c r="R116" s="12"/>
       <c r="T116" s="3"/>
       <c r="U116" s="3"/>
       <c r="V116" s="3"/>
@@ -2476,7 +2386,7 @@
       <c r="AA116" s="4"/>
       <c r="AB116" s="4"/>
     </row>
-    <row r="117" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q117"/>
       <c r="T117" s="3"/>
       <c r="U117" s="3"/>
@@ -2488,7 +2398,7 @@
       <c r="AA117" s="4"/>
       <c r="AB117" s="4"/>
     </row>
-    <row r="118" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q118"/>
       <c r="T118" s="3"/>
       <c r="U118" s="3"/>
@@ -2500,7 +2410,7 @@
       <c r="AA118" s="4"/>
       <c r="AB118" s="4"/>
     </row>
-    <row r="119" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q119"/>
       <c r="T119" s="3"/>
       <c r="U119" s="3"/>
@@ -2512,7 +2422,7 @@
       <c r="AA119" s="4"/>
       <c r="AB119" s="4"/>
     </row>
-    <row r="120" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q120"/>
       <c r="T120" s="3"/>
       <c r="U120" s="3"/>
@@ -2524,9 +2434,8 @@
       <c r="AA120" s="4"/>
       <c r="AB120" s="4"/>
     </row>
-    <row r="121" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q121"/>
-      <c r="R121" s="12"/>
       <c r="T121" s="3"/>
       <c r="U121" s="3"/>
       <c r="V121" s="3"/>
@@ -2537,7 +2446,7 @@
       <c r="AA121" s="4"/>
       <c r="AB121" s="4"/>
     </row>
-    <row r="122" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q122"/>
       <c r="T122" s="3"/>
       <c r="U122" s="3"/>
@@ -2549,7 +2458,7 @@
       <c r="AA122" s="4"/>
       <c r="AB122" s="4"/>
     </row>
-    <row r="123" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q123"/>
       <c r="T123" s="3"/>
       <c r="U123" s="3"/>
@@ -2561,7 +2470,7 @@
       <c r="AA123" s="4"/>
       <c r="AB123" s="4"/>
     </row>
-    <row r="124" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q124"/>
       <c r="T124" s="3"/>
       <c r="U124" s="3"/>
@@ -2573,7 +2482,7 @@
       <c r="AA124" s="4"/>
       <c r="AB124" s="4"/>
     </row>
-    <row r="125" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q125"/>
       <c r="T125" s="3"/>
       <c r="U125" s="3"/>
@@ -2585,7 +2494,7 @@
       <c r="AA125" s="4"/>
       <c r="AB125" s="4"/>
     </row>
-    <row r="126" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q126"/>
       <c r="T126" s="3"/>
       <c r="U126" s="3"/>
@@ -2597,7 +2506,7 @@
       <c r="AA126" s="4"/>
       <c r="AB126" s="4"/>
     </row>
-    <row r="127" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q127"/>
       <c r="T127" s="3"/>
       <c r="U127" s="3"/>
@@ -2609,7 +2518,7 @@
       <c r="AA127" s="4"/>
       <c r="AB127" s="4"/>
     </row>
-    <row r="128" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q128"/>
       <c r="T128" s="3"/>
       <c r="U128" s="3"/>
@@ -2623,6 +2532,7 @@
     </row>
     <row r="129" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q129"/>
+      <c r="R129" s="12"/>
       <c r="T129" s="3"/>
       <c r="U129" s="3"/>
       <c r="V129" s="3"/>
@@ -2694,9 +2604,7 @@
       <c r="AB134" s="4"/>
     </row>
     <row r="135" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P135" s="3"/>
       <c r="Q135"/>
-      <c r="R135" s="12"/>
       <c r="T135" s="3"/>
       <c r="U135" s="3"/>
       <c r="V135" s="3"/>
@@ -2792,7 +2700,9 @@
       <c r="AB142" s="4"/>
     </row>
     <row r="143" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P143" s="3"/>
       <c r="Q143"/>
+      <c r="R143" s="12"/>
       <c r="T143" s="3"/>
       <c r="U143" s="3"/>
       <c r="V143" s="3"/>
@@ -2840,9 +2750,7 @@
       <c r="AB146" s="4"/>
     </row>
     <row r="147" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P147" s="3"/>
       <c r="Q147"/>
-      <c r="R147" s="12"/>
       <c r="T147" s="3"/>
       <c r="U147" s="3"/>
       <c r="V147" s="3"/>
@@ -2938,7 +2846,9 @@
       <c r="AB154" s="4"/>
     </row>
     <row r="155" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P155" s="3"/>
       <c r="Q155"/>
+      <c r="R155" s="12"/>
       <c r="T155" s="3"/>
       <c r="U155" s="3"/>
       <c r="V155" s="3"/>
@@ -3009,9 +2919,8 @@
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
     </row>
-    <row r="161" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="161" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q161"/>
-      <c r="R161" s="12"/>
       <c r="T161" s="3"/>
       <c r="U161" s="3"/>
       <c r="V161" s="3"/>
@@ -3022,7 +2931,7 @@
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
     </row>
-    <row r="162" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="162" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q162"/>
       <c r="T162" s="3"/>
       <c r="U162" s="3"/>
@@ -3034,7 +2943,7 @@
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
     </row>
-    <row r="163" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="163" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q163"/>
       <c r="T163" s="3"/>
       <c r="U163" s="3"/>
@@ -3046,7 +2955,7 @@
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
     </row>
-    <row r="164" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="164" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q164"/>
       <c r="T164" s="3"/>
       <c r="U164" s="3"/>
@@ -3058,7 +2967,7 @@
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
     </row>
-    <row r="165" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="165" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q165"/>
       <c r="T165" s="3"/>
       <c r="U165" s="3"/>
@@ -3070,7 +2979,7 @@
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
     </row>
-    <row r="166" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="166" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q166"/>
       <c r="T166" s="3"/>
       <c r="U166" s="3"/>
@@ -3082,7 +2991,7 @@
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
     </row>
-    <row r="167" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="167" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q167"/>
       <c r="T167" s="3"/>
       <c r="U167" s="3"/>
@@ -3094,7 +3003,7 @@
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
     </row>
-    <row r="168" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="168" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q168"/>
       <c r="T168" s="3"/>
       <c r="U168" s="3"/>
@@ -3106,8 +3015,9 @@
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
     </row>
-    <row r="169" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="169" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q169"/>
+      <c r="R169" s="12"/>
       <c r="T169" s="3"/>
       <c r="U169" s="3"/>
       <c r="V169" s="3"/>
@@ -3118,7 +3028,7 @@
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
     </row>
-    <row r="170" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="170" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q170"/>
       <c r="T170" s="3"/>
       <c r="U170" s="3"/>
@@ -3130,7 +3040,7 @@
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
     </row>
-    <row r="171" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="171" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q171"/>
       <c r="T171" s="3"/>
       <c r="U171" s="3"/>
@@ -3142,7 +3052,7 @@
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
     </row>
-    <row r="172" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="172" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q172"/>
       <c r="T172" s="3"/>
       <c r="U172" s="3"/>
@@ -3154,10 +3064,8 @@
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
     </row>
-    <row r="173" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P173" s="3"/>
+    <row r="173" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q173"/>
-      <c r="R173" s="12"/>
       <c r="T173" s="3"/>
       <c r="U173" s="3"/>
       <c r="V173" s="3"/>
@@ -3168,7 +3076,7 @@
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
     </row>
-    <row r="174" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="174" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q174"/>
       <c r="T174" s="3"/>
       <c r="U174" s="3"/>
@@ -3180,7 +3088,7 @@
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
     </row>
-    <row r="175" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="175" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q175"/>
       <c r="T175" s="3"/>
       <c r="U175" s="3"/>
@@ -3192,7 +3100,7 @@
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
     </row>
-    <row r="176" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="176" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q176"/>
       <c r="T176" s="3"/>
       <c r="U176" s="3"/>
@@ -3253,7 +3161,9 @@
       <c r="AB180" s="4"/>
     </row>
     <row r="181" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P181" s="3"/>
       <c r="Q181"/>
+      <c r="R181" s="12"/>
       <c r="T181" s="3"/>
       <c r="U181" s="3"/>
       <c r="V181" s="3"/>
@@ -3313,9 +3223,7 @@
       <c r="AB185" s="4"/>
     </row>
     <row r="186" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P186" s="3"/>
       <c r="Q186"/>
-      <c r="R186" s="12"/>
       <c r="T186" s="3"/>
       <c r="U186" s="3"/>
       <c r="V186" s="3"/>
@@ -3398,7 +3306,7 @@
       <c r="AA192" s="4"/>
       <c r="AB192" s="4"/>
     </row>
-    <row r="193" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="193" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q193"/>
       <c r="T193" s="3"/>
       <c r="U193" s="3"/>
@@ -3410,8 +3318,10 @@
       <c r="AA193" s="4"/>
       <c r="AB193" s="4"/>
     </row>
-    <row r="194" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="194" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P194" s="3"/>
       <c r="Q194"/>
+      <c r="R194" s="12"/>
       <c r="T194" s="3"/>
       <c r="U194" s="3"/>
       <c r="V194" s="3"/>
@@ -3422,9 +3332,8 @@
       <c r="AA194" s="4"/>
       <c r="AB194" s="4"/>
     </row>
-    <row r="195" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="195" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q195"/>
-      <c r="R195" s="12"/>
       <c r="T195" s="3"/>
       <c r="U195" s="3"/>
       <c r="V195" s="3"/>
@@ -3435,7 +3344,7 @@
       <c r="AA195" s="4"/>
       <c r="AB195" s="4"/>
     </row>
-    <row r="196" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="196" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q196"/>
       <c r="T196" s="3"/>
       <c r="U196" s="3"/>
@@ -3447,7 +3356,7 @@
       <c r="AA196" s="4"/>
       <c r="AB196" s="4"/>
     </row>
-    <row r="197" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="197" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q197"/>
       <c r="T197" s="3"/>
       <c r="U197" s="3"/>
@@ -3459,7 +3368,7 @@
       <c r="AA197" s="4"/>
       <c r="AB197" s="4"/>
     </row>
-    <row r="198" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="198" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q198"/>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
@@ -3471,7 +3380,7 @@
       <c r="AA198" s="4"/>
       <c r="AB198" s="4"/>
     </row>
-    <row r="199" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="199" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q199"/>
       <c r="T199" s="3"/>
       <c r="U199" s="3"/>
@@ -3483,7 +3392,7 @@
       <c r="AA199" s="4"/>
       <c r="AB199" s="4"/>
     </row>
-    <row r="200" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="200" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q200"/>
       <c r="T200" s="3"/>
       <c r="U200" s="3"/>
@@ -3495,7 +3404,7 @@
       <c r="AA200" s="4"/>
       <c r="AB200" s="4"/>
     </row>
-    <row r="201" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="201" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q201"/>
       <c r="T201" s="3"/>
       <c r="U201" s="3"/>
@@ -3507,7 +3416,7 @@
       <c r="AA201" s="4"/>
       <c r="AB201" s="4"/>
     </row>
-    <row r="202" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="202" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q202"/>
       <c r="T202" s="3"/>
       <c r="U202" s="3"/>
@@ -3519,8 +3428,9 @@
       <c r="AA202" s="4"/>
       <c r="AB202" s="4"/>
     </row>
-    <row r="203" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="203" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q203"/>
+      <c r="R203" s="12"/>
       <c r="T203" s="3"/>
       <c r="U203" s="3"/>
       <c r="V203" s="3"/>
@@ -3531,7 +3441,7 @@
       <c r="AA203" s="4"/>
       <c r="AB203" s="4"/>
     </row>
-    <row r="204" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="204" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q204"/>
       <c r="T204" s="3"/>
       <c r="U204" s="3"/>
@@ -3543,7 +3453,7 @@
       <c r="AA204" s="4"/>
       <c r="AB204" s="4"/>
     </row>
-    <row r="205" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="205" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q205"/>
       <c r="T205" s="3"/>
       <c r="U205" s="3"/>
@@ -3555,7 +3465,7 @@
       <c r="AA205" s="4"/>
       <c r="AB205" s="4"/>
     </row>
-    <row r="206" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="206" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q206"/>
       <c r="T206" s="3"/>
       <c r="U206" s="3"/>
@@ -3567,7 +3477,7 @@
       <c r="AA206" s="4"/>
       <c r="AB206" s="4"/>
     </row>
-    <row r="207" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="207" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q207"/>
       <c r="T207" s="3"/>
       <c r="U207" s="3"/>
@@ -3579,7 +3489,7 @@
       <c r="AA207" s="4"/>
       <c r="AB207" s="4"/>
     </row>
-    <row r="208" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="208" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q208"/>
       <c r="T208" s="3"/>
       <c r="U208" s="3"/>
@@ -3591,7 +3501,7 @@
       <c r="AA208" s="4"/>
       <c r="AB208" s="4"/>
     </row>
-    <row r="209" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="209" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q209"/>
       <c r="T209" s="3"/>
       <c r="U209" s="3"/>
@@ -3603,7 +3513,7 @@
       <c r="AA209" s="4"/>
       <c r="AB209" s="4"/>
     </row>
-    <row r="210" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="210" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q210"/>
       <c r="T210" s="3"/>
       <c r="U210" s="3"/>
@@ -3615,7 +3525,7 @@
       <c r="AA210" s="4"/>
       <c r="AB210" s="4"/>
     </row>
-    <row r="211" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="211" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q211"/>
       <c r="T211" s="3"/>
       <c r="U211" s="3"/>
@@ -3627,7 +3537,7 @@
       <c r="AA211" s="4"/>
       <c r="AB211" s="4"/>
     </row>
-    <row r="212" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="212" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q212"/>
       <c r="T212" s="3"/>
       <c r="U212" s="3"/>
@@ -3639,7 +3549,7 @@
       <c r="AA212" s="4"/>
       <c r="AB212" s="4"/>
     </row>
-    <row r="213" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="213" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q213"/>
       <c r="T213" s="3"/>
       <c r="U213" s="3"/>
@@ -3651,7 +3561,7 @@
       <c r="AA213" s="4"/>
       <c r="AB213" s="4"/>
     </row>
-    <row r="214" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="214" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q214"/>
       <c r="T214" s="3"/>
       <c r="U214" s="3"/>
@@ -3663,7 +3573,7 @@
       <c r="AA214" s="4"/>
       <c r="AB214" s="4"/>
     </row>
-    <row r="215" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="215" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q215"/>
       <c r="T215" s="3"/>
       <c r="U215" s="3"/>
@@ -3675,7 +3585,7 @@
       <c r="AA215" s="4"/>
       <c r="AB215" s="4"/>
     </row>
-    <row r="216" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="216" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q216"/>
       <c r="T216" s="3"/>
       <c r="U216" s="3"/>
@@ -3687,10 +3597,8 @@
       <c r="AA216" s="4"/>
       <c r="AB216" s="4"/>
     </row>
-    <row r="217" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P217" s="3"/>
+    <row r="217" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q217"/>
-      <c r="R217" s="12"/>
       <c r="T217" s="3"/>
       <c r="U217" s="3"/>
       <c r="V217" s="3"/>
@@ -3701,7 +3609,7 @@
       <c r="AA217" s="4"/>
       <c r="AB217" s="4"/>
     </row>
-    <row r="218" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="218" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q218"/>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
@@ -3713,7 +3621,7 @@
       <c r="AA218" s="4"/>
       <c r="AB218" s="4"/>
     </row>
-    <row r="219" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="219" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q219"/>
       <c r="T219" s="3"/>
       <c r="U219" s="3"/>
@@ -3725,7 +3633,7 @@
       <c r="AA219" s="4"/>
       <c r="AB219" s="4"/>
     </row>
-    <row r="220" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="220" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q220"/>
       <c r="T220" s="3"/>
       <c r="U220" s="3"/>
@@ -3737,7 +3645,7 @@
       <c r="AA220" s="4"/>
       <c r="AB220" s="4"/>
     </row>
-    <row r="221" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="221" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q221"/>
       <c r="T221" s="3"/>
       <c r="U221" s="3"/>
@@ -3749,7 +3657,7 @@
       <c r="AA221" s="4"/>
       <c r="AB221" s="4"/>
     </row>
-    <row r="222" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="222" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q222"/>
       <c r="T222" s="3"/>
       <c r="U222" s="3"/>
@@ -3761,7 +3669,7 @@
       <c r="AA222" s="4"/>
       <c r="AB222" s="4"/>
     </row>
-    <row r="223" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="223" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q223"/>
       <c r="T223" s="3"/>
       <c r="U223" s="3"/>
@@ -3773,7 +3681,7 @@
       <c r="AA223" s="4"/>
       <c r="AB223" s="4"/>
     </row>
-    <row r="224" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="224" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q224"/>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
@@ -3786,7 +3694,9 @@
       <c r="AB224" s="4"/>
     </row>
     <row r="225" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P225" s="3"/>
       <c r="Q225"/>
+      <c r="R225" s="12"/>
       <c r="T225" s="3"/>
       <c r="U225" s="3"/>
       <c r="V225" s="3"/>
@@ -3906,9 +3816,7 @@
       <c r="AB234" s="4"/>
     </row>
     <row r="235" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P235" s="3"/>
       <c r="Q235"/>
-      <c r="R235" s="12"/>
       <c r="T235" s="3"/>
       <c r="U235" s="3"/>
       <c r="V235" s="3"/>
@@ -3993,7 +3901,6 @@
     </row>
     <row r="242" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q242"/>
-      <c r="R242" s="12"/>
       <c r="T242" s="3"/>
       <c r="U242" s="3"/>
       <c r="V242" s="3"/>
@@ -4005,7 +3912,9 @@
       <c r="AB242" s="4"/>
     </row>
     <row r="243" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P243" s="3"/>
       <c r="Q243"/>
+      <c r="R243" s="12"/>
       <c r="T243" s="3"/>
       <c r="U243" s="3"/>
       <c r="V243" s="3"/>
@@ -4090,6 +3999,7 @@
     </row>
     <row r="250" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q250"/>
+      <c r="R250" s="12"/>
       <c r="T250" s="3"/>
       <c r="U250" s="3"/>
       <c r="V250" s="3"/>
@@ -4113,9 +4023,7 @@
       <c r="AB251" s="4"/>
     </row>
     <row r="252" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P252" s="3"/>
       <c r="Q252"/>
-      <c r="R252" s="12"/>
       <c r="T252" s="3"/>
       <c r="U252" s="3"/>
       <c r="V252" s="3"/>
@@ -4211,7 +4119,9 @@
       <c r="AB259" s="4"/>
     </row>
     <row r="260" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P260" s="3"/>
       <c r="Q260"/>
+      <c r="R260" s="12"/>
       <c r="T260" s="3"/>
       <c r="U260" s="3"/>
       <c r="V260" s="3"/>
@@ -4223,9 +4133,7 @@
       <c r="AB260" s="4"/>
     </row>
     <row r="261" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P261" s="3"/>
       <c r="Q261"/>
-      <c r="R261" s="12"/>
       <c r="T261" s="3"/>
       <c r="U261" s="3"/>
       <c r="V261" s="3"/>
@@ -4321,7 +4229,9 @@
       <c r="AB268" s="4"/>
     </row>
     <row r="269" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P269" s="3"/>
       <c r="Q269"/>
+      <c r="R269" s="12"/>
       <c r="T269" s="3"/>
       <c r="U269" s="3"/>
       <c r="V269" s="3"/>
@@ -4334,7 +4244,6 @@
     </row>
     <row r="270" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q270"/>
-      <c r="R270" s="12"/>
       <c r="T270" s="3"/>
       <c r="U270" s="3"/>
       <c r="V270" s="3"/>
@@ -4369,7 +4278,7 @@
       <c r="AA272" s="4"/>
       <c r="AB272" s="4"/>
     </row>
-    <row r="273" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="273" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q273"/>
       <c r="T273" s="3"/>
       <c r="U273" s="3"/>
@@ -4381,7 +4290,7 @@
       <c r="AA273" s="4"/>
       <c r="AB273" s="4"/>
     </row>
-    <row r="274" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="274" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q274"/>
       <c r="T274" s="3"/>
       <c r="U274" s="3"/>
@@ -4393,7 +4302,7 @@
       <c r="AA274" s="4"/>
       <c r="AB274" s="4"/>
     </row>
-    <row r="275" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="275" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q275"/>
       <c r="T275" s="3"/>
       <c r="U275" s="3"/>
@@ -4405,7 +4314,7 @@
       <c r="AA275" s="4"/>
       <c r="AB275" s="4"/>
     </row>
-    <row r="276" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="276" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q276"/>
       <c r="T276" s="3"/>
       <c r="U276" s="3"/>
@@ -4417,7 +4326,7 @@
       <c r="AA276" s="4"/>
       <c r="AB276" s="4"/>
     </row>
-    <row r="277" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="277" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q277"/>
       <c r="T277" s="3"/>
       <c r="U277" s="3"/>
@@ -4429,8 +4338,9 @@
       <c r="AA277" s="4"/>
       <c r="AB277" s="4"/>
     </row>
-    <row r="278" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="278" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q278"/>
+      <c r="R278" s="12"/>
       <c r="T278" s="3"/>
       <c r="U278" s="3"/>
       <c r="V278" s="3"/>
@@ -4441,7 +4351,7 @@
       <c r="AA278" s="4"/>
       <c r="AB278" s="4"/>
     </row>
-    <row r="279" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="279" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q279"/>
       <c r="T279" s="3"/>
       <c r="U279" s="3"/>
@@ -4453,7 +4363,7 @@
       <c r="AA279" s="4"/>
       <c r="AB279" s="4"/>
     </row>
-    <row r="280" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="280" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q280"/>
       <c r="T280" s="3"/>
       <c r="U280" s="3"/>
@@ -4465,10 +4375,8 @@
       <c r="AA280" s="4"/>
       <c r="AB280" s="4"/>
     </row>
-    <row r="281" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P281" s="3"/>
+    <row r="281" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q281"/>
-      <c r="R281" s="12"/>
       <c r="T281" s="3"/>
       <c r="U281" s="3"/>
       <c r="V281" s="3"/>
@@ -4479,7 +4387,7 @@
       <c r="AA281" s="4"/>
       <c r="AB281" s="4"/>
     </row>
-    <row r="282" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="282" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q282"/>
       <c r="T282" s="3"/>
       <c r="U282" s="3"/>
@@ -4491,7 +4399,7 @@
       <c r="AA282" s="4"/>
       <c r="AB282" s="4"/>
     </row>
-    <row r="283" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="283" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q283"/>
       <c r="T283" s="3"/>
       <c r="U283" s="3"/>
@@ -4503,7 +4411,7 @@
       <c r="AA283" s="4"/>
       <c r="AB283" s="4"/>
     </row>
-    <row r="284" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="284" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q284"/>
       <c r="T284" s="3"/>
       <c r="U284" s="3"/>
@@ -4515,7 +4423,7 @@
       <c r="AA284" s="4"/>
       <c r="AB284" s="4"/>
     </row>
-    <row r="285" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="285" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q285"/>
       <c r="T285" s="3"/>
       <c r="U285" s="3"/>
@@ -4527,7 +4435,7 @@
       <c r="AA285" s="4"/>
       <c r="AB285" s="4"/>
     </row>
-    <row r="286" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="286" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q286"/>
       <c r="T286" s="3"/>
       <c r="U286" s="3"/>
@@ -4539,7 +4447,7 @@
       <c r="AA286" s="4"/>
       <c r="AB286" s="4"/>
     </row>
-    <row r="287" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="287" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q287"/>
       <c r="T287" s="3"/>
       <c r="U287" s="3"/>
@@ -4551,7 +4459,7 @@
       <c r="AA287" s="4"/>
       <c r="AB287" s="4"/>
     </row>
-    <row r="288" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="288" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q288"/>
       <c r="T288" s="3"/>
       <c r="U288" s="3"/>
@@ -4564,7 +4472,9 @@
       <c r="AB288" s="4"/>
     </row>
     <row r="289" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P289" s="3"/>
       <c r="Q289"/>
+      <c r="R289" s="12"/>
       <c r="T289" s="3"/>
       <c r="U289" s="3"/>
       <c r="V289" s="3"/>
@@ -4708,9 +4618,7 @@
       <c r="AB300" s="4"/>
     </row>
     <row r="301" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P301" s="3"/>
       <c r="Q301"/>
-      <c r="R301" s="12"/>
       <c r="T301" s="3"/>
       <c r="U301" s="3"/>
       <c r="V301" s="3"/>
@@ -4806,7 +4714,9 @@
       <c r="AB308" s="4"/>
     </row>
     <row r="309" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P309" s="3"/>
       <c r="Q309"/>
+      <c r="R309" s="12"/>
       <c r="T309" s="3"/>
       <c r="U309" s="3"/>
       <c r="V309" s="3"/>
@@ -4830,9 +4740,7 @@
       <c r="AB310" s="4"/>
     </row>
     <row r="311" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P311" s="3"/>
       <c r="Q311"/>
-      <c r="R311" s="12"/>
       <c r="T311" s="3"/>
       <c r="U311" s="3"/>
       <c r="V311" s="3"/>
@@ -4928,7 +4836,9 @@
       <c r="AB318" s="4"/>
     </row>
     <row r="319" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P319" s="3"/>
       <c r="Q319"/>
+      <c r="R319" s="12"/>
       <c r="T319" s="3"/>
       <c r="U319" s="3"/>
       <c r="V319" s="3"/>
@@ -5061,7 +4971,6 @@
     </row>
     <row r="330" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q330"/>
-      <c r="R330" s="12"/>
       <c r="T330" s="3"/>
       <c r="U330" s="3"/>
       <c r="V330" s="3"/>
@@ -5144,9 +5053,8 @@
       <c r="AA336" s="4"/>
       <c r="AB336" s="4"/>
     </row>
-    <row r="337" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="337" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q337"/>
-      <c r="R337" s="12"/>
       <c r="T337" s="3"/>
       <c r="U337" s="3"/>
       <c r="V337" s="3"/>
@@ -5157,8 +5065,9 @@
       <c r="AA337" s="4"/>
       <c r="AB337" s="4"/>
     </row>
-    <row r="338" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="338" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q338"/>
+      <c r="R338" s="12"/>
       <c r="T338" s="3"/>
       <c r="U338" s="3"/>
       <c r="V338" s="3"/>
@@ -5169,7 +5078,7 @@
       <c r="AA338" s="4"/>
       <c r="AB338" s="4"/>
     </row>
-    <row r="339" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="339" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q339"/>
       <c r="T339" s="3"/>
       <c r="U339" s="3"/>
@@ -5181,7 +5090,7 @@
       <c r="AA339" s="4"/>
       <c r="AB339" s="4"/>
     </row>
-    <row r="340" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="340" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q340"/>
       <c r="T340" s="3"/>
       <c r="U340" s="3"/>
@@ -5193,7 +5102,7 @@
       <c r="AA340" s="4"/>
       <c r="AB340" s="4"/>
     </row>
-    <row r="341" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="341" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q341"/>
       <c r="T341" s="3"/>
       <c r="U341" s="3"/>
@@ -5205,7 +5114,7 @@
       <c r="AA341" s="4"/>
       <c r="AB341" s="4"/>
     </row>
-    <row r="342" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="342" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q342"/>
       <c r="T342" s="3"/>
       <c r="U342" s="3"/>
@@ -5217,7 +5126,7 @@
       <c r="AA342" s="4"/>
       <c r="AB342" s="4"/>
     </row>
-    <row r="343" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="343" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q343"/>
       <c r="T343" s="3"/>
       <c r="U343" s="3"/>
@@ -5229,7 +5138,7 @@
       <c r="AA343" s="4"/>
       <c r="AB343" s="4"/>
     </row>
-    <row r="344" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="344" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q344"/>
       <c r="T344" s="3"/>
       <c r="U344" s="3"/>
@@ -5241,8 +5150,7 @@
       <c r="AA344" s="4"/>
       <c r="AB344" s="4"/>
     </row>
-    <row r="345" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P345" s="3"/>
+    <row r="345" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q345"/>
       <c r="R345" s="12"/>
       <c r="T345" s="3"/>
@@ -5255,7 +5163,7 @@
       <c r="AA345" s="4"/>
       <c r="AB345" s="4"/>
     </row>
-    <row r="346" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="346" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q346"/>
       <c r="T346" s="3"/>
       <c r="U346" s="3"/>
@@ -5267,7 +5175,7 @@
       <c r="AA346" s="4"/>
       <c r="AB346" s="4"/>
     </row>
-    <row r="347" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="347" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q347"/>
       <c r="T347" s="3"/>
       <c r="U347" s="3"/>
@@ -5279,7 +5187,7 @@
       <c r="AA347" s="4"/>
       <c r="AB347" s="4"/>
     </row>
-    <row r="348" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="348" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q348"/>
       <c r="T348" s="3"/>
       <c r="U348" s="3"/>
@@ -5291,7 +5199,7 @@
       <c r="AA348" s="4"/>
       <c r="AB348" s="4"/>
     </row>
-    <row r="349" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="349" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q349"/>
       <c r="T349" s="3"/>
       <c r="U349" s="3"/>
@@ -5303,7 +5211,7 @@
       <c r="AA349" s="4"/>
       <c r="AB349" s="4"/>
     </row>
-    <row r="350" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="350" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q350"/>
       <c r="T350" s="3"/>
       <c r="U350" s="3"/>
@@ -5315,9 +5223,8 @@
       <c r="AA350" s="4"/>
       <c r="AB350" s="4"/>
     </row>
-    <row r="351" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="351" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q351"/>
-      <c r="R351" s="12"/>
       <c r="T351" s="3"/>
       <c r="U351" s="3"/>
       <c r="V351" s="3"/>
@@ -5328,7 +5235,7 @@
       <c r="AA351" s="4"/>
       <c r="AB351" s="4"/>
     </row>
-    <row r="352" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="352" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q352"/>
       <c r="T352" s="3"/>
       <c r="U352" s="3"/>
@@ -5341,7 +5248,9 @@
       <c r="AB352" s="4"/>
     </row>
     <row r="353" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P353" s="3"/>
       <c r="Q353"/>
+      <c r="R353" s="12"/>
       <c r="T353" s="3"/>
       <c r="U353" s="3"/>
       <c r="V353" s="3"/>
@@ -5377,9 +5286,7 @@
       <c r="AB355" s="4"/>
     </row>
     <row r="356" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P356" s="3"/>
       <c r="Q356"/>
-      <c r="R356" s="12"/>
       <c r="T356" s="3"/>
       <c r="U356" s="3"/>
       <c r="V356" s="3"/>
@@ -5416,6 +5323,7 @@
     </row>
     <row r="359" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q359"/>
+      <c r="R359" s="12"/>
       <c r="T359" s="3"/>
       <c r="U359" s="3"/>
       <c r="V359" s="3"/>
@@ -5475,7 +5383,9 @@
       <c r="AB363" s="4"/>
     </row>
     <row r="364" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P364" s="3"/>
       <c r="Q364"/>
+      <c r="R364" s="12"/>
       <c r="T364" s="3"/>
       <c r="U364" s="3"/>
       <c r="V364" s="3"/>
@@ -5499,9 +5409,7 @@
       <c r="AB365" s="4"/>
     </row>
     <row r="366" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P366" s="3"/>
       <c r="Q366"/>
-      <c r="R366" s="12"/>
       <c r="T366" s="3"/>
       <c r="U366" s="3"/>
       <c r="V366" s="3"/>
@@ -5536,7 +5444,7 @@
       <c r="AA368" s="4"/>
       <c r="AB368" s="4"/>
     </row>
-    <row r="369" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="369" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q369"/>
       <c r="T369" s="3"/>
       <c r="U369" s="3"/>
@@ -5548,7 +5456,7 @@
       <c r="AA369" s="4"/>
       <c r="AB369" s="4"/>
     </row>
-    <row r="370" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="370" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q370"/>
       <c r="T370" s="3"/>
       <c r="U370" s="3"/>
@@ -5560,7 +5468,7 @@
       <c r="AA370" s="4"/>
       <c r="AB370" s="4"/>
     </row>
-    <row r="371" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="371" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q371"/>
       <c r="T371" s="3"/>
       <c r="U371" s="3"/>
@@ -5572,7 +5480,7 @@
       <c r="AA371" s="4"/>
       <c r="AB371" s="4"/>
     </row>
-    <row r="372" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="372" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q372"/>
       <c r="T372" s="3"/>
       <c r="U372" s="3"/>
@@ -5584,7 +5492,7 @@
       <c r="AA372" s="4"/>
       <c r="AB372" s="4"/>
     </row>
-    <row r="373" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="373" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q373"/>
       <c r="T373" s="3"/>
       <c r="U373" s="3"/>
@@ -5596,8 +5504,10 @@
       <c r="AA373" s="4"/>
       <c r="AB373" s="4"/>
     </row>
-    <row r="374" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="374" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P374" s="3"/>
       <c r="Q374"/>
+      <c r="R374" s="12"/>
       <c r="T374" s="3"/>
       <c r="U374" s="3"/>
       <c r="V374" s="3"/>
@@ -5608,7 +5518,7 @@
       <c r="AA374" s="4"/>
       <c r="AB374" s="4"/>
     </row>
-    <row r="375" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="375" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q375"/>
       <c r="T375" s="3"/>
       <c r="U375" s="3"/>
@@ -5620,7 +5530,7 @@
       <c r="AA375" s="4"/>
       <c r="AB375" s="4"/>
     </row>
-    <row r="376" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="376" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q376"/>
       <c r="T376" s="3"/>
       <c r="U376" s="3"/>
@@ -5632,7 +5542,7 @@
       <c r="AA376" s="4"/>
       <c r="AB376" s="4"/>
     </row>
-    <row r="377" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="377" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q377"/>
       <c r="T377" s="3"/>
       <c r="U377" s="3"/>
@@ -5644,7 +5554,7 @@
       <c r="AA377" s="4"/>
       <c r="AB377" s="4"/>
     </row>
-    <row r="378" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="378" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q378"/>
       <c r="T378" s="3"/>
       <c r="U378" s="3"/>
@@ -5656,7 +5566,7 @@
       <c r="AA378" s="4"/>
       <c r="AB378" s="4"/>
     </row>
-    <row r="379" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="379" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q379"/>
       <c r="T379" s="3"/>
       <c r="U379" s="3"/>
@@ -5668,7 +5578,7 @@
       <c r="AA379" s="4"/>
       <c r="AB379" s="4"/>
     </row>
-    <row r="380" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="380" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q380"/>
       <c r="T380" s="3"/>
       <c r="U380" s="3"/>
@@ -5680,7 +5590,7 @@
       <c r="AA380" s="4"/>
       <c r="AB380" s="4"/>
     </row>
-    <row r="381" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="381" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q381"/>
       <c r="T381" s="3"/>
       <c r="U381" s="3"/>
@@ -5692,7 +5602,7 @@
       <c r="AA381" s="4"/>
       <c r="AB381" s="4"/>
     </row>
-    <row r="382" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="382" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q382"/>
       <c r="T382" s="3"/>
       <c r="U382" s="3"/>
@@ -5704,7 +5614,7 @@
       <c r="AA382" s="4"/>
       <c r="AB382" s="4"/>
     </row>
-    <row r="383" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="383" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q383"/>
       <c r="T383" s="3"/>
       <c r="U383" s="3"/>
@@ -5716,7 +5626,7 @@
       <c r="AA383" s="4"/>
       <c r="AB383" s="4"/>
     </row>
-    <row r="384" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="384" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q384"/>
       <c r="T384" s="3"/>
       <c r="U384" s="3"/>
@@ -5729,9 +5639,7 @@
       <c r="AB384" s="4"/>
     </row>
     <row r="385" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P385" s="3"/>
       <c r="Q385"/>
-      <c r="R385" s="12"/>
       <c r="T385" s="3"/>
       <c r="U385" s="3"/>
       <c r="V385" s="3"/>
@@ -5827,7 +5735,9 @@
       <c r="AB392" s="4"/>
     </row>
     <row r="393" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P393" s="3"/>
       <c r="Q393"/>
+      <c r="R393" s="12"/>
       <c r="T393" s="3"/>
       <c r="U393" s="3"/>
       <c r="V393" s="3"/>
@@ -5983,9 +5893,7 @@
       <c r="AB405" s="4"/>
     </row>
     <row r="406" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P406" s="3"/>
       <c r="Q406"/>
-      <c r="R406" s="12"/>
       <c r="T406" s="3"/>
       <c r="U406" s="3"/>
       <c r="V406" s="3"/>
@@ -6081,7 +5989,9 @@
       <c r="AB413" s="4"/>
     </row>
     <row r="414" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P414" s="3"/>
       <c r="Q414"/>
+      <c r="R414" s="12"/>
       <c r="T414" s="3"/>
       <c r="U414" s="3"/>
       <c r="V414" s="3"/>
@@ -6238,7 +6148,6 @@
     </row>
     <row r="427" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q427"/>
-      <c r="R427" s="12"/>
       <c r="T427" s="3"/>
       <c r="U427" s="3"/>
       <c r="V427" s="3"/>
@@ -6309,7 +6218,7 @@
       <c r="AA432" s="4"/>
       <c r="AB432" s="4"/>
     </row>
-    <row r="433" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="433" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q433"/>
       <c r="T433" s="3"/>
       <c r="U433" s="3"/>
@@ -6321,7 +6230,7 @@
       <c r="AA433" s="4"/>
       <c r="AB433" s="4"/>
     </row>
-    <row r="434" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="434" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q434"/>
       <c r="T434" s="3"/>
       <c r="U434" s="3"/>
@@ -6333,8 +6242,9 @@
       <c r="AA434" s="4"/>
       <c r="AB434" s="4"/>
     </row>
-    <row r="435" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="435" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q435"/>
+      <c r="R435" s="12"/>
       <c r="T435" s="3"/>
       <c r="U435" s="3"/>
       <c r="V435" s="3"/>
@@ -6345,7 +6255,7 @@
       <c r="AA435" s="4"/>
       <c r="AB435" s="4"/>
     </row>
-    <row r="436" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="436" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q436"/>
       <c r="T436" s="3"/>
       <c r="U436" s="3"/>
@@ -6357,7 +6267,7 @@
       <c r="AA436" s="4"/>
       <c r="AB436" s="4"/>
     </row>
-    <row r="437" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="437" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q437"/>
       <c r="T437" s="3"/>
       <c r="U437" s="3"/>
@@ -6369,7 +6279,7 @@
       <c r="AA437" s="4"/>
       <c r="AB437" s="4"/>
     </row>
-    <row r="438" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="438" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q438"/>
       <c r="T438" s="3"/>
       <c r="U438" s="3"/>
@@ -6381,7 +6291,7 @@
       <c r="AA438" s="4"/>
       <c r="AB438" s="4"/>
     </row>
-    <row r="439" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="439" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q439"/>
       <c r="T439" s="3"/>
       <c r="U439" s="3"/>
@@ -6393,7 +6303,7 @@
       <c r="AA439" s="4"/>
       <c r="AB439" s="4"/>
     </row>
-    <row r="440" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="440" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q440"/>
       <c r="T440" s="3"/>
       <c r="U440" s="3"/>
@@ -6405,7 +6315,7 @@
       <c r="AA440" s="4"/>
       <c r="AB440" s="4"/>
     </row>
-    <row r="441" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="441" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q441"/>
       <c r="T441" s="3"/>
       <c r="U441" s="3"/>
@@ -6417,7 +6327,7 @@
       <c r="AA441" s="4"/>
       <c r="AB441" s="4"/>
     </row>
-    <row r="442" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="442" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q442"/>
       <c r="T442" s="3"/>
       <c r="U442" s="3"/>
@@ -6429,7 +6339,7 @@
       <c r="AA442" s="4"/>
       <c r="AB442" s="4"/>
     </row>
-    <row r="443" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="443" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q443"/>
       <c r="T443" s="3"/>
       <c r="U443" s="3"/>
@@ -6441,7 +6351,7 @@
       <c r="AA443" s="4"/>
       <c r="AB443" s="4"/>
     </row>
-    <row r="444" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="444" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q444"/>
       <c r="T444" s="3"/>
       <c r="U444" s="3"/>
@@ -6453,7 +6363,7 @@
       <c r="AA444" s="4"/>
       <c r="AB444" s="4"/>
     </row>
-    <row r="445" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="445" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q445"/>
       <c r="T445" s="3"/>
       <c r="U445" s="3"/>
@@ -6465,10 +6375,8 @@
       <c r="AA445" s="4"/>
       <c r="AB445" s="4"/>
     </row>
-    <row r="446" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P446" s="3"/>
+    <row r="446" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q446"/>
-      <c r="R446" s="12"/>
       <c r="T446" s="3"/>
       <c r="U446" s="3"/>
       <c r="V446" s="3"/>
@@ -6479,7 +6387,7 @@
       <c r="AA446" s="4"/>
       <c r="AB446" s="4"/>
     </row>
-    <row r="447" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="447" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q447"/>
       <c r="T447" s="3"/>
       <c r="U447" s="3"/>
@@ -6491,7 +6399,7 @@
       <c r="AA447" s="4"/>
       <c r="AB447" s="4"/>
     </row>
-    <row r="448" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="448" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q448"/>
       <c r="T448" s="3"/>
       <c r="U448" s="3"/>
@@ -6503,7 +6411,7 @@
       <c r="AA448" s="4"/>
       <c r="AB448" s="4"/>
     </row>
-    <row r="449" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="449" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q449"/>
       <c r="T449" s="3"/>
       <c r="U449" s="3"/>
@@ -6515,7 +6423,7 @@
       <c r="AA449" s="4"/>
       <c r="AB449" s="4"/>
     </row>
-    <row r="450" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="450" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q450"/>
       <c r="T450" s="3"/>
       <c r="U450" s="3"/>
@@ -6527,7 +6435,7 @@
       <c r="AA450" s="4"/>
       <c r="AB450" s="4"/>
     </row>
-    <row r="451" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="451" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q451"/>
       <c r="T451" s="3"/>
       <c r="U451" s="3"/>
@@ -6539,7 +6447,7 @@
       <c r="AA451" s="4"/>
       <c r="AB451" s="4"/>
     </row>
-    <row r="452" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="452" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q452"/>
       <c r="T452" s="3"/>
       <c r="U452" s="3"/>
@@ -6551,7 +6459,7 @@
       <c r="AA452" s="4"/>
       <c r="AB452" s="4"/>
     </row>
-    <row r="453" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="453" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q453"/>
       <c r="T453" s="3"/>
       <c r="U453" s="3"/>
@@ -6563,8 +6471,10 @@
       <c r="AA453" s="4"/>
       <c r="AB453" s="4"/>
     </row>
-    <row r="454" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="454" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P454" s="3"/>
       <c r="Q454"/>
+      <c r="R454" s="12"/>
       <c r="T454" s="3"/>
       <c r="U454" s="3"/>
       <c r="V454" s="3"/>
@@ -6575,7 +6485,7 @@
       <c r="AA454" s="4"/>
       <c r="AB454" s="4"/>
     </row>
-    <row r="455" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="455" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q455"/>
       <c r="T455" s="3"/>
       <c r="U455" s="3"/>
@@ -6587,7 +6497,7 @@
       <c r="AA455" s="4"/>
       <c r="AB455" s="4"/>
     </row>
-    <row r="456" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="456" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q456"/>
       <c r="T456" s="3"/>
       <c r="U456" s="3"/>
@@ -6599,7 +6509,7 @@
       <c r="AA456" s="4"/>
       <c r="AB456" s="4"/>
     </row>
-    <row r="457" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="457" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q457"/>
       <c r="T457" s="3"/>
       <c r="U457" s="3"/>
@@ -6611,7 +6521,7 @@
       <c r="AA457" s="4"/>
       <c r="AB457" s="4"/>
     </row>
-    <row r="458" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="458" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q458"/>
       <c r="T458" s="3"/>
       <c r="U458" s="3"/>
@@ -6623,7 +6533,7 @@
       <c r="AA458" s="4"/>
       <c r="AB458" s="4"/>
     </row>
-    <row r="459" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="459" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q459"/>
       <c r="T459" s="3"/>
       <c r="U459" s="3"/>
@@ -6635,7 +6545,7 @@
       <c r="AA459" s="4"/>
       <c r="AB459" s="4"/>
     </row>
-    <row r="460" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="460" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q460"/>
       <c r="T460" s="3"/>
       <c r="U460" s="3"/>
@@ -6647,7 +6557,7 @@
       <c r="AA460" s="4"/>
       <c r="AB460" s="4"/>
     </row>
-    <row r="461" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="461" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q461"/>
       <c r="T461" s="3"/>
       <c r="U461" s="3"/>
@@ -6659,7 +6569,7 @@
       <c r="AA461" s="4"/>
       <c r="AB461" s="4"/>
     </row>
-    <row r="462" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="462" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q462"/>
       <c r="T462" s="3"/>
       <c r="U462" s="3"/>
@@ -6671,7 +6581,7 @@
       <c r="AA462" s="4"/>
       <c r="AB462" s="4"/>
     </row>
-    <row r="463" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="463" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q463"/>
       <c r="T463" s="3"/>
       <c r="U463" s="3"/>
@@ -6683,7 +6593,7 @@
       <c r="AA463" s="4"/>
       <c r="AB463" s="4"/>
     </row>
-    <row r="464" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="464" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q464"/>
       <c r="T464" s="3"/>
       <c r="U464" s="3"/>
@@ -6756,9 +6666,7 @@
       <c r="AB469" s="4"/>
     </row>
     <row r="470" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P470" s="3"/>
       <c r="Q470"/>
-      <c r="R470" s="12"/>
       <c r="T470" s="3"/>
       <c r="U470" s="3"/>
       <c r="V470" s="3"/>
@@ -6854,7 +6762,9 @@
       <c r="AB477" s="4"/>
     </row>
     <row r="478" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P478" s="3"/>
       <c r="Q478"/>
+      <c r="R478" s="12"/>
       <c r="T478" s="3"/>
       <c r="U478" s="3"/>
       <c r="V478" s="3"/>
@@ -6889,7 +6799,7 @@
       <c r="AA480" s="4"/>
       <c r="AB480" s="4"/>
     </row>
-    <row r="481" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="481" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q481"/>
       <c r="T481" s="3"/>
       <c r="U481" s="3"/>
@@ -6901,7 +6811,7 @@
       <c r="AA481" s="4"/>
       <c r="AB481" s="4"/>
     </row>
-    <row r="482" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="482" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q482"/>
       <c r="T482" s="3"/>
       <c r="U482" s="3"/>
@@ -6913,7 +6823,7 @@
       <c r="AA482" s="4"/>
       <c r="AB482" s="4"/>
     </row>
-    <row r="483" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="483" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q483"/>
       <c r="T483" s="3"/>
       <c r="U483" s="3"/>
@@ -6925,7 +6835,7 @@
       <c r="AA483" s="4"/>
       <c r="AB483" s="4"/>
     </row>
-    <row r="484" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="484" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q484"/>
       <c r="T484" s="3"/>
       <c r="U484" s="3"/>
@@ -6937,7 +6847,7 @@
       <c r="AA484" s="4"/>
       <c r="AB484" s="4"/>
     </row>
-    <row r="485" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="485" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q485"/>
       <c r="T485" s="3"/>
       <c r="U485" s="3"/>
@@ -6949,7 +6859,7 @@
       <c r="AA485" s="4"/>
       <c r="AB485" s="4"/>
     </row>
-    <row r="486" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="486" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q486"/>
       <c r="T486" s="3"/>
       <c r="U486" s="3"/>
@@ -6961,7 +6871,7 @@
       <c r="AA486" s="4"/>
       <c r="AB486" s="4"/>
     </row>
-    <row r="487" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="487" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q487"/>
       <c r="T487" s="3"/>
       <c r="U487" s="3"/>
@@ -6973,7 +6883,7 @@
       <c r="AA487" s="4"/>
       <c r="AB487" s="4"/>
     </row>
-    <row r="488" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="488" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q488"/>
       <c r="T488" s="3"/>
       <c r="U488" s="3"/>
@@ -6985,10 +6895,8 @@
       <c r="AA488" s="4"/>
       <c r="AB488" s="4"/>
     </row>
-    <row r="489" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P489" s="3"/>
+    <row r="489" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q489"/>
-      <c r="R489" s="12"/>
       <c r="T489" s="3"/>
       <c r="U489" s="3"/>
       <c r="V489" s="3"/>
@@ -6999,7 +6907,7 @@
       <c r="AA489" s="4"/>
       <c r="AB489" s="4"/>
     </row>
-    <row r="490" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="490" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q490"/>
       <c r="T490" s="3"/>
       <c r="U490" s="3"/>
@@ -7011,7 +6919,7 @@
       <c r="AA490" s="4"/>
       <c r="AB490" s="4"/>
     </row>
-    <row r="491" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="491" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q491"/>
       <c r="T491" s="3"/>
       <c r="U491" s="3"/>
@@ -7023,7 +6931,7 @@
       <c r="AA491" s="4"/>
       <c r="AB491" s="4"/>
     </row>
-    <row r="492" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="492" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q492"/>
       <c r="T492" s="3"/>
       <c r="U492" s="3"/>
@@ -7035,7 +6943,7 @@
       <c r="AA492" s="4"/>
       <c r="AB492" s="4"/>
     </row>
-    <row r="493" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="493" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q493"/>
       <c r="T493" s="3"/>
       <c r="U493" s="3"/>
@@ -7047,7 +6955,7 @@
       <c r="AA493" s="4"/>
       <c r="AB493" s="4"/>
     </row>
-    <row r="494" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="494" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q494"/>
       <c r="T494" s="3"/>
       <c r="U494" s="3"/>
@@ -7059,10 +6967,8 @@
       <c r="AA494" s="4"/>
       <c r="AB494" s="4"/>
     </row>
-    <row r="495" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P495" s="3"/>
+    <row r="495" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q495"/>
-      <c r="R495" s="12"/>
       <c r="T495" s="3"/>
       <c r="U495" s="3"/>
       <c r="V495" s="3"/>
@@ -7073,7 +6979,7 @@
       <c r="AA495" s="4"/>
       <c r="AB495" s="4"/>
     </row>
-    <row r="496" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="496" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q496"/>
       <c r="T496" s="3"/>
       <c r="U496" s="3"/>
@@ -7085,8 +6991,10 @@
       <c r="AA496" s="4"/>
       <c r="AB496" s="4"/>
     </row>
-    <row r="497" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="497" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P497" s="3"/>
       <c r="Q497"/>
+      <c r="R497" s="12"/>
       <c r="T497" s="3"/>
       <c r="U497" s="3"/>
       <c r="V497" s="3"/>
@@ -7097,7 +7005,7 @@
       <c r="AA497" s="4"/>
       <c r="AB497" s="4"/>
     </row>
-    <row r="498" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="498" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q498"/>
       <c r="T498" s="3"/>
       <c r="U498" s="3"/>
@@ -7109,7 +7017,7 @@
       <c r="AA498" s="4"/>
       <c r="AB498" s="4"/>
     </row>
-    <row r="499" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="499" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q499"/>
       <c r="T499" s="3"/>
       <c r="U499" s="3"/>
@@ -7121,7 +7029,7 @@
       <c r="AA499" s="4"/>
       <c r="AB499" s="4"/>
     </row>
-    <row r="500" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="500" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q500"/>
       <c r="T500" s="3"/>
       <c r="U500" s="3"/>
@@ -7133,7 +7041,7 @@
       <c r="AA500" s="4"/>
       <c r="AB500" s="4"/>
     </row>
-    <row r="501" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="501" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q501"/>
       <c r="T501" s="3"/>
       <c r="U501" s="3"/>
@@ -7145,7 +7053,7 @@
       <c r="AA501" s="4"/>
       <c r="AB501" s="4"/>
     </row>
-    <row r="502" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="502" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q502"/>
       <c r="T502" s="3"/>
       <c r="U502" s="3"/>
@@ -7157,8 +7065,10 @@
       <c r="AA502" s="4"/>
       <c r="AB502" s="4"/>
     </row>
-    <row r="503" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="503" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P503" s="3"/>
       <c r="Q503"/>
+      <c r="R503" s="12"/>
       <c r="T503" s="3"/>
       <c r="U503" s="3"/>
       <c r="V503" s="3"/>
@@ -7169,7 +7079,7 @@
       <c r="AA503" s="4"/>
       <c r="AB503" s="4"/>
     </row>
-    <row r="504" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="504" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q504"/>
       <c r="T504" s="3"/>
       <c r="U504" s="3"/>
@@ -7181,7 +7091,7 @@
       <c r="AA504" s="4"/>
       <c r="AB504" s="4"/>
     </row>
-    <row r="505" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="505" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q505"/>
       <c r="T505" s="3"/>
       <c r="U505" s="3"/>
@@ -7193,7 +7103,7 @@
       <c r="AA505" s="4"/>
       <c r="AB505" s="4"/>
     </row>
-    <row r="506" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="506" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q506"/>
       <c r="T506" s="3"/>
       <c r="U506" s="3"/>
@@ -7205,7 +7115,7 @@
       <c r="AA506" s="4"/>
       <c r="AB506" s="4"/>
     </row>
-    <row r="507" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="507" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q507"/>
       <c r="T507" s="3"/>
       <c r="U507" s="3"/>
@@ -7217,9 +7127,8 @@
       <c r="AA507" s="4"/>
       <c r="AB507" s="4"/>
     </row>
-    <row r="508" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="508" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q508"/>
-      <c r="R508" s="12"/>
       <c r="T508" s="3"/>
       <c r="U508" s="3"/>
       <c r="V508" s="3"/>
@@ -7230,7 +7139,7 @@
       <c r="AA508" s="4"/>
       <c r="AB508" s="4"/>
     </row>
-    <row r="509" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="509" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q509"/>
       <c r="T509" s="3"/>
       <c r="U509" s="3"/>
@@ -7242,7 +7151,7 @@
       <c r="AA509" s="4"/>
       <c r="AB509" s="4"/>
     </row>
-    <row r="510" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="510" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q510"/>
       <c r="T510" s="3"/>
       <c r="U510" s="3"/>
@@ -7254,7 +7163,7 @@
       <c r="AA510" s="4"/>
       <c r="AB510" s="4"/>
     </row>
-    <row r="511" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="511" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q511"/>
       <c r="T511" s="3"/>
       <c r="U511" s="3"/>
@@ -7266,7 +7175,7 @@
       <c r="AA511" s="4"/>
       <c r="AB511" s="4"/>
     </row>
-    <row r="512" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="512" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q512"/>
       <c r="T512" s="3"/>
       <c r="U512" s="3"/>
@@ -7316,6 +7225,7 @@
     </row>
     <row r="516" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q516"/>
+      <c r="R516" s="12"/>
       <c r="T516" s="3"/>
       <c r="U516" s="3"/>
       <c r="V516" s="3"/>
@@ -7351,9 +7261,7 @@
       <c r="AB518" s="4"/>
     </row>
     <row r="519" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P519" s="3"/>
       <c r="Q519"/>
-      <c r="R519" s="12"/>
       <c r="T519" s="3"/>
       <c r="U519" s="3"/>
       <c r="V519" s="3"/>
@@ -7449,7 +7357,9 @@
       <c r="AB526" s="4"/>
     </row>
     <row r="527" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P527" s="3"/>
       <c r="Q527"/>
+      <c r="R527" s="12"/>
       <c r="T527" s="3"/>
       <c r="U527" s="3"/>
       <c r="V527" s="3"/>
@@ -7497,9 +7407,7 @@
       <c r="AB530" s="4"/>
     </row>
     <row r="531" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P531" s="3"/>
       <c r="Q531"/>
-      <c r="R531" s="12"/>
       <c r="T531" s="3"/>
       <c r="U531" s="3"/>
       <c r="V531" s="3"/>
@@ -7693,7 +7601,9 @@
       <c r="AB546" s="4"/>
     </row>
     <row r="547" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P547" s="3"/>
       <c r="Q547"/>
+      <c r="R547" s="12"/>
       <c r="T547" s="3"/>
       <c r="U547" s="3"/>
       <c r="V547" s="3"/>
@@ -7801,9 +7711,7 @@
       <c r="AB555" s="4"/>
     </row>
     <row r="556" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P556" s="3"/>
       <c r="Q556"/>
-      <c r="R556" s="12"/>
       <c r="T556" s="3"/>
       <c r="U556" s="3"/>
       <c r="V556" s="3"/>
@@ -7899,7 +7807,9 @@
       <c r="AB563" s="4"/>
     </row>
     <row r="564" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P564" s="3"/>
       <c r="Q564"/>
+      <c r="R564" s="12"/>
       <c r="T564" s="3"/>
       <c r="U564" s="3"/>
       <c r="V564" s="3"/>
@@ -7924,7 +7834,6 @@
     </row>
     <row r="566" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q566"/>
-      <c r="R566" s="12"/>
       <c r="T566" s="3"/>
       <c r="U566" s="3"/>
       <c r="V566" s="3"/>
@@ -7984,9 +7893,7 @@
       <c r="AB570" s="4"/>
     </row>
     <row r="571" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P571" s="3"/>
       <c r="Q571"/>
-      <c r="R571" s="12"/>
       <c r="T571" s="3"/>
       <c r="U571" s="3"/>
       <c r="V571" s="3"/>
@@ -8023,6 +7930,7 @@
     </row>
     <row r="574" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q574"/>
+      <c r="R574" s="12"/>
       <c r="T574" s="3"/>
       <c r="U574" s="3"/>
       <c r="V574" s="3"/>
@@ -8057,7 +7965,7 @@
       <c r="AA576" s="4"/>
       <c r="AB576" s="4"/>
     </row>
-    <row r="577" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="577" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q577"/>
       <c r="T577" s="3"/>
       <c r="U577" s="3"/>
@@ -8069,7 +7977,7 @@
       <c r="AA577" s="4"/>
       <c r="AB577" s="4"/>
     </row>
-    <row r="578" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="578" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q578"/>
       <c r="T578" s="3"/>
       <c r="U578" s="3"/>
@@ -8081,8 +7989,10 @@
       <c r="AA578" s="4"/>
       <c r="AB578" s="4"/>
     </row>
-    <row r="579" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="579" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P579" s="3"/>
       <c r="Q579"/>
+      <c r="R579" s="12"/>
       <c r="T579" s="3"/>
       <c r="U579" s="3"/>
       <c r="V579" s="3"/>
@@ -8093,7 +8003,7 @@
       <c r="AA579" s="4"/>
       <c r="AB579" s="4"/>
     </row>
-    <row r="580" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="580" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q580"/>
       <c r="T580" s="3"/>
       <c r="U580" s="3"/>
@@ -8105,7 +8015,7 @@
       <c r="AA580" s="4"/>
       <c r="AB580" s="4"/>
     </row>
-    <row r="581" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="581" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q581"/>
       <c r="T581" s="3"/>
       <c r="U581" s="3"/>
@@ -8117,7 +8027,7 @@
       <c r="AA581" s="4"/>
       <c r="AB581" s="4"/>
     </row>
-    <row r="582" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="582" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q582"/>
       <c r="T582" s="3"/>
       <c r="U582" s="3"/>
@@ -8129,7 +8039,7 @@
       <c r="AA582" s="4"/>
       <c r="AB582" s="4"/>
     </row>
-    <row r="583" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="583" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q583"/>
       <c r="T583" s="3"/>
       <c r="U583" s="3"/>
@@ -8141,7 +8051,7 @@
       <c r="AA583" s="4"/>
       <c r="AB583" s="4"/>
     </row>
-    <row r="584" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="584" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q584"/>
       <c r="T584" s="3"/>
       <c r="U584" s="3"/>
@@ -8153,7 +8063,7 @@
       <c r="AA584" s="4"/>
       <c r="AB584" s="4"/>
     </row>
-    <row r="585" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="585" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q585"/>
       <c r="T585" s="3"/>
       <c r="U585" s="3"/>
@@ -8165,7 +8075,7 @@
       <c r="AA585" s="4"/>
       <c r="AB585" s="4"/>
     </row>
-    <row r="586" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="586" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q586"/>
       <c r="T586" s="3"/>
       <c r="U586" s="3"/>
@@ -8177,7 +8087,7 @@
       <c r="AA586" s="4"/>
       <c r="AB586" s="4"/>
     </row>
-    <row r="587" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="587" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q587"/>
       <c r="T587" s="3"/>
       <c r="U587" s="3"/>
@@ -8189,7 +8099,7 @@
       <c r="AA587" s="4"/>
       <c r="AB587" s="4"/>
     </row>
-    <row r="588" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="588" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q588"/>
       <c r="T588" s="3"/>
       <c r="U588" s="3"/>
@@ -8201,7 +8111,7 @@
       <c r="AA588" s="4"/>
       <c r="AB588" s="4"/>
     </row>
-    <row r="589" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="589" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q589"/>
       <c r="T589" s="3"/>
       <c r="U589" s="3"/>
@@ -8213,7 +8123,7 @@
       <c r="AA589" s="4"/>
       <c r="AB589" s="4"/>
     </row>
-    <row r="590" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="590" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q590"/>
       <c r="T590" s="3"/>
       <c r="U590" s="3"/>
@@ -8225,7 +8135,7 @@
       <c r="AA590" s="4"/>
       <c r="AB590" s="4"/>
     </row>
-    <row r="591" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="591" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q591"/>
       <c r="T591" s="3"/>
       <c r="U591" s="3"/>
@@ -8237,7 +8147,7 @@
       <c r="AA591" s="4"/>
       <c r="AB591" s="4"/>
     </row>
-    <row r="592" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="592" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q592"/>
       <c r="T592" s="3"/>
       <c r="U592" s="3"/>
@@ -8322,36 +8232,100 @@
       <c r="AB598" s="4"/>
     </row>
     <row r="599" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T599" s="6"/>
-      <c r="U599" s="6"/>
+      <c r="Q599"/>
+      <c r="T599" s="3"/>
+      <c r="U599" s="3"/>
+      <c r="V599" s="3"/>
+      <c r="W599"/>
+      <c r="X599" s="10"/>
+      <c r="Y599"/>
+      <c r="Z599"/>
+      <c r="AA599" s="4"/>
+      <c r="AB599" s="4"/>
     </row>
     <row r="600" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T600" s="6"/>
-      <c r="U600" s="6"/>
+      <c r="Q600"/>
+      <c r="T600" s="3"/>
+      <c r="U600" s="3"/>
+      <c r="V600" s="3"/>
+      <c r="W600"/>
+      <c r="X600" s="10"/>
+      <c r="Y600"/>
+      <c r="Z600"/>
+      <c r="AA600" s="4"/>
+      <c r="AB600" s="4"/>
     </row>
     <row r="601" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T601" s="6"/>
-      <c r="U601" s="6"/>
+      <c r="Q601"/>
+      <c r="T601" s="3"/>
+      <c r="U601" s="3"/>
+      <c r="V601" s="3"/>
+      <c r="W601"/>
+      <c r="X601" s="10"/>
+      <c r="Y601"/>
+      <c r="Z601"/>
+      <c r="AA601" s="4"/>
+      <c r="AB601" s="4"/>
     </row>
     <row r="602" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T602" s="6"/>
-      <c r="U602" s="6"/>
+      <c r="Q602"/>
+      <c r="T602" s="3"/>
+      <c r="U602" s="3"/>
+      <c r="V602" s="3"/>
+      <c r="W602"/>
+      <c r="X602" s="10"/>
+      <c r="Y602"/>
+      <c r="Z602"/>
+      <c r="AA602" s="4"/>
+      <c r="AB602" s="4"/>
     </row>
     <row r="603" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T603" s="6"/>
-      <c r="U603" s="6"/>
+      <c r="Q603"/>
+      <c r="T603" s="3"/>
+      <c r="U603" s="3"/>
+      <c r="V603" s="3"/>
+      <c r="W603"/>
+      <c r="X603" s="10"/>
+      <c r="Y603"/>
+      <c r="Z603"/>
+      <c r="AA603" s="4"/>
+      <c r="AB603" s="4"/>
     </row>
     <row r="604" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T604" s="6"/>
-      <c r="U604" s="6"/>
+      <c r="Q604"/>
+      <c r="T604" s="3"/>
+      <c r="U604" s="3"/>
+      <c r="V604" s="3"/>
+      <c r="W604"/>
+      <c r="X604" s="10"/>
+      <c r="Y604"/>
+      <c r="Z604"/>
+      <c r="AA604" s="4"/>
+      <c r="AB604" s="4"/>
     </row>
     <row r="605" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T605" s="6"/>
-      <c r="U605" s="6"/>
+      <c r="Q605"/>
+      <c r="T605" s="3"/>
+      <c r="U605" s="3"/>
+      <c r="V605" s="3"/>
+      <c r="W605"/>
+      <c r="X605" s="10"/>
+      <c r="Y605"/>
+      <c r="Z605"/>
+      <c r="AA605" s="4"/>
+      <c r="AB605" s="4"/>
     </row>
     <row r="606" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T606" s="6"/>
-      <c r="U606" s="6"/>
+      <c r="Q606"/>
+      <c r="T606" s="3"/>
+      <c r="U606" s="3"/>
+      <c r="V606" s="3"/>
+      <c r="W606"/>
+      <c r="X606" s="10"/>
+      <c r="Y606"/>
+      <c r="Z606"/>
+      <c r="AA606" s="4"/>
+      <c r="AB606" s="4"/>
     </row>
     <row r="607" spans="17:28" x14ac:dyDescent="0.2">
       <c r="T607" s="6"/>
@@ -8440,6 +8414,38 @@
     <row r="628" spans="20:21" x14ac:dyDescent="0.2">
       <c r="T628" s="6"/>
       <c r="U628" s="6"/>
+    </row>
+    <row r="629" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T629" s="6"/>
+      <c r="U629" s="6"/>
+    </row>
+    <row r="630" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T630" s="6"/>
+      <c r="U630" s="6"/>
+    </row>
+    <row r="631" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T631" s="6"/>
+      <c r="U631" s="6"/>
+    </row>
+    <row r="632" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T632" s="6"/>
+      <c r="U632" s="6"/>
+    </row>
+    <row r="633" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T633" s="6"/>
+      <c r="U633" s="6"/>
+    </row>
+    <row r="634" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T634" s="6"/>
+      <c r="U634" s="6"/>
+    </row>
+    <row r="635" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T635" s="6"/>
+      <c r="U635" s="6"/>
+    </row>
+    <row r="636" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T636" s="6"/>
+      <c r="U636" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -8451,12 +8457,9 @@
     <hyperlink ref="F7" r:id="rId5"/>
     <hyperlink ref="F8" r:id="rId6"/>
     <hyperlink ref="F11" r:id="rId7"/>
-    <hyperlink ref="F12" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add checkbox, select, switch, text UI component add questionnaire
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Customers.xlsx
+++ b/EDI/Web/wwwroot/Upload/Customers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>School Name</t>
   </si>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB628"/>
+  <dimension ref="A1:AB636"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1116,36 +1116,6 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="20">
-        <v>42299</v>
-      </c>
-      <c r="K12" s="21">
-        <v>200122609501901</v>
-      </c>
       <c r="Q12"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -1158,36 +1128,6 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="20">
-        <v>41876</v>
-      </c>
-      <c r="K13" s="21">
-        <v>200122604903901</v>
-      </c>
       <c r="Q13"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -1199,37 +1139,7 @@
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="20">
-        <v>42113</v>
-      </c>
-      <c r="K14" s="21">
-        <v>200122699902901</v>
-      </c>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Q14"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1399,7 +1309,6 @@
     </row>
     <row r="28" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q28"/>
-      <c r="R28" s="12"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -1496,6 +1405,7 @@
     </row>
     <row r="36" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q36"/>
+      <c r="R36" s="12"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -1687,9 +1597,7 @@
       <c r="AB51" s="4"/>
     </row>
     <row r="52" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P52" s="3"/>
       <c r="Q52"/>
-      <c r="R52" s="12"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -1785,7 +1693,9 @@
       <c r="AB59" s="4"/>
     </row>
     <row r="60" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P60" s="3"/>
       <c r="Q60"/>
+      <c r="R60" s="12"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="3"/>
@@ -1929,9 +1839,7 @@
       <c r="AB71" s="4"/>
     </row>
     <row r="72" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P72" s="3"/>
       <c r="Q72"/>
-      <c r="R72" s="12"/>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
@@ -2016,7 +1924,6 @@
     </row>
     <row r="79" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q79"/>
-      <c r="R79" s="12"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
@@ -2028,7 +1935,9 @@
       <c r="AB79" s="4"/>
     </row>
     <row r="80" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P80" s="3"/>
       <c r="Q80"/>
+      <c r="R80" s="12"/>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
@@ -2112,7 +2021,6 @@
       <c r="AB86" s="4"/>
     </row>
     <row r="87" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P87" s="3"/>
       <c r="Q87"/>
       <c r="R87" s="12"/>
       <c r="T87" s="3"/>
@@ -2210,7 +2118,9 @@
       <c r="AB94" s="4"/>
     </row>
     <row r="95" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P95" s="3"/>
       <c r="Q95"/>
+      <c r="R95" s="12"/>
       <c r="T95" s="3"/>
       <c r="U95" s="3"/>
       <c r="V95" s="3"/>
@@ -2233,7 +2143,7 @@
       <c r="AA96" s="4"/>
       <c r="AB96" s="4"/>
     </row>
-    <row r="97" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q97"/>
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
@@ -2245,7 +2155,7 @@
       <c r="AA97" s="4"/>
       <c r="AB97" s="4"/>
     </row>
-    <row r="98" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q98"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -2257,7 +2167,7 @@
       <c r="AA98" s="4"/>
       <c r="AB98" s="4"/>
     </row>
-    <row r="99" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q99"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -2269,9 +2179,8 @@
       <c r="AA99" s="4"/>
       <c r="AB99" s="4"/>
     </row>
-    <row r="100" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="100" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q100"/>
-      <c r="R100" s="12"/>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
       <c r="V100" s="3"/>
@@ -2282,7 +2191,7 @@
       <c r="AA100" s="4"/>
       <c r="AB100" s="4"/>
     </row>
-    <row r="101" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q101"/>
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
@@ -2294,7 +2203,7 @@
       <c r="AA101" s="4"/>
       <c r="AB101" s="4"/>
     </row>
-    <row r="102" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q102"/>
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
@@ -2306,7 +2215,7 @@
       <c r="AA102" s="4"/>
       <c r="AB102" s="4"/>
     </row>
-    <row r="103" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q103"/>
       <c r="T103" s="3"/>
       <c r="U103" s="3"/>
@@ -2318,7 +2227,7 @@
       <c r="AA103" s="4"/>
       <c r="AB103" s="4"/>
     </row>
-    <row r="104" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q104"/>
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
@@ -2330,7 +2239,7 @@
       <c r="AA104" s="4"/>
       <c r="AB104" s="4"/>
     </row>
-    <row r="105" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q105"/>
       <c r="T105" s="3"/>
       <c r="U105" s="3"/>
@@ -2342,7 +2251,7 @@
       <c r="AA105" s="4"/>
       <c r="AB105" s="4"/>
     </row>
-    <row r="106" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q106"/>
       <c r="T106" s="3"/>
       <c r="U106" s="3"/>
@@ -2354,7 +2263,7 @@
       <c r="AA106" s="4"/>
       <c r="AB106" s="4"/>
     </row>
-    <row r="107" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q107"/>
       <c r="T107" s="3"/>
       <c r="U107" s="3"/>
@@ -2366,8 +2275,7 @@
       <c r="AA107" s="4"/>
       <c r="AB107" s="4"/>
     </row>
-    <row r="108" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P108" s="3"/>
+    <row r="108" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q108"/>
       <c r="R108" s="12"/>
       <c r="T108" s="3"/>
@@ -2380,7 +2288,7 @@
       <c r="AA108" s="4"/>
       <c r="AB108" s="4"/>
     </row>
-    <row r="109" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q109"/>
       <c r="T109" s="3"/>
       <c r="U109" s="3"/>
@@ -2392,7 +2300,7 @@
       <c r="AA109" s="4"/>
       <c r="AB109" s="4"/>
     </row>
-    <row r="110" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q110"/>
       <c r="T110" s="3"/>
       <c r="U110" s="3"/>
@@ -2404,7 +2312,7 @@
       <c r="AA110" s="4"/>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q111"/>
       <c r="T111" s="3"/>
       <c r="U111" s="3"/>
@@ -2416,7 +2324,7 @@
       <c r="AA111" s="4"/>
       <c r="AB111" s="4"/>
     </row>
-    <row r="112" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q112"/>
       <c r="T112" s="3"/>
       <c r="U112" s="3"/>
@@ -2428,7 +2336,7 @@
       <c r="AA112" s="4"/>
       <c r="AB112" s="4"/>
     </row>
-    <row r="113" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q113"/>
       <c r="T113" s="3"/>
       <c r="U113" s="3"/>
@@ -2440,7 +2348,7 @@
       <c r="AA113" s="4"/>
       <c r="AB113" s="4"/>
     </row>
-    <row r="114" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q114"/>
       <c r="T114" s="3"/>
       <c r="U114" s="3"/>
@@ -2452,7 +2360,7 @@
       <c r="AA114" s="4"/>
       <c r="AB114" s="4"/>
     </row>
-    <row r="115" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q115"/>
       <c r="T115" s="3"/>
       <c r="U115" s="3"/>
@@ -2464,8 +2372,10 @@
       <c r="AA115" s="4"/>
       <c r="AB115" s="4"/>
     </row>
-    <row r="116" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P116" s="3"/>
       <c r="Q116"/>
+      <c r="R116" s="12"/>
       <c r="T116" s="3"/>
       <c r="U116" s="3"/>
       <c r="V116" s="3"/>
@@ -2476,7 +2386,7 @@
       <c r="AA116" s="4"/>
       <c r="AB116" s="4"/>
     </row>
-    <row r="117" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q117"/>
       <c r="T117" s="3"/>
       <c r="U117" s="3"/>
@@ -2488,7 +2398,7 @@
       <c r="AA117" s="4"/>
       <c r="AB117" s="4"/>
     </row>
-    <row r="118" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q118"/>
       <c r="T118" s="3"/>
       <c r="U118" s="3"/>
@@ -2500,7 +2410,7 @@
       <c r="AA118" s="4"/>
       <c r="AB118" s="4"/>
     </row>
-    <row r="119" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q119"/>
       <c r="T119" s="3"/>
       <c r="U119" s="3"/>
@@ -2512,7 +2422,7 @@
       <c r="AA119" s="4"/>
       <c r="AB119" s="4"/>
     </row>
-    <row r="120" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q120"/>
       <c r="T120" s="3"/>
       <c r="U120" s="3"/>
@@ -2524,9 +2434,8 @@
       <c r="AA120" s="4"/>
       <c r="AB120" s="4"/>
     </row>
-    <row r="121" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q121"/>
-      <c r="R121" s="12"/>
       <c r="T121" s="3"/>
       <c r="U121" s="3"/>
       <c r="V121" s="3"/>
@@ -2537,7 +2446,7 @@
       <c r="AA121" s="4"/>
       <c r="AB121" s="4"/>
     </row>
-    <row r="122" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q122"/>
       <c r="T122" s="3"/>
       <c r="U122" s="3"/>
@@ -2549,7 +2458,7 @@
       <c r="AA122" s="4"/>
       <c r="AB122" s="4"/>
     </row>
-    <row r="123" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q123"/>
       <c r="T123" s="3"/>
       <c r="U123" s="3"/>
@@ -2561,7 +2470,7 @@
       <c r="AA123" s="4"/>
       <c r="AB123" s="4"/>
     </row>
-    <row r="124" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q124"/>
       <c r="T124" s="3"/>
       <c r="U124" s="3"/>
@@ -2573,7 +2482,7 @@
       <c r="AA124" s="4"/>
       <c r="AB124" s="4"/>
     </row>
-    <row r="125" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q125"/>
       <c r="T125" s="3"/>
       <c r="U125" s="3"/>
@@ -2585,7 +2494,7 @@
       <c r="AA125" s="4"/>
       <c r="AB125" s="4"/>
     </row>
-    <row r="126" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q126"/>
       <c r="T126" s="3"/>
       <c r="U126" s="3"/>
@@ -2597,7 +2506,7 @@
       <c r="AA126" s="4"/>
       <c r="AB126" s="4"/>
     </row>
-    <row r="127" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q127"/>
       <c r="T127" s="3"/>
       <c r="U127" s="3"/>
@@ -2609,7 +2518,7 @@
       <c r="AA127" s="4"/>
       <c r="AB127" s="4"/>
     </row>
-    <row r="128" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q128"/>
       <c r="T128" s="3"/>
       <c r="U128" s="3"/>
@@ -2623,6 +2532,7 @@
     </row>
     <row r="129" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q129"/>
+      <c r="R129" s="12"/>
       <c r="T129" s="3"/>
       <c r="U129" s="3"/>
       <c r="V129" s="3"/>
@@ -2694,9 +2604,7 @@
       <c r="AB134" s="4"/>
     </row>
     <row r="135" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P135" s="3"/>
       <c r="Q135"/>
-      <c r="R135" s="12"/>
       <c r="T135" s="3"/>
       <c r="U135" s="3"/>
       <c r="V135" s="3"/>
@@ -2792,7 +2700,9 @@
       <c r="AB142" s="4"/>
     </row>
     <row r="143" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P143" s="3"/>
       <c r="Q143"/>
+      <c r="R143" s="12"/>
       <c r="T143" s="3"/>
       <c r="U143" s="3"/>
       <c r="V143" s="3"/>
@@ -2840,9 +2750,7 @@
       <c r="AB146" s="4"/>
     </row>
     <row r="147" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P147" s="3"/>
       <c r="Q147"/>
-      <c r="R147" s="12"/>
       <c r="T147" s="3"/>
       <c r="U147" s="3"/>
       <c r="V147" s="3"/>
@@ -2938,7 +2846,9 @@
       <c r="AB154" s="4"/>
     </row>
     <row r="155" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P155" s="3"/>
       <c r="Q155"/>
+      <c r="R155" s="12"/>
       <c r="T155" s="3"/>
       <c r="U155" s="3"/>
       <c r="V155" s="3"/>
@@ -3009,9 +2919,8 @@
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
     </row>
-    <row r="161" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="161" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q161"/>
-      <c r="R161" s="12"/>
       <c r="T161" s="3"/>
       <c r="U161" s="3"/>
       <c r="V161" s="3"/>
@@ -3022,7 +2931,7 @@
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
     </row>
-    <row r="162" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="162" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q162"/>
       <c r="T162" s="3"/>
       <c r="U162" s="3"/>
@@ -3034,7 +2943,7 @@
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
     </row>
-    <row r="163" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="163" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q163"/>
       <c r="T163" s="3"/>
       <c r="U163" s="3"/>
@@ -3046,7 +2955,7 @@
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
     </row>
-    <row r="164" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="164" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q164"/>
       <c r="T164" s="3"/>
       <c r="U164" s="3"/>
@@ -3058,7 +2967,7 @@
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
     </row>
-    <row r="165" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="165" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q165"/>
       <c r="T165" s="3"/>
       <c r="U165" s="3"/>
@@ -3070,7 +2979,7 @@
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
     </row>
-    <row r="166" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="166" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q166"/>
       <c r="T166" s="3"/>
       <c r="U166" s="3"/>
@@ -3082,7 +2991,7 @@
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
     </row>
-    <row r="167" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="167" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q167"/>
       <c r="T167" s="3"/>
       <c r="U167" s="3"/>
@@ -3094,7 +3003,7 @@
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
     </row>
-    <row r="168" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="168" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q168"/>
       <c r="T168" s="3"/>
       <c r="U168" s="3"/>
@@ -3106,8 +3015,9 @@
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
     </row>
-    <row r="169" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="169" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q169"/>
+      <c r="R169" s="12"/>
       <c r="T169" s="3"/>
       <c r="U169" s="3"/>
       <c r="V169" s="3"/>
@@ -3118,7 +3028,7 @@
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
     </row>
-    <row r="170" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="170" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q170"/>
       <c r="T170" s="3"/>
       <c r="U170" s="3"/>
@@ -3130,7 +3040,7 @@
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
     </row>
-    <row r="171" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="171" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q171"/>
       <c r="T171" s="3"/>
       <c r="U171" s="3"/>
@@ -3142,7 +3052,7 @@
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
     </row>
-    <row r="172" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="172" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q172"/>
       <c r="T172" s="3"/>
       <c r="U172" s="3"/>
@@ -3154,10 +3064,8 @@
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
     </row>
-    <row r="173" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P173" s="3"/>
+    <row r="173" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q173"/>
-      <c r="R173" s="12"/>
       <c r="T173" s="3"/>
       <c r="U173" s="3"/>
       <c r="V173" s="3"/>
@@ -3168,7 +3076,7 @@
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
     </row>
-    <row r="174" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="174" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q174"/>
       <c r="T174" s="3"/>
       <c r="U174" s="3"/>
@@ -3180,7 +3088,7 @@
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
     </row>
-    <row r="175" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="175" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q175"/>
       <c r="T175" s="3"/>
       <c r="U175" s="3"/>
@@ -3192,7 +3100,7 @@
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
     </row>
-    <row r="176" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="176" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q176"/>
       <c r="T176" s="3"/>
       <c r="U176" s="3"/>
@@ -3253,7 +3161,9 @@
       <c r="AB180" s="4"/>
     </row>
     <row r="181" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P181" s="3"/>
       <c r="Q181"/>
+      <c r="R181" s="12"/>
       <c r="T181" s="3"/>
       <c r="U181" s="3"/>
       <c r="V181" s="3"/>
@@ -3313,9 +3223,7 @@
       <c r="AB185" s="4"/>
     </row>
     <row r="186" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P186" s="3"/>
       <c r="Q186"/>
-      <c r="R186" s="12"/>
       <c r="T186" s="3"/>
       <c r="U186" s="3"/>
       <c r="V186" s="3"/>
@@ -3398,7 +3306,7 @@
       <c r="AA192" s="4"/>
       <c r="AB192" s="4"/>
     </row>
-    <row r="193" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="193" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q193"/>
       <c r="T193" s="3"/>
       <c r="U193" s="3"/>
@@ -3410,8 +3318,10 @@
       <c r="AA193" s="4"/>
       <c r="AB193" s="4"/>
     </row>
-    <row r="194" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="194" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P194" s="3"/>
       <c r="Q194"/>
+      <c r="R194" s="12"/>
       <c r="T194" s="3"/>
       <c r="U194" s="3"/>
       <c r="V194" s="3"/>
@@ -3422,9 +3332,8 @@
       <c r="AA194" s="4"/>
       <c r="AB194" s="4"/>
     </row>
-    <row r="195" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="195" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q195"/>
-      <c r="R195" s="12"/>
       <c r="T195" s="3"/>
       <c r="U195" s="3"/>
       <c r="V195" s="3"/>
@@ -3435,7 +3344,7 @@
       <c r="AA195" s="4"/>
       <c r="AB195" s="4"/>
     </row>
-    <row r="196" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="196" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q196"/>
       <c r="T196" s="3"/>
       <c r="U196" s="3"/>
@@ -3447,7 +3356,7 @@
       <c r="AA196" s="4"/>
       <c r="AB196" s="4"/>
     </row>
-    <row r="197" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="197" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q197"/>
       <c r="T197" s="3"/>
       <c r="U197" s="3"/>
@@ -3459,7 +3368,7 @@
       <c r="AA197" s="4"/>
       <c r="AB197" s="4"/>
     </row>
-    <row r="198" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="198" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q198"/>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
@@ -3471,7 +3380,7 @@
       <c r="AA198" s="4"/>
       <c r="AB198" s="4"/>
     </row>
-    <row r="199" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="199" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q199"/>
       <c r="T199" s="3"/>
       <c r="U199" s="3"/>
@@ -3483,7 +3392,7 @@
       <c r="AA199" s="4"/>
       <c r="AB199" s="4"/>
     </row>
-    <row r="200" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="200" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q200"/>
       <c r="T200" s="3"/>
       <c r="U200" s="3"/>
@@ -3495,7 +3404,7 @@
       <c r="AA200" s="4"/>
       <c r="AB200" s="4"/>
     </row>
-    <row r="201" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="201" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q201"/>
       <c r="T201" s="3"/>
       <c r="U201" s="3"/>
@@ -3507,7 +3416,7 @@
       <c r="AA201" s="4"/>
       <c r="AB201" s="4"/>
     </row>
-    <row r="202" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="202" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q202"/>
       <c r="T202" s="3"/>
       <c r="U202" s="3"/>
@@ -3519,8 +3428,9 @@
       <c r="AA202" s="4"/>
       <c r="AB202" s="4"/>
     </row>
-    <row r="203" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="203" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q203"/>
+      <c r="R203" s="12"/>
       <c r="T203" s="3"/>
       <c r="U203" s="3"/>
       <c r="V203" s="3"/>
@@ -3531,7 +3441,7 @@
       <c r="AA203" s="4"/>
       <c r="AB203" s="4"/>
     </row>
-    <row r="204" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="204" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q204"/>
       <c r="T204" s="3"/>
       <c r="U204" s="3"/>
@@ -3543,7 +3453,7 @@
       <c r="AA204" s="4"/>
       <c r="AB204" s="4"/>
     </row>
-    <row r="205" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="205" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q205"/>
       <c r="T205" s="3"/>
       <c r="U205" s="3"/>
@@ -3555,7 +3465,7 @@
       <c r="AA205" s="4"/>
       <c r="AB205" s="4"/>
     </row>
-    <row r="206" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="206" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q206"/>
       <c r="T206" s="3"/>
       <c r="U206" s="3"/>
@@ -3567,7 +3477,7 @@
       <c r="AA206" s="4"/>
       <c r="AB206" s="4"/>
     </row>
-    <row r="207" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="207" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q207"/>
       <c r="T207" s="3"/>
       <c r="U207" s="3"/>
@@ -3579,7 +3489,7 @@
       <c r="AA207" s="4"/>
       <c r="AB207" s="4"/>
     </row>
-    <row r="208" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="208" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q208"/>
       <c r="T208" s="3"/>
       <c r="U208" s="3"/>
@@ -3591,7 +3501,7 @@
       <c r="AA208" s="4"/>
       <c r="AB208" s="4"/>
     </row>
-    <row r="209" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="209" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q209"/>
       <c r="T209" s="3"/>
       <c r="U209" s="3"/>
@@ -3603,7 +3513,7 @@
       <c r="AA209" s="4"/>
       <c r="AB209" s="4"/>
     </row>
-    <row r="210" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="210" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q210"/>
       <c r="T210" s="3"/>
       <c r="U210" s="3"/>
@@ -3615,7 +3525,7 @@
       <c r="AA210" s="4"/>
       <c r="AB210" s="4"/>
     </row>
-    <row r="211" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="211" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q211"/>
       <c r="T211" s="3"/>
       <c r="U211" s="3"/>
@@ -3627,7 +3537,7 @@
       <c r="AA211" s="4"/>
       <c r="AB211" s="4"/>
     </row>
-    <row r="212" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="212" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q212"/>
       <c r="T212" s="3"/>
       <c r="U212" s="3"/>
@@ -3639,7 +3549,7 @@
       <c r="AA212" s="4"/>
       <c r="AB212" s="4"/>
     </row>
-    <row r="213" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="213" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q213"/>
       <c r="T213" s="3"/>
       <c r="U213" s="3"/>
@@ -3651,7 +3561,7 @@
       <c r="AA213" s="4"/>
       <c r="AB213" s="4"/>
     </row>
-    <row r="214" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="214" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q214"/>
       <c r="T214" s="3"/>
       <c r="U214" s="3"/>
@@ -3663,7 +3573,7 @@
       <c r="AA214" s="4"/>
       <c r="AB214" s="4"/>
     </row>
-    <row r="215" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="215" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q215"/>
       <c r="T215" s="3"/>
       <c r="U215" s="3"/>
@@ -3675,7 +3585,7 @@
       <c r="AA215" s="4"/>
       <c r="AB215" s="4"/>
     </row>
-    <row r="216" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="216" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q216"/>
       <c r="T216" s="3"/>
       <c r="U216" s="3"/>
@@ -3687,10 +3597,8 @@
       <c r="AA216" s="4"/>
       <c r="AB216" s="4"/>
     </row>
-    <row r="217" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P217" s="3"/>
+    <row r="217" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q217"/>
-      <c r="R217" s="12"/>
       <c r="T217" s="3"/>
       <c r="U217" s="3"/>
       <c r="V217" s="3"/>
@@ -3701,7 +3609,7 @@
       <c r="AA217" s="4"/>
       <c r="AB217" s="4"/>
     </row>
-    <row r="218" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="218" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q218"/>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
@@ -3713,7 +3621,7 @@
       <c r="AA218" s="4"/>
       <c r="AB218" s="4"/>
     </row>
-    <row r="219" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="219" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q219"/>
       <c r="T219" s="3"/>
       <c r="U219" s="3"/>
@@ -3725,7 +3633,7 @@
       <c r="AA219" s="4"/>
       <c r="AB219" s="4"/>
     </row>
-    <row r="220" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="220" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q220"/>
       <c r="T220" s="3"/>
       <c r="U220" s="3"/>
@@ -3737,7 +3645,7 @@
       <c r="AA220" s="4"/>
       <c r="AB220" s="4"/>
     </row>
-    <row r="221" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="221" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q221"/>
       <c r="T221" s="3"/>
       <c r="U221" s="3"/>
@@ -3749,7 +3657,7 @@
       <c r="AA221" s="4"/>
       <c r="AB221" s="4"/>
     </row>
-    <row r="222" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="222" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q222"/>
       <c r="T222" s="3"/>
       <c r="U222" s="3"/>
@@ -3761,7 +3669,7 @@
       <c r="AA222" s="4"/>
       <c r="AB222" s="4"/>
     </row>
-    <row r="223" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="223" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q223"/>
       <c r="T223" s="3"/>
       <c r="U223" s="3"/>
@@ -3773,7 +3681,7 @@
       <c r="AA223" s="4"/>
       <c r="AB223" s="4"/>
     </row>
-    <row r="224" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="224" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q224"/>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
@@ -3786,7 +3694,9 @@
       <c r="AB224" s="4"/>
     </row>
     <row r="225" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P225" s="3"/>
       <c r="Q225"/>
+      <c r="R225" s="12"/>
       <c r="T225" s="3"/>
       <c r="U225" s="3"/>
       <c r="V225" s="3"/>
@@ -3906,9 +3816,7 @@
       <c r="AB234" s="4"/>
     </row>
     <row r="235" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P235" s="3"/>
       <c r="Q235"/>
-      <c r="R235" s="12"/>
       <c r="T235" s="3"/>
       <c r="U235" s="3"/>
       <c r="V235" s="3"/>
@@ -3993,7 +3901,6 @@
     </row>
     <row r="242" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q242"/>
-      <c r="R242" s="12"/>
       <c r="T242" s="3"/>
       <c r="U242" s="3"/>
       <c r="V242" s="3"/>
@@ -4005,7 +3912,9 @@
       <c r="AB242" s="4"/>
     </row>
     <row r="243" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P243" s="3"/>
       <c r="Q243"/>
+      <c r="R243" s="12"/>
       <c r="T243" s="3"/>
       <c r="U243" s="3"/>
       <c r="V243" s="3"/>
@@ -4090,6 +3999,7 @@
     </row>
     <row r="250" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q250"/>
+      <c r="R250" s="12"/>
       <c r="T250" s="3"/>
       <c r="U250" s="3"/>
       <c r="V250" s="3"/>
@@ -4113,9 +4023,7 @@
       <c r="AB251" s="4"/>
     </row>
     <row r="252" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P252" s="3"/>
       <c r="Q252"/>
-      <c r="R252" s="12"/>
       <c r="T252" s="3"/>
       <c r="U252" s="3"/>
       <c r="V252" s="3"/>
@@ -4211,7 +4119,9 @@
       <c r="AB259" s="4"/>
     </row>
     <row r="260" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P260" s="3"/>
       <c r="Q260"/>
+      <c r="R260" s="12"/>
       <c r="T260" s="3"/>
       <c r="U260" s="3"/>
       <c r="V260" s="3"/>
@@ -4223,9 +4133,7 @@
       <c r="AB260" s="4"/>
     </row>
     <row r="261" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P261" s="3"/>
       <c r="Q261"/>
-      <c r="R261" s="12"/>
       <c r="T261" s="3"/>
       <c r="U261" s="3"/>
       <c r="V261" s="3"/>
@@ -4321,7 +4229,9 @@
       <c r="AB268" s="4"/>
     </row>
     <row r="269" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P269" s="3"/>
       <c r="Q269"/>
+      <c r="R269" s="12"/>
       <c r="T269" s="3"/>
       <c r="U269" s="3"/>
       <c r="V269" s="3"/>
@@ -4334,7 +4244,6 @@
     </row>
     <row r="270" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q270"/>
-      <c r="R270" s="12"/>
       <c r="T270" s="3"/>
       <c r="U270" s="3"/>
       <c r="V270" s="3"/>
@@ -4369,7 +4278,7 @@
       <c r="AA272" s="4"/>
       <c r="AB272" s="4"/>
     </row>
-    <row r="273" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="273" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q273"/>
       <c r="T273" s="3"/>
       <c r="U273" s="3"/>
@@ -4381,7 +4290,7 @@
       <c r="AA273" s="4"/>
       <c r="AB273" s="4"/>
     </row>
-    <row r="274" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="274" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q274"/>
       <c r="T274" s="3"/>
       <c r="U274" s="3"/>
@@ -4393,7 +4302,7 @@
       <c r="AA274" s="4"/>
       <c r="AB274" s="4"/>
     </row>
-    <row r="275" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="275" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q275"/>
       <c r="T275" s="3"/>
       <c r="U275" s="3"/>
@@ -4405,7 +4314,7 @@
       <c r="AA275" s="4"/>
       <c r="AB275" s="4"/>
     </row>
-    <row r="276" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="276" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q276"/>
       <c r="T276" s="3"/>
       <c r="U276" s="3"/>
@@ -4417,7 +4326,7 @@
       <c r="AA276" s="4"/>
       <c r="AB276" s="4"/>
     </row>
-    <row r="277" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="277" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q277"/>
       <c r="T277" s="3"/>
       <c r="U277" s="3"/>
@@ -4429,8 +4338,9 @@
       <c r="AA277" s="4"/>
       <c r="AB277" s="4"/>
     </row>
-    <row r="278" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="278" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q278"/>
+      <c r="R278" s="12"/>
       <c r="T278" s="3"/>
       <c r="U278" s="3"/>
       <c r="V278" s="3"/>
@@ -4441,7 +4351,7 @@
       <c r="AA278" s="4"/>
       <c r="AB278" s="4"/>
     </row>
-    <row r="279" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="279" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q279"/>
       <c r="T279" s="3"/>
       <c r="U279" s="3"/>
@@ -4453,7 +4363,7 @@
       <c r="AA279" s="4"/>
       <c r="AB279" s="4"/>
     </row>
-    <row r="280" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="280" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q280"/>
       <c r="T280" s="3"/>
       <c r="U280" s="3"/>
@@ -4465,10 +4375,8 @@
       <c r="AA280" s="4"/>
       <c r="AB280" s="4"/>
     </row>
-    <row r="281" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P281" s="3"/>
+    <row r="281" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q281"/>
-      <c r="R281" s="12"/>
       <c r="T281" s="3"/>
       <c r="U281" s="3"/>
       <c r="V281" s="3"/>
@@ -4479,7 +4387,7 @@
       <c r="AA281" s="4"/>
       <c r="AB281" s="4"/>
     </row>
-    <row r="282" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="282" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q282"/>
       <c r="T282" s="3"/>
       <c r="U282" s="3"/>
@@ -4491,7 +4399,7 @@
       <c r="AA282" s="4"/>
       <c r="AB282" s="4"/>
     </row>
-    <row r="283" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="283" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q283"/>
       <c r="T283" s="3"/>
       <c r="U283" s="3"/>
@@ -4503,7 +4411,7 @@
       <c r="AA283" s="4"/>
       <c r="AB283" s="4"/>
     </row>
-    <row r="284" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="284" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q284"/>
       <c r="T284" s="3"/>
       <c r="U284" s="3"/>
@@ -4515,7 +4423,7 @@
       <c r="AA284" s="4"/>
       <c r="AB284" s="4"/>
     </row>
-    <row r="285" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="285" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q285"/>
       <c r="T285" s="3"/>
       <c r="U285" s="3"/>
@@ -4527,7 +4435,7 @@
       <c r="AA285" s="4"/>
       <c r="AB285" s="4"/>
     </row>
-    <row r="286" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="286" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q286"/>
       <c r="T286" s="3"/>
       <c r="U286" s="3"/>
@@ -4539,7 +4447,7 @@
       <c r="AA286" s="4"/>
       <c r="AB286" s="4"/>
     </row>
-    <row r="287" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="287" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q287"/>
       <c r="T287" s="3"/>
       <c r="U287" s="3"/>
@@ -4551,7 +4459,7 @@
       <c r="AA287" s="4"/>
       <c r="AB287" s="4"/>
     </row>
-    <row r="288" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="288" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q288"/>
       <c r="T288" s="3"/>
       <c r="U288" s="3"/>
@@ -4564,7 +4472,9 @@
       <c r="AB288" s="4"/>
     </row>
     <row r="289" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P289" s="3"/>
       <c r="Q289"/>
+      <c r="R289" s="12"/>
       <c r="T289" s="3"/>
       <c r="U289" s="3"/>
       <c r="V289" s="3"/>
@@ -4708,9 +4618,7 @@
       <c r="AB300" s="4"/>
     </row>
     <row r="301" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P301" s="3"/>
       <c r="Q301"/>
-      <c r="R301" s="12"/>
       <c r="T301" s="3"/>
       <c r="U301" s="3"/>
       <c r="V301" s="3"/>
@@ -4806,7 +4714,9 @@
       <c r="AB308" s="4"/>
     </row>
     <row r="309" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P309" s="3"/>
       <c r="Q309"/>
+      <c r="R309" s="12"/>
       <c r="T309" s="3"/>
       <c r="U309" s="3"/>
       <c r="V309" s="3"/>
@@ -4830,9 +4740,7 @@
       <c r="AB310" s="4"/>
     </row>
     <row r="311" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P311" s="3"/>
       <c r="Q311"/>
-      <c r="R311" s="12"/>
       <c r="T311" s="3"/>
       <c r="U311" s="3"/>
       <c r="V311" s="3"/>
@@ -4928,7 +4836,9 @@
       <c r="AB318" s="4"/>
     </row>
     <row r="319" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P319" s="3"/>
       <c r="Q319"/>
+      <c r="R319" s="12"/>
       <c r="T319" s="3"/>
       <c r="U319" s="3"/>
       <c r="V319" s="3"/>
@@ -5061,7 +4971,6 @@
     </row>
     <row r="330" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q330"/>
-      <c r="R330" s="12"/>
       <c r="T330" s="3"/>
       <c r="U330" s="3"/>
       <c r="V330" s="3"/>
@@ -5144,9 +5053,8 @@
       <c r="AA336" s="4"/>
       <c r="AB336" s="4"/>
     </row>
-    <row r="337" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="337" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q337"/>
-      <c r="R337" s="12"/>
       <c r="T337" s="3"/>
       <c r="U337" s="3"/>
       <c r="V337" s="3"/>
@@ -5157,8 +5065,9 @@
       <c r="AA337" s="4"/>
       <c r="AB337" s="4"/>
     </row>
-    <row r="338" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="338" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q338"/>
+      <c r="R338" s="12"/>
       <c r="T338" s="3"/>
       <c r="U338" s="3"/>
       <c r="V338" s="3"/>
@@ -5169,7 +5078,7 @@
       <c r="AA338" s="4"/>
       <c r="AB338" s="4"/>
     </row>
-    <row r="339" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="339" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q339"/>
       <c r="T339" s="3"/>
       <c r="U339" s="3"/>
@@ -5181,7 +5090,7 @@
       <c r="AA339" s="4"/>
       <c r="AB339" s="4"/>
     </row>
-    <row r="340" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="340" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q340"/>
       <c r="T340" s="3"/>
       <c r="U340" s="3"/>
@@ -5193,7 +5102,7 @@
       <c r="AA340" s="4"/>
       <c r="AB340" s="4"/>
     </row>
-    <row r="341" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="341" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q341"/>
       <c r="T341" s="3"/>
       <c r="U341" s="3"/>
@@ -5205,7 +5114,7 @@
       <c r="AA341" s="4"/>
       <c r="AB341" s="4"/>
     </row>
-    <row r="342" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="342" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q342"/>
       <c r="T342" s="3"/>
       <c r="U342" s="3"/>
@@ -5217,7 +5126,7 @@
       <c r="AA342" s="4"/>
       <c r="AB342" s="4"/>
     </row>
-    <row r="343" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="343" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q343"/>
       <c r="T343" s="3"/>
       <c r="U343" s="3"/>
@@ -5229,7 +5138,7 @@
       <c r="AA343" s="4"/>
       <c r="AB343" s="4"/>
     </row>
-    <row r="344" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="344" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q344"/>
       <c r="T344" s="3"/>
       <c r="U344" s="3"/>
@@ -5241,8 +5150,7 @@
       <c r="AA344" s="4"/>
       <c r="AB344" s="4"/>
     </row>
-    <row r="345" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P345" s="3"/>
+    <row r="345" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q345"/>
       <c r="R345" s="12"/>
       <c r="T345" s="3"/>
@@ -5255,7 +5163,7 @@
       <c r="AA345" s="4"/>
       <c r="AB345" s="4"/>
     </row>
-    <row r="346" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="346" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q346"/>
       <c r="T346" s="3"/>
       <c r="U346" s="3"/>
@@ -5267,7 +5175,7 @@
       <c r="AA346" s="4"/>
       <c r="AB346" s="4"/>
     </row>
-    <row r="347" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="347" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q347"/>
       <c r="T347" s="3"/>
       <c r="U347" s="3"/>
@@ -5279,7 +5187,7 @@
       <c r="AA347" s="4"/>
       <c r="AB347" s="4"/>
     </row>
-    <row r="348" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="348" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q348"/>
       <c r="T348" s="3"/>
       <c r="U348" s="3"/>
@@ -5291,7 +5199,7 @@
       <c r="AA348" s="4"/>
       <c r="AB348" s="4"/>
     </row>
-    <row r="349" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="349" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q349"/>
       <c r="T349" s="3"/>
       <c r="U349" s="3"/>
@@ -5303,7 +5211,7 @@
       <c r="AA349" s="4"/>
       <c r="AB349" s="4"/>
     </row>
-    <row r="350" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="350" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q350"/>
       <c r="T350" s="3"/>
       <c r="U350" s="3"/>
@@ -5315,9 +5223,8 @@
       <c r="AA350" s="4"/>
       <c r="AB350" s="4"/>
     </row>
-    <row r="351" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="351" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q351"/>
-      <c r="R351" s="12"/>
       <c r="T351" s="3"/>
       <c r="U351" s="3"/>
       <c r="V351" s="3"/>
@@ -5328,7 +5235,7 @@
       <c r="AA351" s="4"/>
       <c r="AB351" s="4"/>
     </row>
-    <row r="352" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="352" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q352"/>
       <c r="T352" s="3"/>
       <c r="U352" s="3"/>
@@ -5341,7 +5248,9 @@
       <c r="AB352" s="4"/>
     </row>
     <row r="353" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P353" s="3"/>
       <c r="Q353"/>
+      <c r="R353" s="12"/>
       <c r="T353" s="3"/>
       <c r="U353" s="3"/>
       <c r="V353" s="3"/>
@@ -5377,9 +5286,7 @@
       <c r="AB355" s="4"/>
     </row>
     <row r="356" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P356" s="3"/>
       <c r="Q356"/>
-      <c r="R356" s="12"/>
       <c r="T356" s="3"/>
       <c r="U356" s="3"/>
       <c r="V356" s="3"/>
@@ -5416,6 +5323,7 @@
     </row>
     <row r="359" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q359"/>
+      <c r="R359" s="12"/>
       <c r="T359" s="3"/>
       <c r="U359" s="3"/>
       <c r="V359" s="3"/>
@@ -5475,7 +5383,9 @@
       <c r="AB363" s="4"/>
     </row>
     <row r="364" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P364" s="3"/>
       <c r="Q364"/>
+      <c r="R364" s="12"/>
       <c r="T364" s="3"/>
       <c r="U364" s="3"/>
       <c r="V364" s="3"/>
@@ -5499,9 +5409,7 @@
       <c r="AB365" s="4"/>
     </row>
     <row r="366" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P366" s="3"/>
       <c r="Q366"/>
-      <c r="R366" s="12"/>
       <c r="T366" s="3"/>
       <c r="U366" s="3"/>
       <c r="V366" s="3"/>
@@ -5536,7 +5444,7 @@
       <c r="AA368" s="4"/>
       <c r="AB368" s="4"/>
     </row>
-    <row r="369" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="369" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q369"/>
       <c r="T369" s="3"/>
       <c r="U369" s="3"/>
@@ -5548,7 +5456,7 @@
       <c r="AA369" s="4"/>
       <c r="AB369" s="4"/>
     </row>
-    <row r="370" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="370" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q370"/>
       <c r="T370" s="3"/>
       <c r="U370" s="3"/>
@@ -5560,7 +5468,7 @@
       <c r="AA370" s="4"/>
       <c r="AB370" s="4"/>
     </row>
-    <row r="371" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="371" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q371"/>
       <c r="T371" s="3"/>
       <c r="U371" s="3"/>
@@ -5572,7 +5480,7 @@
       <c r="AA371" s="4"/>
       <c r="AB371" s="4"/>
     </row>
-    <row r="372" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="372" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q372"/>
       <c r="T372" s="3"/>
       <c r="U372" s="3"/>
@@ -5584,7 +5492,7 @@
       <c r="AA372" s="4"/>
       <c r="AB372" s="4"/>
     </row>
-    <row r="373" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="373" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q373"/>
       <c r="T373" s="3"/>
       <c r="U373" s="3"/>
@@ -5596,8 +5504,10 @@
       <c r="AA373" s="4"/>
       <c r="AB373" s="4"/>
     </row>
-    <row r="374" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="374" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P374" s="3"/>
       <c r="Q374"/>
+      <c r="R374" s="12"/>
       <c r="T374" s="3"/>
       <c r="U374" s="3"/>
       <c r="V374" s="3"/>
@@ -5608,7 +5518,7 @@
       <c r="AA374" s="4"/>
       <c r="AB374" s="4"/>
     </row>
-    <row r="375" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="375" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q375"/>
       <c r="T375" s="3"/>
       <c r="U375" s="3"/>
@@ -5620,7 +5530,7 @@
       <c r="AA375" s="4"/>
       <c r="AB375" s="4"/>
     </row>
-    <row r="376" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="376" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q376"/>
       <c r="T376" s="3"/>
       <c r="U376" s="3"/>
@@ -5632,7 +5542,7 @@
       <c r="AA376" s="4"/>
       <c r="AB376" s="4"/>
     </row>
-    <row r="377" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="377" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q377"/>
       <c r="T377" s="3"/>
       <c r="U377" s="3"/>
@@ -5644,7 +5554,7 @@
       <c r="AA377" s="4"/>
       <c r="AB377" s="4"/>
     </row>
-    <row r="378" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="378" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q378"/>
       <c r="T378" s="3"/>
       <c r="U378" s="3"/>
@@ -5656,7 +5566,7 @@
       <c r="AA378" s="4"/>
       <c r="AB378" s="4"/>
     </row>
-    <row r="379" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="379" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q379"/>
       <c r="T379" s="3"/>
       <c r="U379" s="3"/>
@@ -5668,7 +5578,7 @@
       <c r="AA379" s="4"/>
       <c r="AB379" s="4"/>
     </row>
-    <row r="380" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="380" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q380"/>
       <c r="T380" s="3"/>
       <c r="U380" s="3"/>
@@ -5680,7 +5590,7 @@
       <c r="AA380" s="4"/>
       <c r="AB380" s="4"/>
     </row>
-    <row r="381" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="381" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q381"/>
       <c r="T381" s="3"/>
       <c r="U381" s="3"/>
@@ -5692,7 +5602,7 @@
       <c r="AA381" s="4"/>
       <c r="AB381" s="4"/>
     </row>
-    <row r="382" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="382" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q382"/>
       <c r="T382" s="3"/>
       <c r="U382" s="3"/>
@@ -5704,7 +5614,7 @@
       <c r="AA382" s="4"/>
       <c r="AB382" s="4"/>
     </row>
-    <row r="383" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="383" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q383"/>
       <c r="T383" s="3"/>
       <c r="U383" s="3"/>
@@ -5716,7 +5626,7 @@
       <c r="AA383" s="4"/>
       <c r="AB383" s="4"/>
     </row>
-    <row r="384" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="384" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q384"/>
       <c r="T384" s="3"/>
       <c r="U384" s="3"/>
@@ -5729,9 +5639,7 @@
       <c r="AB384" s="4"/>
     </row>
     <row r="385" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P385" s="3"/>
       <c r="Q385"/>
-      <c r="R385" s="12"/>
       <c r="T385" s="3"/>
       <c r="U385" s="3"/>
       <c r="V385" s="3"/>
@@ -5827,7 +5735,9 @@
       <c r="AB392" s="4"/>
     </row>
     <row r="393" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P393" s="3"/>
       <c r="Q393"/>
+      <c r="R393" s="12"/>
       <c r="T393" s="3"/>
       <c r="U393" s="3"/>
       <c r="V393" s="3"/>
@@ -5983,9 +5893,7 @@
       <c r="AB405" s="4"/>
     </row>
     <row r="406" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P406" s="3"/>
       <c r="Q406"/>
-      <c r="R406" s="12"/>
       <c r="T406" s="3"/>
       <c r="U406" s="3"/>
       <c r="V406" s="3"/>
@@ -6081,7 +5989,9 @@
       <c r="AB413" s="4"/>
     </row>
     <row r="414" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P414" s="3"/>
       <c r="Q414"/>
+      <c r="R414" s="12"/>
       <c r="T414" s="3"/>
       <c r="U414" s="3"/>
       <c r="V414" s="3"/>
@@ -6238,7 +6148,6 @@
     </row>
     <row r="427" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q427"/>
-      <c r="R427" s="12"/>
       <c r="T427" s="3"/>
       <c r="U427" s="3"/>
       <c r="V427" s="3"/>
@@ -6309,7 +6218,7 @@
       <c r="AA432" s="4"/>
       <c r="AB432" s="4"/>
     </row>
-    <row r="433" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="433" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q433"/>
       <c r="T433" s="3"/>
       <c r="U433" s="3"/>
@@ -6321,7 +6230,7 @@
       <c r="AA433" s="4"/>
       <c r="AB433" s="4"/>
     </row>
-    <row r="434" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="434" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q434"/>
       <c r="T434" s="3"/>
       <c r="U434" s="3"/>
@@ -6333,8 +6242,9 @@
       <c r="AA434" s="4"/>
       <c r="AB434" s="4"/>
     </row>
-    <row r="435" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="435" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q435"/>
+      <c r="R435" s="12"/>
       <c r="T435" s="3"/>
       <c r="U435" s="3"/>
       <c r="V435" s="3"/>
@@ -6345,7 +6255,7 @@
       <c r="AA435" s="4"/>
       <c r="AB435" s="4"/>
     </row>
-    <row r="436" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="436" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q436"/>
       <c r="T436" s="3"/>
       <c r="U436" s="3"/>
@@ -6357,7 +6267,7 @@
       <c r="AA436" s="4"/>
       <c r="AB436" s="4"/>
     </row>
-    <row r="437" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="437" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q437"/>
       <c r="T437" s="3"/>
       <c r="U437" s="3"/>
@@ -6369,7 +6279,7 @@
       <c r="AA437" s="4"/>
       <c r="AB437" s="4"/>
     </row>
-    <row r="438" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="438" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q438"/>
       <c r="T438" s="3"/>
       <c r="U438" s="3"/>
@@ -6381,7 +6291,7 @@
       <c r="AA438" s="4"/>
       <c r="AB438" s="4"/>
     </row>
-    <row r="439" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="439" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q439"/>
       <c r="T439" s="3"/>
       <c r="U439" s="3"/>
@@ -6393,7 +6303,7 @@
       <c r="AA439" s="4"/>
       <c r="AB439" s="4"/>
     </row>
-    <row r="440" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="440" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q440"/>
       <c r="T440" s="3"/>
       <c r="U440" s="3"/>
@@ -6405,7 +6315,7 @@
       <c r="AA440" s="4"/>
       <c r="AB440" s="4"/>
     </row>
-    <row r="441" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="441" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q441"/>
       <c r="T441" s="3"/>
       <c r="U441" s="3"/>
@@ -6417,7 +6327,7 @@
       <c r="AA441" s="4"/>
       <c r="AB441" s="4"/>
     </row>
-    <row r="442" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="442" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q442"/>
       <c r="T442" s="3"/>
       <c r="U442" s="3"/>
@@ -6429,7 +6339,7 @@
       <c r="AA442" s="4"/>
       <c r="AB442" s="4"/>
     </row>
-    <row r="443" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="443" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q443"/>
       <c r="T443" s="3"/>
       <c r="U443" s="3"/>
@@ -6441,7 +6351,7 @@
       <c r="AA443" s="4"/>
       <c r="AB443" s="4"/>
     </row>
-    <row r="444" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="444" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q444"/>
       <c r="T444" s="3"/>
       <c r="U444" s="3"/>
@@ -6453,7 +6363,7 @@
       <c r="AA444" s="4"/>
       <c r="AB444" s="4"/>
     </row>
-    <row r="445" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="445" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q445"/>
       <c r="T445" s="3"/>
       <c r="U445" s="3"/>
@@ -6465,10 +6375,8 @@
       <c r="AA445" s="4"/>
       <c r="AB445" s="4"/>
     </row>
-    <row r="446" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P446" s="3"/>
+    <row r="446" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q446"/>
-      <c r="R446" s="12"/>
       <c r="T446" s="3"/>
       <c r="U446" s="3"/>
       <c r="V446" s="3"/>
@@ -6479,7 +6387,7 @@
       <c r="AA446" s="4"/>
       <c r="AB446" s="4"/>
     </row>
-    <row r="447" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="447" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q447"/>
       <c r="T447" s="3"/>
       <c r="U447" s="3"/>
@@ -6491,7 +6399,7 @@
       <c r="AA447" s="4"/>
       <c r="AB447" s="4"/>
     </row>
-    <row r="448" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="448" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q448"/>
       <c r="T448" s="3"/>
       <c r="U448" s="3"/>
@@ -6503,7 +6411,7 @@
       <c r="AA448" s="4"/>
       <c r="AB448" s="4"/>
     </row>
-    <row r="449" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="449" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q449"/>
       <c r="T449" s="3"/>
       <c r="U449" s="3"/>
@@ -6515,7 +6423,7 @@
       <c r="AA449" s="4"/>
       <c r="AB449" s="4"/>
     </row>
-    <row r="450" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="450" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q450"/>
       <c r="T450" s="3"/>
       <c r="U450" s="3"/>
@@ -6527,7 +6435,7 @@
       <c r="AA450" s="4"/>
       <c r="AB450" s="4"/>
     </row>
-    <row r="451" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="451" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q451"/>
       <c r="T451" s="3"/>
       <c r="U451" s="3"/>
@@ -6539,7 +6447,7 @@
       <c r="AA451" s="4"/>
       <c r="AB451" s="4"/>
     </row>
-    <row r="452" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="452" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q452"/>
       <c r="T452" s="3"/>
       <c r="U452" s="3"/>
@@ -6551,7 +6459,7 @@
       <c r="AA452" s="4"/>
       <c r="AB452" s="4"/>
     </row>
-    <row r="453" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="453" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q453"/>
       <c r="T453" s="3"/>
       <c r="U453" s="3"/>
@@ -6563,8 +6471,10 @@
       <c r="AA453" s="4"/>
       <c r="AB453" s="4"/>
     </row>
-    <row r="454" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="454" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P454" s="3"/>
       <c r="Q454"/>
+      <c r="R454" s="12"/>
       <c r="T454" s="3"/>
       <c r="U454" s="3"/>
       <c r="V454" s="3"/>
@@ -6575,7 +6485,7 @@
       <c r="AA454" s="4"/>
       <c r="AB454" s="4"/>
     </row>
-    <row r="455" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="455" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q455"/>
       <c r="T455" s="3"/>
       <c r="U455" s="3"/>
@@ -6587,7 +6497,7 @@
       <c r="AA455" s="4"/>
       <c r="AB455" s="4"/>
     </row>
-    <row r="456" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="456" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q456"/>
       <c r="T456" s="3"/>
       <c r="U456" s="3"/>
@@ -6599,7 +6509,7 @@
       <c r="AA456" s="4"/>
       <c r="AB456" s="4"/>
     </row>
-    <row r="457" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="457" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q457"/>
       <c r="T457" s="3"/>
       <c r="U457" s="3"/>
@@ -6611,7 +6521,7 @@
       <c r="AA457" s="4"/>
       <c r="AB457" s="4"/>
     </row>
-    <row r="458" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="458" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q458"/>
       <c r="T458" s="3"/>
       <c r="U458" s="3"/>
@@ -6623,7 +6533,7 @@
       <c r="AA458" s="4"/>
       <c r="AB458" s="4"/>
     </row>
-    <row r="459" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="459" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q459"/>
       <c r="T459" s="3"/>
       <c r="U459" s="3"/>
@@ -6635,7 +6545,7 @@
       <c r="AA459" s="4"/>
       <c r="AB459" s="4"/>
     </row>
-    <row r="460" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="460" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q460"/>
       <c r="T460" s="3"/>
       <c r="U460" s="3"/>
@@ -6647,7 +6557,7 @@
       <c r="AA460" s="4"/>
       <c r="AB460" s="4"/>
     </row>
-    <row r="461" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="461" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q461"/>
       <c r="T461" s="3"/>
       <c r="U461" s="3"/>
@@ -6659,7 +6569,7 @@
       <c r="AA461" s="4"/>
       <c r="AB461" s="4"/>
     </row>
-    <row r="462" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="462" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q462"/>
       <c r="T462" s="3"/>
       <c r="U462" s="3"/>
@@ -6671,7 +6581,7 @@
       <c r="AA462" s="4"/>
       <c r="AB462" s="4"/>
     </row>
-    <row r="463" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="463" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q463"/>
       <c r="T463" s="3"/>
       <c r="U463" s="3"/>
@@ -6683,7 +6593,7 @@
       <c r="AA463" s="4"/>
       <c r="AB463" s="4"/>
     </row>
-    <row r="464" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="464" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q464"/>
       <c r="T464" s="3"/>
       <c r="U464" s="3"/>
@@ -6756,9 +6666,7 @@
       <c r="AB469" s="4"/>
     </row>
     <row r="470" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P470" s="3"/>
       <c r="Q470"/>
-      <c r="R470" s="12"/>
       <c r="T470" s="3"/>
       <c r="U470" s="3"/>
       <c r="V470" s="3"/>
@@ -6854,7 +6762,9 @@
       <c r="AB477" s="4"/>
     </row>
     <row r="478" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P478" s="3"/>
       <c r="Q478"/>
+      <c r="R478" s="12"/>
       <c r="T478" s="3"/>
       <c r="U478" s="3"/>
       <c r="V478" s="3"/>
@@ -6889,7 +6799,7 @@
       <c r="AA480" s="4"/>
       <c r="AB480" s="4"/>
     </row>
-    <row r="481" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="481" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q481"/>
       <c r="T481" s="3"/>
       <c r="U481" s="3"/>
@@ -6901,7 +6811,7 @@
       <c r="AA481" s="4"/>
       <c r="AB481" s="4"/>
     </row>
-    <row r="482" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="482" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q482"/>
       <c r="T482" s="3"/>
       <c r="U482" s="3"/>
@@ -6913,7 +6823,7 @@
       <c r="AA482" s="4"/>
       <c r="AB482" s="4"/>
     </row>
-    <row r="483" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="483" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q483"/>
       <c r="T483" s="3"/>
       <c r="U483" s="3"/>
@@ -6925,7 +6835,7 @@
       <c r="AA483" s="4"/>
       <c r="AB483" s="4"/>
     </row>
-    <row r="484" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="484" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q484"/>
       <c r="T484" s="3"/>
       <c r="U484" s="3"/>
@@ -6937,7 +6847,7 @@
       <c r="AA484" s="4"/>
       <c r="AB484" s="4"/>
     </row>
-    <row r="485" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="485" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q485"/>
       <c r="T485" s="3"/>
       <c r="U485" s="3"/>
@@ -6949,7 +6859,7 @@
       <c r="AA485" s="4"/>
       <c r="AB485" s="4"/>
     </row>
-    <row r="486" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="486" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q486"/>
       <c r="T486" s="3"/>
       <c r="U486" s="3"/>
@@ -6961,7 +6871,7 @@
       <c r="AA486" s="4"/>
       <c r="AB486" s="4"/>
     </row>
-    <row r="487" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="487" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q487"/>
       <c r="T487" s="3"/>
       <c r="U487" s="3"/>
@@ -6973,7 +6883,7 @@
       <c r="AA487" s="4"/>
       <c r="AB487" s="4"/>
     </row>
-    <row r="488" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="488" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q488"/>
       <c r="T488" s="3"/>
       <c r="U488" s="3"/>
@@ -6985,10 +6895,8 @@
       <c r="AA488" s="4"/>
       <c r="AB488" s="4"/>
     </row>
-    <row r="489" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P489" s="3"/>
+    <row r="489" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q489"/>
-      <c r="R489" s="12"/>
       <c r="T489" s="3"/>
       <c r="U489" s="3"/>
       <c r="V489" s="3"/>
@@ -6999,7 +6907,7 @@
       <c r="AA489" s="4"/>
       <c r="AB489" s="4"/>
     </row>
-    <row r="490" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="490" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q490"/>
       <c r="T490" s="3"/>
       <c r="U490" s="3"/>
@@ -7011,7 +6919,7 @@
       <c r="AA490" s="4"/>
       <c r="AB490" s="4"/>
     </row>
-    <row r="491" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="491" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q491"/>
       <c r="T491" s="3"/>
       <c r="U491" s="3"/>
@@ -7023,7 +6931,7 @@
       <c r="AA491" s="4"/>
       <c r="AB491" s="4"/>
     </row>
-    <row r="492" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="492" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q492"/>
       <c r="T492" s="3"/>
       <c r="U492" s="3"/>
@@ -7035,7 +6943,7 @@
       <c r="AA492" s="4"/>
       <c r="AB492" s="4"/>
     </row>
-    <row r="493" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="493" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q493"/>
       <c r="T493" s="3"/>
       <c r="U493" s="3"/>
@@ -7047,7 +6955,7 @@
       <c r="AA493" s="4"/>
       <c r="AB493" s="4"/>
     </row>
-    <row r="494" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="494" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q494"/>
       <c r="T494" s="3"/>
       <c r="U494" s="3"/>
@@ -7059,10 +6967,8 @@
       <c r="AA494" s="4"/>
       <c r="AB494" s="4"/>
     </row>
-    <row r="495" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P495" s="3"/>
+    <row r="495" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q495"/>
-      <c r="R495" s="12"/>
       <c r="T495" s="3"/>
       <c r="U495" s="3"/>
       <c r="V495" s="3"/>
@@ -7073,7 +6979,7 @@
       <c r="AA495" s="4"/>
       <c r="AB495" s="4"/>
     </row>
-    <row r="496" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="496" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q496"/>
       <c r="T496" s="3"/>
       <c r="U496" s="3"/>
@@ -7085,8 +6991,10 @@
       <c r="AA496" s="4"/>
       <c r="AB496" s="4"/>
     </row>
-    <row r="497" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="497" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P497" s="3"/>
       <c r="Q497"/>
+      <c r="R497" s="12"/>
       <c r="T497" s="3"/>
       <c r="U497" s="3"/>
       <c r="V497" s="3"/>
@@ -7097,7 +7005,7 @@
       <c r="AA497" s="4"/>
       <c r="AB497" s="4"/>
     </row>
-    <row r="498" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="498" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q498"/>
       <c r="T498" s="3"/>
       <c r="U498" s="3"/>
@@ -7109,7 +7017,7 @@
       <c r="AA498" s="4"/>
       <c r="AB498" s="4"/>
     </row>
-    <row r="499" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="499" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q499"/>
       <c r="T499" s="3"/>
       <c r="U499" s="3"/>
@@ -7121,7 +7029,7 @@
       <c r="AA499" s="4"/>
       <c r="AB499" s="4"/>
     </row>
-    <row r="500" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="500" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q500"/>
       <c r="T500" s="3"/>
       <c r="U500" s="3"/>
@@ -7133,7 +7041,7 @@
       <c r="AA500" s="4"/>
       <c r="AB500" s="4"/>
     </row>
-    <row r="501" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="501" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q501"/>
       <c r="T501" s="3"/>
       <c r="U501" s="3"/>
@@ -7145,7 +7053,7 @@
       <c r="AA501" s="4"/>
       <c r="AB501" s="4"/>
     </row>
-    <row r="502" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="502" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q502"/>
       <c r="T502" s="3"/>
       <c r="U502" s="3"/>
@@ -7157,8 +7065,10 @@
       <c r="AA502" s="4"/>
       <c r="AB502" s="4"/>
     </row>
-    <row r="503" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="503" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P503" s="3"/>
       <c r="Q503"/>
+      <c r="R503" s="12"/>
       <c r="T503" s="3"/>
       <c r="U503" s="3"/>
       <c r="V503" s="3"/>
@@ -7169,7 +7079,7 @@
       <c r="AA503" s="4"/>
       <c r="AB503" s="4"/>
     </row>
-    <row r="504" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="504" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q504"/>
       <c r="T504" s="3"/>
       <c r="U504" s="3"/>
@@ -7181,7 +7091,7 @@
       <c r="AA504" s="4"/>
       <c r="AB504" s="4"/>
     </row>
-    <row r="505" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="505" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q505"/>
       <c r="T505" s="3"/>
       <c r="U505" s="3"/>
@@ -7193,7 +7103,7 @@
       <c r="AA505" s="4"/>
       <c r="AB505" s="4"/>
     </row>
-    <row r="506" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="506" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q506"/>
       <c r="T506" s="3"/>
       <c r="U506" s="3"/>
@@ -7205,7 +7115,7 @@
       <c r="AA506" s="4"/>
       <c r="AB506" s="4"/>
     </row>
-    <row r="507" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="507" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q507"/>
       <c r="T507" s="3"/>
       <c r="U507" s="3"/>
@@ -7217,9 +7127,8 @@
       <c r="AA507" s="4"/>
       <c r="AB507" s="4"/>
     </row>
-    <row r="508" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="508" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q508"/>
-      <c r="R508" s="12"/>
       <c r="T508" s="3"/>
       <c r="U508" s="3"/>
       <c r="V508" s="3"/>
@@ -7230,7 +7139,7 @@
       <c r="AA508" s="4"/>
       <c r="AB508" s="4"/>
     </row>
-    <row r="509" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="509" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q509"/>
       <c r="T509" s="3"/>
       <c r="U509" s="3"/>
@@ -7242,7 +7151,7 @@
       <c r="AA509" s="4"/>
       <c r="AB509" s="4"/>
     </row>
-    <row r="510" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="510" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q510"/>
       <c r="T510" s="3"/>
       <c r="U510" s="3"/>
@@ -7254,7 +7163,7 @@
       <c r="AA510" s="4"/>
       <c r="AB510" s="4"/>
     </row>
-    <row r="511" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="511" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q511"/>
       <c r="T511" s="3"/>
       <c r="U511" s="3"/>
@@ -7266,7 +7175,7 @@
       <c r="AA511" s="4"/>
       <c r="AB511" s="4"/>
     </row>
-    <row r="512" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="512" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q512"/>
       <c r="T512" s="3"/>
       <c r="U512" s="3"/>
@@ -7316,6 +7225,7 @@
     </row>
     <row r="516" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q516"/>
+      <c r="R516" s="12"/>
       <c r="T516" s="3"/>
       <c r="U516" s="3"/>
       <c r="V516" s="3"/>
@@ -7351,9 +7261,7 @@
       <c r="AB518" s="4"/>
     </row>
     <row r="519" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P519" s="3"/>
       <c r="Q519"/>
-      <c r="R519" s="12"/>
       <c r="T519" s="3"/>
       <c r="U519" s="3"/>
       <c r="V519" s="3"/>
@@ -7449,7 +7357,9 @@
       <c r="AB526" s="4"/>
     </row>
     <row r="527" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P527" s="3"/>
       <c r="Q527"/>
+      <c r="R527" s="12"/>
       <c r="T527" s="3"/>
       <c r="U527" s="3"/>
       <c r="V527" s="3"/>
@@ -7497,9 +7407,7 @@
       <c r="AB530" s="4"/>
     </row>
     <row r="531" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P531" s="3"/>
       <c r="Q531"/>
-      <c r="R531" s="12"/>
       <c r="T531" s="3"/>
       <c r="U531" s="3"/>
       <c r="V531" s="3"/>
@@ -7693,7 +7601,9 @@
       <c r="AB546" s="4"/>
     </row>
     <row r="547" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P547" s="3"/>
       <c r="Q547"/>
+      <c r="R547" s="12"/>
       <c r="T547" s="3"/>
       <c r="U547" s="3"/>
       <c r="V547" s="3"/>
@@ -7801,9 +7711,7 @@
       <c r="AB555" s="4"/>
     </row>
     <row r="556" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P556" s="3"/>
       <c r="Q556"/>
-      <c r="R556" s="12"/>
       <c r="T556" s="3"/>
       <c r="U556" s="3"/>
       <c r="V556" s="3"/>
@@ -7899,7 +7807,9 @@
       <c r="AB563" s="4"/>
     </row>
     <row r="564" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P564" s="3"/>
       <c r="Q564"/>
+      <c r="R564" s="12"/>
       <c r="T564" s="3"/>
       <c r="U564" s="3"/>
       <c r="V564" s="3"/>
@@ -7924,7 +7834,6 @@
     </row>
     <row r="566" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q566"/>
-      <c r="R566" s="12"/>
       <c r="T566" s="3"/>
       <c r="U566" s="3"/>
       <c r="V566" s="3"/>
@@ -7984,9 +7893,7 @@
       <c r="AB570" s="4"/>
     </row>
     <row r="571" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P571" s="3"/>
       <c r="Q571"/>
-      <c r="R571" s="12"/>
       <c r="T571" s="3"/>
       <c r="U571" s="3"/>
       <c r="V571" s="3"/>
@@ -8023,6 +7930,7 @@
     </row>
     <row r="574" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q574"/>
+      <c r="R574" s="12"/>
       <c r="T574" s="3"/>
       <c r="U574" s="3"/>
       <c r="V574" s="3"/>
@@ -8057,7 +7965,7 @@
       <c r="AA576" s="4"/>
       <c r="AB576" s="4"/>
     </row>
-    <row r="577" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="577" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q577"/>
       <c r="T577" s="3"/>
       <c r="U577" s="3"/>
@@ -8069,7 +7977,7 @@
       <c r="AA577" s="4"/>
       <c r="AB577" s="4"/>
     </row>
-    <row r="578" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="578" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q578"/>
       <c r="T578" s="3"/>
       <c r="U578" s="3"/>
@@ -8081,8 +7989,10 @@
       <c r="AA578" s="4"/>
       <c r="AB578" s="4"/>
     </row>
-    <row r="579" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="579" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P579" s="3"/>
       <c r="Q579"/>
+      <c r="R579" s="12"/>
       <c r="T579" s="3"/>
       <c r="U579" s="3"/>
       <c r="V579" s="3"/>
@@ -8093,7 +8003,7 @@
       <c r="AA579" s="4"/>
       <c r="AB579" s="4"/>
     </row>
-    <row r="580" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="580" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q580"/>
       <c r="T580" s="3"/>
       <c r="U580" s="3"/>
@@ -8105,7 +8015,7 @@
       <c r="AA580" s="4"/>
       <c r="AB580" s="4"/>
     </row>
-    <row r="581" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="581" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q581"/>
       <c r="T581" s="3"/>
       <c r="U581" s="3"/>
@@ -8117,7 +8027,7 @@
       <c r="AA581" s="4"/>
       <c r="AB581" s="4"/>
     </row>
-    <row r="582" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="582" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q582"/>
       <c r="T582" s="3"/>
       <c r="U582" s="3"/>
@@ -8129,7 +8039,7 @@
       <c r="AA582" s="4"/>
       <c r="AB582" s="4"/>
     </row>
-    <row r="583" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="583" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q583"/>
       <c r="T583" s="3"/>
       <c r="U583" s="3"/>
@@ -8141,7 +8051,7 @@
       <c r="AA583" s="4"/>
       <c r="AB583" s="4"/>
     </row>
-    <row r="584" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="584" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q584"/>
       <c r="T584" s="3"/>
       <c r="U584" s="3"/>
@@ -8153,7 +8063,7 @@
       <c r="AA584" s="4"/>
       <c r="AB584" s="4"/>
     </row>
-    <row r="585" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="585" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q585"/>
       <c r="T585" s="3"/>
       <c r="U585" s="3"/>
@@ -8165,7 +8075,7 @@
       <c r="AA585" s="4"/>
       <c r="AB585" s="4"/>
     </row>
-    <row r="586" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="586" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q586"/>
       <c r="T586" s="3"/>
       <c r="U586" s="3"/>
@@ -8177,7 +8087,7 @@
       <c r="AA586" s="4"/>
       <c r="AB586" s="4"/>
     </row>
-    <row r="587" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="587" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q587"/>
       <c r="T587" s="3"/>
       <c r="U587" s="3"/>
@@ -8189,7 +8099,7 @@
       <c r="AA587" s="4"/>
       <c r="AB587" s="4"/>
     </row>
-    <row r="588" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="588" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q588"/>
       <c r="T588" s="3"/>
       <c r="U588" s="3"/>
@@ -8201,7 +8111,7 @@
       <c r="AA588" s="4"/>
       <c r="AB588" s="4"/>
     </row>
-    <row r="589" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="589" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q589"/>
       <c r="T589" s="3"/>
       <c r="U589" s="3"/>
@@ -8213,7 +8123,7 @@
       <c r="AA589" s="4"/>
       <c r="AB589" s="4"/>
     </row>
-    <row r="590" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="590" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q590"/>
       <c r="T590" s="3"/>
       <c r="U590" s="3"/>
@@ -8225,7 +8135,7 @@
       <c r="AA590" s="4"/>
       <c r="AB590" s="4"/>
     </row>
-    <row r="591" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="591" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q591"/>
       <c r="T591" s="3"/>
       <c r="U591" s="3"/>
@@ -8237,7 +8147,7 @@
       <c r="AA591" s="4"/>
       <c r="AB591" s="4"/>
     </row>
-    <row r="592" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="592" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q592"/>
       <c r="T592" s="3"/>
       <c r="U592" s="3"/>
@@ -8322,36 +8232,100 @@
       <c r="AB598" s="4"/>
     </row>
     <row r="599" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T599" s="6"/>
-      <c r="U599" s="6"/>
+      <c r="Q599"/>
+      <c r="T599" s="3"/>
+      <c r="U599" s="3"/>
+      <c r="V599" s="3"/>
+      <c r="W599"/>
+      <c r="X599" s="10"/>
+      <c r="Y599"/>
+      <c r="Z599"/>
+      <c r="AA599" s="4"/>
+      <c r="AB599" s="4"/>
     </row>
     <row r="600" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T600" s="6"/>
-      <c r="U600" s="6"/>
+      <c r="Q600"/>
+      <c r="T600" s="3"/>
+      <c r="U600" s="3"/>
+      <c r="V600" s="3"/>
+      <c r="W600"/>
+      <c r="X600" s="10"/>
+      <c r="Y600"/>
+      <c r="Z600"/>
+      <c r="AA600" s="4"/>
+      <c r="AB600" s="4"/>
     </row>
     <row r="601" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T601" s="6"/>
-      <c r="U601" s="6"/>
+      <c r="Q601"/>
+      <c r="T601" s="3"/>
+      <c r="U601" s="3"/>
+      <c r="V601" s="3"/>
+      <c r="W601"/>
+      <c r="X601" s="10"/>
+      <c r="Y601"/>
+      <c r="Z601"/>
+      <c r="AA601" s="4"/>
+      <c r="AB601" s="4"/>
     </row>
     <row r="602" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T602" s="6"/>
-      <c r="U602" s="6"/>
+      <c r="Q602"/>
+      <c r="T602" s="3"/>
+      <c r="U602" s="3"/>
+      <c r="V602" s="3"/>
+      <c r="W602"/>
+      <c r="X602" s="10"/>
+      <c r="Y602"/>
+      <c r="Z602"/>
+      <c r="AA602" s="4"/>
+      <c r="AB602" s="4"/>
     </row>
     <row r="603" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T603" s="6"/>
-      <c r="U603" s="6"/>
+      <c r="Q603"/>
+      <c r="T603" s="3"/>
+      <c r="U603" s="3"/>
+      <c r="V603" s="3"/>
+      <c r="W603"/>
+      <c r="X603" s="10"/>
+      <c r="Y603"/>
+      <c r="Z603"/>
+      <c r="AA603" s="4"/>
+      <c r="AB603" s="4"/>
     </row>
     <row r="604" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T604" s="6"/>
-      <c r="U604" s="6"/>
+      <c r="Q604"/>
+      <c r="T604" s="3"/>
+      <c r="U604" s="3"/>
+      <c r="V604" s="3"/>
+      <c r="W604"/>
+      <c r="X604" s="10"/>
+      <c r="Y604"/>
+      <c r="Z604"/>
+      <c r="AA604" s="4"/>
+      <c r="AB604" s="4"/>
     </row>
     <row r="605" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T605" s="6"/>
-      <c r="U605" s="6"/>
+      <c r="Q605"/>
+      <c r="T605" s="3"/>
+      <c r="U605" s="3"/>
+      <c r="V605" s="3"/>
+      <c r="W605"/>
+      <c r="X605" s="10"/>
+      <c r="Y605"/>
+      <c r="Z605"/>
+      <c r="AA605" s="4"/>
+      <c r="AB605" s="4"/>
     </row>
     <row r="606" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T606" s="6"/>
-      <c r="U606" s="6"/>
+      <c r="Q606"/>
+      <c r="T606" s="3"/>
+      <c r="U606" s="3"/>
+      <c r="V606" s="3"/>
+      <c r="W606"/>
+      <c r="X606" s="10"/>
+      <c r="Y606"/>
+      <c r="Z606"/>
+      <c r="AA606" s="4"/>
+      <c r="AB606" s="4"/>
     </row>
     <row r="607" spans="17:28" x14ac:dyDescent="0.2">
       <c r="T607" s="6"/>
@@ -8440,6 +8414,38 @@
     <row r="628" spans="20:21" x14ac:dyDescent="0.2">
       <c r="T628" s="6"/>
       <c r="U628" s="6"/>
+    </row>
+    <row r="629" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T629" s="6"/>
+      <c r="U629" s="6"/>
+    </row>
+    <row r="630" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T630" s="6"/>
+      <c r="U630" s="6"/>
+    </row>
+    <row r="631" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T631" s="6"/>
+      <c r="U631" s="6"/>
+    </row>
+    <row r="632" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T632" s="6"/>
+      <c r="U632" s="6"/>
+    </row>
+    <row r="633" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T633" s="6"/>
+      <c r="U633" s="6"/>
+    </row>
+    <row r="634" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T634" s="6"/>
+      <c r="U634" s="6"/>
+    </row>
+    <row r="635" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T635" s="6"/>
+      <c r="U635" s="6"/>
+    </row>
+    <row r="636" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T636" s="6"/>
+      <c r="U636" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -8451,12 +8457,9 @@
     <hyperlink ref="F7" r:id="rId5"/>
     <hyperlink ref="F8" r:id="rId6"/>
     <hyperlink ref="F11" r:id="rId7"/>
-    <hyperlink ref="F12" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
get data from TextBox
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Customers.xlsx
+++ b/EDI/Web/wwwroot/Upload/Customers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>School Name</t>
   </si>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB628"/>
+  <dimension ref="A1:AB636"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1116,36 +1116,6 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="20">
-        <v>42299</v>
-      </c>
-      <c r="K12" s="21">
-        <v>200122609501901</v>
-      </c>
       <c r="Q12"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -1158,36 +1128,6 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="20">
-        <v>41876</v>
-      </c>
-      <c r="K13" s="21">
-        <v>200122604903901</v>
-      </c>
       <c r="Q13"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -1199,37 +1139,7 @@
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="20">
-        <v>42113</v>
-      </c>
-      <c r="K14" s="21">
-        <v>200122699902901</v>
-      </c>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Q14"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1399,7 +1309,6 @@
     </row>
     <row r="28" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q28"/>
-      <c r="R28" s="12"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -1496,6 +1405,7 @@
     </row>
     <row r="36" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q36"/>
+      <c r="R36" s="12"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -1687,9 +1597,7 @@
       <c r="AB51" s="4"/>
     </row>
     <row r="52" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P52" s="3"/>
       <c r="Q52"/>
-      <c r="R52" s="12"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -1785,7 +1693,9 @@
       <c r="AB59" s="4"/>
     </row>
     <row r="60" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P60" s="3"/>
       <c r="Q60"/>
+      <c r="R60" s="12"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="3"/>
@@ -1929,9 +1839,7 @@
       <c r="AB71" s="4"/>
     </row>
     <row r="72" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P72" s="3"/>
       <c r="Q72"/>
-      <c r="R72" s="12"/>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
@@ -2016,7 +1924,6 @@
     </row>
     <row r="79" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q79"/>
-      <c r="R79" s="12"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
@@ -2028,7 +1935,9 @@
       <c r="AB79" s="4"/>
     </row>
     <row r="80" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P80" s="3"/>
       <c r="Q80"/>
+      <c r="R80" s="12"/>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
@@ -2112,7 +2021,6 @@
       <c r="AB86" s="4"/>
     </row>
     <row r="87" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P87" s="3"/>
       <c r="Q87"/>
       <c r="R87" s="12"/>
       <c r="T87" s="3"/>
@@ -2210,7 +2118,9 @@
       <c r="AB94" s="4"/>
     </row>
     <row r="95" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P95" s="3"/>
       <c r="Q95"/>
+      <c r="R95" s="12"/>
       <c r="T95" s="3"/>
       <c r="U95" s="3"/>
       <c r="V95" s="3"/>
@@ -2233,7 +2143,7 @@
       <c r="AA96" s="4"/>
       <c r="AB96" s="4"/>
     </row>
-    <row r="97" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q97"/>
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
@@ -2245,7 +2155,7 @@
       <c r="AA97" s="4"/>
       <c r="AB97" s="4"/>
     </row>
-    <row r="98" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q98"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -2257,7 +2167,7 @@
       <c r="AA98" s="4"/>
       <c r="AB98" s="4"/>
     </row>
-    <row r="99" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q99"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -2269,9 +2179,8 @@
       <c r="AA99" s="4"/>
       <c r="AB99" s="4"/>
     </row>
-    <row r="100" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="100" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q100"/>
-      <c r="R100" s="12"/>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
       <c r="V100" s="3"/>
@@ -2282,7 +2191,7 @@
       <c r="AA100" s="4"/>
       <c r="AB100" s="4"/>
     </row>
-    <row r="101" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q101"/>
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
@@ -2294,7 +2203,7 @@
       <c r="AA101" s="4"/>
       <c r="AB101" s="4"/>
     </row>
-    <row r="102" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q102"/>
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
@@ -2306,7 +2215,7 @@
       <c r="AA102" s="4"/>
       <c r="AB102" s="4"/>
     </row>
-    <row r="103" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q103"/>
       <c r="T103" s="3"/>
       <c r="U103" s="3"/>
@@ -2318,7 +2227,7 @@
       <c r="AA103" s="4"/>
       <c r="AB103" s="4"/>
     </row>
-    <row r="104" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q104"/>
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
@@ -2330,7 +2239,7 @@
       <c r="AA104" s="4"/>
       <c r="AB104" s="4"/>
     </row>
-    <row r="105" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q105"/>
       <c r="T105" s="3"/>
       <c r="U105" s="3"/>
@@ -2342,7 +2251,7 @@
       <c r="AA105" s="4"/>
       <c r="AB105" s="4"/>
     </row>
-    <row r="106" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q106"/>
       <c r="T106" s="3"/>
       <c r="U106" s="3"/>
@@ -2354,7 +2263,7 @@
       <c r="AA106" s="4"/>
       <c r="AB106" s="4"/>
     </row>
-    <row r="107" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q107"/>
       <c r="T107" s="3"/>
       <c r="U107" s="3"/>
@@ -2366,8 +2275,7 @@
       <c r="AA107" s="4"/>
       <c r="AB107" s="4"/>
     </row>
-    <row r="108" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P108" s="3"/>
+    <row r="108" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q108"/>
       <c r="R108" s="12"/>
       <c r="T108" s="3"/>
@@ -2380,7 +2288,7 @@
       <c r="AA108" s="4"/>
       <c r="AB108" s="4"/>
     </row>
-    <row r="109" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q109"/>
       <c r="T109" s="3"/>
       <c r="U109" s="3"/>
@@ -2392,7 +2300,7 @@
       <c r="AA109" s="4"/>
       <c r="AB109" s="4"/>
     </row>
-    <row r="110" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q110"/>
       <c r="T110" s="3"/>
       <c r="U110" s="3"/>
@@ -2404,7 +2312,7 @@
       <c r="AA110" s="4"/>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q111"/>
       <c r="T111" s="3"/>
       <c r="U111" s="3"/>
@@ -2416,7 +2324,7 @@
       <c r="AA111" s="4"/>
       <c r="AB111" s="4"/>
     </row>
-    <row r="112" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q112"/>
       <c r="T112" s="3"/>
       <c r="U112" s="3"/>
@@ -2428,7 +2336,7 @@
       <c r="AA112" s="4"/>
       <c r="AB112" s="4"/>
     </row>
-    <row r="113" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q113"/>
       <c r="T113" s="3"/>
       <c r="U113" s="3"/>
@@ -2440,7 +2348,7 @@
       <c r="AA113" s="4"/>
       <c r="AB113" s="4"/>
     </row>
-    <row r="114" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q114"/>
       <c r="T114" s="3"/>
       <c r="U114" s="3"/>
@@ -2452,7 +2360,7 @@
       <c r="AA114" s="4"/>
       <c r="AB114" s="4"/>
     </row>
-    <row r="115" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q115"/>
       <c r="T115" s="3"/>
       <c r="U115" s="3"/>
@@ -2464,8 +2372,10 @@
       <c r="AA115" s="4"/>
       <c r="AB115" s="4"/>
     </row>
-    <row r="116" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P116" s="3"/>
       <c r="Q116"/>
+      <c r="R116" s="12"/>
       <c r="T116" s="3"/>
       <c r="U116" s="3"/>
       <c r="V116" s="3"/>
@@ -2476,7 +2386,7 @@
       <c r="AA116" s="4"/>
       <c r="AB116" s="4"/>
     </row>
-    <row r="117" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q117"/>
       <c r="T117" s="3"/>
       <c r="U117" s="3"/>
@@ -2488,7 +2398,7 @@
       <c r="AA117" s="4"/>
       <c r="AB117" s="4"/>
     </row>
-    <row r="118" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q118"/>
       <c r="T118" s="3"/>
       <c r="U118" s="3"/>
@@ -2500,7 +2410,7 @@
       <c r="AA118" s="4"/>
       <c r="AB118" s="4"/>
     </row>
-    <row r="119" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q119"/>
       <c r="T119" s="3"/>
       <c r="U119" s="3"/>
@@ -2512,7 +2422,7 @@
       <c r="AA119" s="4"/>
       <c r="AB119" s="4"/>
     </row>
-    <row r="120" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q120"/>
       <c r="T120" s="3"/>
       <c r="U120" s="3"/>
@@ -2524,9 +2434,8 @@
       <c r="AA120" s="4"/>
       <c r="AB120" s="4"/>
     </row>
-    <row r="121" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q121"/>
-      <c r="R121" s="12"/>
       <c r="T121" s="3"/>
       <c r="U121" s="3"/>
       <c r="V121" s="3"/>
@@ -2537,7 +2446,7 @@
       <c r="AA121" s="4"/>
       <c r="AB121" s="4"/>
     </row>
-    <row r="122" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q122"/>
       <c r="T122" s="3"/>
       <c r="U122" s="3"/>
@@ -2549,7 +2458,7 @@
       <c r="AA122" s="4"/>
       <c r="AB122" s="4"/>
     </row>
-    <row r="123" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q123"/>
       <c r="T123" s="3"/>
       <c r="U123" s="3"/>
@@ -2561,7 +2470,7 @@
       <c r="AA123" s="4"/>
       <c r="AB123" s="4"/>
     </row>
-    <row r="124" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q124"/>
       <c r="T124" s="3"/>
       <c r="U124" s="3"/>
@@ -2573,7 +2482,7 @@
       <c r="AA124" s="4"/>
       <c r="AB124" s="4"/>
     </row>
-    <row r="125" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q125"/>
       <c r="T125" s="3"/>
       <c r="U125" s="3"/>
@@ -2585,7 +2494,7 @@
       <c r="AA125" s="4"/>
       <c r="AB125" s="4"/>
     </row>
-    <row r="126" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q126"/>
       <c r="T126" s="3"/>
       <c r="U126" s="3"/>
@@ -2597,7 +2506,7 @@
       <c r="AA126" s="4"/>
       <c r="AB126" s="4"/>
     </row>
-    <row r="127" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q127"/>
       <c r="T127" s="3"/>
       <c r="U127" s="3"/>
@@ -2609,7 +2518,7 @@
       <c r="AA127" s="4"/>
       <c r="AB127" s="4"/>
     </row>
-    <row r="128" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q128"/>
       <c r="T128" s="3"/>
       <c r="U128" s="3"/>
@@ -2623,6 +2532,7 @@
     </row>
     <row r="129" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q129"/>
+      <c r="R129" s="12"/>
       <c r="T129" s="3"/>
       <c r="U129" s="3"/>
       <c r="V129" s="3"/>
@@ -2694,9 +2604,7 @@
       <c r="AB134" s="4"/>
     </row>
     <row r="135" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P135" s="3"/>
       <c r="Q135"/>
-      <c r="R135" s="12"/>
       <c r="T135" s="3"/>
       <c r="U135" s="3"/>
       <c r="V135" s="3"/>
@@ -2792,7 +2700,9 @@
       <c r="AB142" s="4"/>
     </row>
     <row r="143" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P143" s="3"/>
       <c r="Q143"/>
+      <c r="R143" s="12"/>
       <c r="T143" s="3"/>
       <c r="U143" s="3"/>
       <c r="V143" s="3"/>
@@ -2840,9 +2750,7 @@
       <c r="AB146" s="4"/>
     </row>
     <row r="147" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P147" s="3"/>
       <c r="Q147"/>
-      <c r="R147" s="12"/>
       <c r="T147" s="3"/>
       <c r="U147" s="3"/>
       <c r="V147" s="3"/>
@@ -2938,7 +2846,9 @@
       <c r="AB154" s="4"/>
     </row>
     <row r="155" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P155" s="3"/>
       <c r="Q155"/>
+      <c r="R155" s="12"/>
       <c r="T155" s="3"/>
       <c r="U155" s="3"/>
       <c r="V155" s="3"/>
@@ -3009,9 +2919,8 @@
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
     </row>
-    <row r="161" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="161" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q161"/>
-      <c r="R161" s="12"/>
       <c r="T161" s="3"/>
       <c r="U161" s="3"/>
       <c r="V161" s="3"/>
@@ -3022,7 +2931,7 @@
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
     </row>
-    <row r="162" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="162" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q162"/>
       <c r="T162" s="3"/>
       <c r="U162" s="3"/>
@@ -3034,7 +2943,7 @@
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
     </row>
-    <row r="163" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="163" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q163"/>
       <c r="T163" s="3"/>
       <c r="U163" s="3"/>
@@ -3046,7 +2955,7 @@
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
     </row>
-    <row r="164" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="164" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q164"/>
       <c r="T164" s="3"/>
       <c r="U164" s="3"/>
@@ -3058,7 +2967,7 @@
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
     </row>
-    <row r="165" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="165" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q165"/>
       <c r="T165" s="3"/>
       <c r="U165" s="3"/>
@@ -3070,7 +2979,7 @@
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
     </row>
-    <row r="166" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="166" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q166"/>
       <c r="T166" s="3"/>
       <c r="U166" s="3"/>
@@ -3082,7 +2991,7 @@
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
     </row>
-    <row r="167" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="167" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q167"/>
       <c r="T167" s="3"/>
       <c r="U167" s="3"/>
@@ -3094,7 +3003,7 @@
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
     </row>
-    <row r="168" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="168" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q168"/>
       <c r="T168" s="3"/>
       <c r="U168" s="3"/>
@@ -3106,8 +3015,9 @@
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
     </row>
-    <row r="169" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="169" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q169"/>
+      <c r="R169" s="12"/>
       <c r="T169" s="3"/>
       <c r="U169" s="3"/>
       <c r="V169" s="3"/>
@@ -3118,7 +3028,7 @@
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
     </row>
-    <row r="170" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="170" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q170"/>
       <c r="T170" s="3"/>
       <c r="U170" s="3"/>
@@ -3130,7 +3040,7 @@
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
     </row>
-    <row r="171" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="171" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q171"/>
       <c r="T171" s="3"/>
       <c r="U171" s="3"/>
@@ -3142,7 +3052,7 @@
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
     </row>
-    <row r="172" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="172" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q172"/>
       <c r="T172" s="3"/>
       <c r="U172" s="3"/>
@@ -3154,10 +3064,8 @@
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
     </row>
-    <row r="173" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P173" s="3"/>
+    <row r="173" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q173"/>
-      <c r="R173" s="12"/>
       <c r="T173" s="3"/>
       <c r="U173" s="3"/>
       <c r="V173" s="3"/>
@@ -3168,7 +3076,7 @@
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
     </row>
-    <row r="174" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="174" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q174"/>
       <c r="T174" s="3"/>
       <c r="U174" s="3"/>
@@ -3180,7 +3088,7 @@
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
     </row>
-    <row r="175" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="175" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q175"/>
       <c r="T175" s="3"/>
       <c r="U175" s="3"/>
@@ -3192,7 +3100,7 @@
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
     </row>
-    <row r="176" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="176" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q176"/>
       <c r="T176" s="3"/>
       <c r="U176" s="3"/>
@@ -3253,7 +3161,9 @@
       <c r="AB180" s="4"/>
     </row>
     <row r="181" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P181" s="3"/>
       <c r="Q181"/>
+      <c r="R181" s="12"/>
       <c r="T181" s="3"/>
       <c r="U181" s="3"/>
       <c r="V181" s="3"/>
@@ -3313,9 +3223,7 @@
       <c r="AB185" s="4"/>
     </row>
     <row r="186" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P186" s="3"/>
       <c r="Q186"/>
-      <c r="R186" s="12"/>
       <c r="T186" s="3"/>
       <c r="U186" s="3"/>
       <c r="V186" s="3"/>
@@ -3398,7 +3306,7 @@
       <c r="AA192" s="4"/>
       <c r="AB192" s="4"/>
     </row>
-    <row r="193" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="193" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q193"/>
       <c r="T193" s="3"/>
       <c r="U193" s="3"/>
@@ -3410,8 +3318,10 @@
       <c r="AA193" s="4"/>
       <c r="AB193" s="4"/>
     </row>
-    <row r="194" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="194" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P194" s="3"/>
       <c r="Q194"/>
+      <c r="R194" s="12"/>
       <c r="T194" s="3"/>
       <c r="U194" s="3"/>
       <c r="V194" s="3"/>
@@ -3422,9 +3332,8 @@
       <c r="AA194" s="4"/>
       <c r="AB194" s="4"/>
     </row>
-    <row r="195" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="195" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q195"/>
-      <c r="R195" s="12"/>
       <c r="T195" s="3"/>
       <c r="U195" s="3"/>
       <c r="V195" s="3"/>
@@ -3435,7 +3344,7 @@
       <c r="AA195" s="4"/>
       <c r="AB195" s="4"/>
     </row>
-    <row r="196" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="196" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q196"/>
       <c r="T196" s="3"/>
       <c r="U196" s="3"/>
@@ -3447,7 +3356,7 @@
       <c r="AA196" s="4"/>
       <c r="AB196" s="4"/>
     </row>
-    <row r="197" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="197" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q197"/>
       <c r="T197" s="3"/>
       <c r="U197" s="3"/>
@@ -3459,7 +3368,7 @@
       <c r="AA197" s="4"/>
       <c r="AB197" s="4"/>
     </row>
-    <row r="198" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="198" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q198"/>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
@@ -3471,7 +3380,7 @@
       <c r="AA198" s="4"/>
       <c r="AB198" s="4"/>
     </row>
-    <row r="199" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="199" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q199"/>
       <c r="T199" s="3"/>
       <c r="U199" s="3"/>
@@ -3483,7 +3392,7 @@
       <c r="AA199" s="4"/>
       <c r="AB199" s="4"/>
     </row>
-    <row r="200" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="200" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q200"/>
       <c r="T200" s="3"/>
       <c r="U200" s="3"/>
@@ -3495,7 +3404,7 @@
       <c r="AA200" s="4"/>
       <c r="AB200" s="4"/>
     </row>
-    <row r="201" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="201" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q201"/>
       <c r="T201" s="3"/>
       <c r="U201" s="3"/>
@@ -3507,7 +3416,7 @@
       <c r="AA201" s="4"/>
       <c r="AB201" s="4"/>
     </row>
-    <row r="202" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="202" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q202"/>
       <c r="T202" s="3"/>
       <c r="U202" s="3"/>
@@ -3519,8 +3428,9 @@
       <c r="AA202" s="4"/>
       <c r="AB202" s="4"/>
     </row>
-    <row r="203" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="203" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q203"/>
+      <c r="R203" s="12"/>
       <c r="T203" s="3"/>
       <c r="U203" s="3"/>
       <c r="V203" s="3"/>
@@ -3531,7 +3441,7 @@
       <c r="AA203" s="4"/>
       <c r="AB203" s="4"/>
     </row>
-    <row r="204" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="204" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q204"/>
       <c r="T204" s="3"/>
       <c r="U204" s="3"/>
@@ -3543,7 +3453,7 @@
       <c r="AA204" s="4"/>
       <c r="AB204" s="4"/>
     </row>
-    <row r="205" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="205" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q205"/>
       <c r="T205" s="3"/>
       <c r="U205" s="3"/>
@@ -3555,7 +3465,7 @@
       <c r="AA205" s="4"/>
       <c r="AB205" s="4"/>
     </row>
-    <row r="206" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="206" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q206"/>
       <c r="T206" s="3"/>
       <c r="U206" s="3"/>
@@ -3567,7 +3477,7 @@
       <c r="AA206" s="4"/>
       <c r="AB206" s="4"/>
     </row>
-    <row r="207" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="207" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q207"/>
       <c r="T207" s="3"/>
       <c r="U207" s="3"/>
@@ -3579,7 +3489,7 @@
       <c r="AA207" s="4"/>
       <c r="AB207" s="4"/>
     </row>
-    <row r="208" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="208" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q208"/>
       <c r="T208" s="3"/>
       <c r="U208" s="3"/>
@@ -3591,7 +3501,7 @@
       <c r="AA208" s="4"/>
       <c r="AB208" s="4"/>
     </row>
-    <row r="209" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="209" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q209"/>
       <c r="T209" s="3"/>
       <c r="U209" s="3"/>
@@ -3603,7 +3513,7 @@
       <c r="AA209" s="4"/>
       <c r="AB209" s="4"/>
     </row>
-    <row r="210" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="210" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q210"/>
       <c r="T210" s="3"/>
       <c r="U210" s="3"/>
@@ -3615,7 +3525,7 @@
       <c r="AA210" s="4"/>
       <c r="AB210" s="4"/>
     </row>
-    <row r="211" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="211" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q211"/>
       <c r="T211" s="3"/>
       <c r="U211" s="3"/>
@@ -3627,7 +3537,7 @@
       <c r="AA211" s="4"/>
       <c r="AB211" s="4"/>
     </row>
-    <row r="212" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="212" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q212"/>
       <c r="T212" s="3"/>
       <c r="U212" s="3"/>
@@ -3639,7 +3549,7 @@
       <c r="AA212" s="4"/>
       <c r="AB212" s="4"/>
     </row>
-    <row r="213" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="213" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q213"/>
       <c r="T213" s="3"/>
       <c r="U213" s="3"/>
@@ -3651,7 +3561,7 @@
       <c r="AA213" s="4"/>
       <c r="AB213" s="4"/>
     </row>
-    <row r="214" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="214" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q214"/>
       <c r="T214" s="3"/>
       <c r="U214" s="3"/>
@@ -3663,7 +3573,7 @@
       <c r="AA214" s="4"/>
       <c r="AB214" s="4"/>
     </row>
-    <row r="215" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="215" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q215"/>
       <c r="T215" s="3"/>
       <c r="U215" s="3"/>
@@ -3675,7 +3585,7 @@
       <c r="AA215" s="4"/>
       <c r="AB215" s="4"/>
     </row>
-    <row r="216" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="216" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q216"/>
       <c r="T216" s="3"/>
       <c r="U216" s="3"/>
@@ -3687,10 +3597,8 @@
       <c r="AA216" s="4"/>
       <c r="AB216" s="4"/>
     </row>
-    <row r="217" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P217" s="3"/>
+    <row r="217" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q217"/>
-      <c r="R217" s="12"/>
       <c r="T217" s="3"/>
       <c r="U217" s="3"/>
       <c r="V217" s="3"/>
@@ -3701,7 +3609,7 @@
       <c r="AA217" s="4"/>
       <c r="AB217" s="4"/>
     </row>
-    <row r="218" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="218" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q218"/>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
@@ -3713,7 +3621,7 @@
       <c r="AA218" s="4"/>
       <c r="AB218" s="4"/>
     </row>
-    <row r="219" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="219" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q219"/>
       <c r="T219" s="3"/>
       <c r="U219" s="3"/>
@@ -3725,7 +3633,7 @@
       <c r="AA219" s="4"/>
       <c r="AB219" s="4"/>
     </row>
-    <row r="220" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="220" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q220"/>
       <c r="T220" s="3"/>
       <c r="U220" s="3"/>
@@ -3737,7 +3645,7 @@
       <c r="AA220" s="4"/>
       <c r="AB220" s="4"/>
     </row>
-    <row r="221" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="221" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q221"/>
       <c r="T221" s="3"/>
       <c r="U221" s="3"/>
@@ -3749,7 +3657,7 @@
       <c r="AA221" s="4"/>
       <c r="AB221" s="4"/>
     </row>
-    <row r="222" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="222" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q222"/>
       <c r="T222" s="3"/>
       <c r="U222" s="3"/>
@@ -3761,7 +3669,7 @@
       <c r="AA222" s="4"/>
       <c r="AB222" s="4"/>
     </row>
-    <row r="223" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="223" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q223"/>
       <c r="T223" s="3"/>
       <c r="U223" s="3"/>
@@ -3773,7 +3681,7 @@
       <c r="AA223" s="4"/>
       <c r="AB223" s="4"/>
     </row>
-    <row r="224" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="224" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q224"/>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
@@ -3786,7 +3694,9 @@
       <c r="AB224" s="4"/>
     </row>
     <row r="225" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P225" s="3"/>
       <c r="Q225"/>
+      <c r="R225" s="12"/>
       <c r="T225" s="3"/>
       <c r="U225" s="3"/>
       <c r="V225" s="3"/>
@@ -3906,9 +3816,7 @@
       <c r="AB234" s="4"/>
     </row>
     <row r="235" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P235" s="3"/>
       <c r="Q235"/>
-      <c r="R235" s="12"/>
       <c r="T235" s="3"/>
       <c r="U235" s="3"/>
       <c r="V235" s="3"/>
@@ -3993,7 +3901,6 @@
     </row>
     <row r="242" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q242"/>
-      <c r="R242" s="12"/>
       <c r="T242" s="3"/>
       <c r="U242" s="3"/>
       <c r="V242" s="3"/>
@@ -4005,7 +3912,9 @@
       <c r="AB242" s="4"/>
     </row>
     <row r="243" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P243" s="3"/>
       <c r="Q243"/>
+      <c r="R243" s="12"/>
       <c r="T243" s="3"/>
       <c r="U243" s="3"/>
       <c r="V243" s="3"/>
@@ -4090,6 +3999,7 @@
     </row>
     <row r="250" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q250"/>
+      <c r="R250" s="12"/>
       <c r="T250" s="3"/>
       <c r="U250" s="3"/>
       <c r="V250" s="3"/>
@@ -4113,9 +4023,7 @@
       <c r="AB251" s="4"/>
     </row>
     <row r="252" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P252" s="3"/>
       <c r="Q252"/>
-      <c r="R252" s="12"/>
       <c r="T252" s="3"/>
       <c r="U252" s="3"/>
       <c r="V252" s="3"/>
@@ -4211,7 +4119,9 @@
       <c r="AB259" s="4"/>
     </row>
     <row r="260" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P260" s="3"/>
       <c r="Q260"/>
+      <c r="R260" s="12"/>
       <c r="T260" s="3"/>
       <c r="U260" s="3"/>
       <c r="V260" s="3"/>
@@ -4223,9 +4133,7 @@
       <c r="AB260" s="4"/>
     </row>
     <row r="261" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P261" s="3"/>
       <c r="Q261"/>
-      <c r="R261" s="12"/>
       <c r="T261" s="3"/>
       <c r="U261" s="3"/>
       <c r="V261" s="3"/>
@@ -4321,7 +4229,9 @@
       <c r="AB268" s="4"/>
     </row>
     <row r="269" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P269" s="3"/>
       <c r="Q269"/>
+      <c r="R269" s="12"/>
       <c r="T269" s="3"/>
       <c r="U269" s="3"/>
       <c r="V269" s="3"/>
@@ -4334,7 +4244,6 @@
     </row>
     <row r="270" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q270"/>
-      <c r="R270" s="12"/>
       <c r="T270" s="3"/>
       <c r="U270" s="3"/>
       <c r="V270" s="3"/>
@@ -4369,7 +4278,7 @@
       <c r="AA272" s="4"/>
       <c r="AB272" s="4"/>
     </row>
-    <row r="273" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="273" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q273"/>
       <c r="T273" s="3"/>
       <c r="U273" s="3"/>
@@ -4381,7 +4290,7 @@
       <c r="AA273" s="4"/>
       <c r="AB273" s="4"/>
     </row>
-    <row r="274" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="274" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q274"/>
       <c r="T274" s="3"/>
       <c r="U274" s="3"/>
@@ -4393,7 +4302,7 @@
       <c r="AA274" s="4"/>
       <c r="AB274" s="4"/>
     </row>
-    <row r="275" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="275" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q275"/>
       <c r="T275" s="3"/>
       <c r="U275" s="3"/>
@@ -4405,7 +4314,7 @@
       <c r="AA275" s="4"/>
       <c r="AB275" s="4"/>
     </row>
-    <row r="276" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="276" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q276"/>
       <c r="T276" s="3"/>
       <c r="U276" s="3"/>
@@ -4417,7 +4326,7 @@
       <c r="AA276" s="4"/>
       <c r="AB276" s="4"/>
     </row>
-    <row r="277" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="277" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q277"/>
       <c r="T277" s="3"/>
       <c r="U277" s="3"/>
@@ -4429,8 +4338,9 @@
       <c r="AA277" s="4"/>
       <c r="AB277" s="4"/>
     </row>
-    <row r="278" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="278" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q278"/>
+      <c r="R278" s="12"/>
       <c r="T278" s="3"/>
       <c r="U278" s="3"/>
       <c r="V278" s="3"/>
@@ -4441,7 +4351,7 @@
       <c r="AA278" s="4"/>
       <c r="AB278" s="4"/>
     </row>
-    <row r="279" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="279" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q279"/>
       <c r="T279" s="3"/>
       <c r="U279" s="3"/>
@@ -4453,7 +4363,7 @@
       <c r="AA279" s="4"/>
       <c r="AB279" s="4"/>
     </row>
-    <row r="280" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="280" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q280"/>
       <c r="T280" s="3"/>
       <c r="U280" s="3"/>
@@ -4465,10 +4375,8 @@
       <c r="AA280" s="4"/>
       <c r="AB280" s="4"/>
     </row>
-    <row r="281" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P281" s="3"/>
+    <row r="281" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q281"/>
-      <c r="R281" s="12"/>
       <c r="T281" s="3"/>
       <c r="U281" s="3"/>
       <c r="V281" s="3"/>
@@ -4479,7 +4387,7 @@
       <c r="AA281" s="4"/>
       <c r="AB281" s="4"/>
     </row>
-    <row r="282" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="282" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q282"/>
       <c r="T282" s="3"/>
       <c r="U282" s="3"/>
@@ -4491,7 +4399,7 @@
       <c r="AA282" s="4"/>
       <c r="AB282" s="4"/>
     </row>
-    <row r="283" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="283" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q283"/>
       <c r="T283" s="3"/>
       <c r="U283" s="3"/>
@@ -4503,7 +4411,7 @@
       <c r="AA283" s="4"/>
       <c r="AB283" s="4"/>
     </row>
-    <row r="284" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="284" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q284"/>
       <c r="T284" s="3"/>
       <c r="U284" s="3"/>
@@ -4515,7 +4423,7 @@
       <c r="AA284" s="4"/>
       <c r="AB284" s="4"/>
     </row>
-    <row r="285" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="285" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q285"/>
       <c r="T285" s="3"/>
       <c r="U285" s="3"/>
@@ -4527,7 +4435,7 @@
       <c r="AA285" s="4"/>
       <c r="AB285" s="4"/>
     </row>
-    <row r="286" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="286" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q286"/>
       <c r="T286" s="3"/>
       <c r="U286" s="3"/>
@@ -4539,7 +4447,7 @@
       <c r="AA286" s="4"/>
       <c r="AB286" s="4"/>
     </row>
-    <row r="287" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="287" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q287"/>
       <c r="T287" s="3"/>
       <c r="U287" s="3"/>
@@ -4551,7 +4459,7 @@
       <c r="AA287" s="4"/>
       <c r="AB287" s="4"/>
     </row>
-    <row r="288" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="288" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q288"/>
       <c r="T288" s="3"/>
       <c r="U288" s="3"/>
@@ -4564,7 +4472,9 @@
       <c r="AB288" s="4"/>
     </row>
     <row r="289" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P289" s="3"/>
       <c r="Q289"/>
+      <c r="R289" s="12"/>
       <c r="T289" s="3"/>
       <c r="U289" s="3"/>
       <c r="V289" s="3"/>
@@ -4708,9 +4618,7 @@
       <c r="AB300" s="4"/>
     </row>
     <row r="301" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P301" s="3"/>
       <c r="Q301"/>
-      <c r="R301" s="12"/>
       <c r="T301" s="3"/>
       <c r="U301" s="3"/>
       <c r="V301" s="3"/>
@@ -4806,7 +4714,9 @@
       <c r="AB308" s="4"/>
     </row>
     <row r="309" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P309" s="3"/>
       <c r="Q309"/>
+      <c r="R309" s="12"/>
       <c r="T309" s="3"/>
       <c r="U309" s="3"/>
       <c r="V309" s="3"/>
@@ -4830,9 +4740,7 @@
       <c r="AB310" s="4"/>
     </row>
     <row r="311" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P311" s="3"/>
       <c r="Q311"/>
-      <c r="R311" s="12"/>
       <c r="T311" s="3"/>
       <c r="U311" s="3"/>
       <c r="V311" s="3"/>
@@ -4928,7 +4836,9 @@
       <c r="AB318" s="4"/>
     </row>
     <row r="319" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P319" s="3"/>
       <c r="Q319"/>
+      <c r="R319" s="12"/>
       <c r="T319" s="3"/>
       <c r="U319" s="3"/>
       <c r="V319" s="3"/>
@@ -5061,7 +4971,6 @@
     </row>
     <row r="330" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q330"/>
-      <c r="R330" s="12"/>
       <c r="T330" s="3"/>
       <c r="U330" s="3"/>
       <c r="V330" s="3"/>
@@ -5144,9 +5053,8 @@
       <c r="AA336" s="4"/>
       <c r="AB336" s="4"/>
     </row>
-    <row r="337" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="337" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q337"/>
-      <c r="R337" s="12"/>
       <c r="T337" s="3"/>
       <c r="U337" s="3"/>
       <c r="V337" s="3"/>
@@ -5157,8 +5065,9 @@
       <c r="AA337" s="4"/>
       <c r="AB337" s="4"/>
     </row>
-    <row r="338" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="338" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q338"/>
+      <c r="R338" s="12"/>
       <c r="T338" s="3"/>
       <c r="U338" s="3"/>
       <c r="V338" s="3"/>
@@ -5169,7 +5078,7 @@
       <c r="AA338" s="4"/>
       <c r="AB338" s="4"/>
     </row>
-    <row r="339" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="339" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q339"/>
       <c r="T339" s="3"/>
       <c r="U339" s="3"/>
@@ -5181,7 +5090,7 @@
       <c r="AA339" s="4"/>
       <c r="AB339" s="4"/>
     </row>
-    <row r="340" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="340" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q340"/>
       <c r="T340" s="3"/>
       <c r="U340" s="3"/>
@@ -5193,7 +5102,7 @@
       <c r="AA340" s="4"/>
       <c r="AB340" s="4"/>
     </row>
-    <row r="341" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="341" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q341"/>
       <c r="T341" s="3"/>
       <c r="U341" s="3"/>
@@ -5205,7 +5114,7 @@
       <c r="AA341" s="4"/>
       <c r="AB341" s="4"/>
     </row>
-    <row r="342" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="342" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q342"/>
       <c r="T342" s="3"/>
       <c r="U342" s="3"/>
@@ -5217,7 +5126,7 @@
       <c r="AA342" s="4"/>
       <c r="AB342" s="4"/>
     </row>
-    <row r="343" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="343" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q343"/>
       <c r="T343" s="3"/>
       <c r="U343" s="3"/>
@@ -5229,7 +5138,7 @@
       <c r="AA343" s="4"/>
       <c r="AB343" s="4"/>
     </row>
-    <row r="344" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="344" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q344"/>
       <c r="T344" s="3"/>
       <c r="U344" s="3"/>
@@ -5241,8 +5150,7 @@
       <c r="AA344" s="4"/>
       <c r="AB344" s="4"/>
     </row>
-    <row r="345" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P345" s="3"/>
+    <row r="345" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q345"/>
       <c r="R345" s="12"/>
       <c r="T345" s="3"/>
@@ -5255,7 +5163,7 @@
       <c r="AA345" s="4"/>
       <c r="AB345" s="4"/>
     </row>
-    <row r="346" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="346" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q346"/>
       <c r="T346" s="3"/>
       <c r="U346" s="3"/>
@@ -5267,7 +5175,7 @@
       <c r="AA346" s="4"/>
       <c r="AB346" s="4"/>
     </row>
-    <row r="347" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="347" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q347"/>
       <c r="T347" s="3"/>
       <c r="U347" s="3"/>
@@ -5279,7 +5187,7 @@
       <c r="AA347" s="4"/>
       <c r="AB347" s="4"/>
     </row>
-    <row r="348" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="348" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q348"/>
       <c r="T348" s="3"/>
       <c r="U348" s="3"/>
@@ -5291,7 +5199,7 @@
       <c r="AA348" s="4"/>
       <c r="AB348" s="4"/>
     </row>
-    <row r="349" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="349" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q349"/>
       <c r="T349" s="3"/>
       <c r="U349" s="3"/>
@@ -5303,7 +5211,7 @@
       <c r="AA349" s="4"/>
       <c r="AB349" s="4"/>
     </row>
-    <row r="350" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="350" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q350"/>
       <c r="T350" s="3"/>
       <c r="U350" s="3"/>
@@ -5315,9 +5223,8 @@
       <c r="AA350" s="4"/>
       <c r="AB350" s="4"/>
     </row>
-    <row r="351" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="351" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q351"/>
-      <c r="R351" s="12"/>
       <c r="T351" s="3"/>
       <c r="U351" s="3"/>
       <c r="V351" s="3"/>
@@ -5328,7 +5235,7 @@
       <c r="AA351" s="4"/>
       <c r="AB351" s="4"/>
     </row>
-    <row r="352" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="352" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q352"/>
       <c r="T352" s="3"/>
       <c r="U352" s="3"/>
@@ -5341,7 +5248,9 @@
       <c r="AB352" s="4"/>
     </row>
     <row r="353" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P353" s="3"/>
       <c r="Q353"/>
+      <c r="R353" s="12"/>
       <c r="T353" s="3"/>
       <c r="U353" s="3"/>
       <c r="V353" s="3"/>
@@ -5377,9 +5286,7 @@
       <c r="AB355" s="4"/>
     </row>
     <row r="356" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P356" s="3"/>
       <c r="Q356"/>
-      <c r="R356" s="12"/>
       <c r="T356" s="3"/>
       <c r="U356" s="3"/>
       <c r="V356" s="3"/>
@@ -5416,6 +5323,7 @@
     </row>
     <row r="359" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q359"/>
+      <c r="R359" s="12"/>
       <c r="T359" s="3"/>
       <c r="U359" s="3"/>
       <c r="V359" s="3"/>
@@ -5475,7 +5383,9 @@
       <c r="AB363" s="4"/>
     </row>
     <row r="364" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P364" s="3"/>
       <c r="Q364"/>
+      <c r="R364" s="12"/>
       <c r="T364" s="3"/>
       <c r="U364" s="3"/>
       <c r="V364" s="3"/>
@@ -5499,9 +5409,7 @@
       <c r="AB365" s="4"/>
     </row>
     <row r="366" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P366" s="3"/>
       <c r="Q366"/>
-      <c r="R366" s="12"/>
       <c r="T366" s="3"/>
       <c r="U366" s="3"/>
       <c r="V366" s="3"/>
@@ -5536,7 +5444,7 @@
       <c r="AA368" s="4"/>
       <c r="AB368" s="4"/>
     </row>
-    <row r="369" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="369" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q369"/>
       <c r="T369" s="3"/>
       <c r="U369" s="3"/>
@@ -5548,7 +5456,7 @@
       <c r="AA369" s="4"/>
       <c r="AB369" s="4"/>
     </row>
-    <row r="370" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="370" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q370"/>
       <c r="T370" s="3"/>
       <c r="U370" s="3"/>
@@ -5560,7 +5468,7 @@
       <c r="AA370" s="4"/>
       <c r="AB370" s="4"/>
     </row>
-    <row r="371" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="371" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q371"/>
       <c r="T371" s="3"/>
       <c r="U371" s="3"/>
@@ -5572,7 +5480,7 @@
       <c r="AA371" s="4"/>
       <c r="AB371" s="4"/>
     </row>
-    <row r="372" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="372" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q372"/>
       <c r="T372" s="3"/>
       <c r="U372" s="3"/>
@@ -5584,7 +5492,7 @@
       <c r="AA372" s="4"/>
       <c r="AB372" s="4"/>
     </row>
-    <row r="373" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="373" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q373"/>
       <c r="T373" s="3"/>
       <c r="U373" s="3"/>
@@ -5596,8 +5504,10 @@
       <c r="AA373" s="4"/>
       <c r="AB373" s="4"/>
     </row>
-    <row r="374" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="374" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P374" s="3"/>
       <c r="Q374"/>
+      <c r="R374" s="12"/>
       <c r="T374" s="3"/>
       <c r="U374" s="3"/>
       <c r="V374" s="3"/>
@@ -5608,7 +5518,7 @@
       <c r="AA374" s="4"/>
       <c r="AB374" s="4"/>
     </row>
-    <row r="375" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="375" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q375"/>
       <c r="T375" s="3"/>
       <c r="U375" s="3"/>
@@ -5620,7 +5530,7 @@
       <c r="AA375" s="4"/>
       <c r="AB375" s="4"/>
     </row>
-    <row r="376" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="376" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q376"/>
       <c r="T376" s="3"/>
       <c r="U376" s="3"/>
@@ -5632,7 +5542,7 @@
       <c r="AA376" s="4"/>
       <c r="AB376" s="4"/>
     </row>
-    <row r="377" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="377" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q377"/>
       <c r="T377" s="3"/>
       <c r="U377" s="3"/>
@@ -5644,7 +5554,7 @@
       <c r="AA377" s="4"/>
       <c r="AB377" s="4"/>
     </row>
-    <row r="378" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="378" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q378"/>
       <c r="T378" s="3"/>
       <c r="U378" s="3"/>
@@ -5656,7 +5566,7 @@
       <c r="AA378" s="4"/>
       <c r="AB378" s="4"/>
     </row>
-    <row r="379" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="379" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q379"/>
       <c r="T379" s="3"/>
       <c r="U379" s="3"/>
@@ -5668,7 +5578,7 @@
       <c r="AA379" s="4"/>
       <c r="AB379" s="4"/>
     </row>
-    <row r="380" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="380" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q380"/>
       <c r="T380" s="3"/>
       <c r="U380" s="3"/>
@@ -5680,7 +5590,7 @@
       <c r="AA380" s="4"/>
       <c r="AB380" s="4"/>
     </row>
-    <row r="381" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="381" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q381"/>
       <c r="T381" s="3"/>
       <c r="U381" s="3"/>
@@ -5692,7 +5602,7 @@
       <c r="AA381" s="4"/>
       <c r="AB381" s="4"/>
     </row>
-    <row r="382" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="382" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q382"/>
       <c r="T382" s="3"/>
       <c r="U382" s="3"/>
@@ -5704,7 +5614,7 @@
       <c r="AA382" s="4"/>
       <c r="AB382" s="4"/>
     </row>
-    <row r="383" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="383" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q383"/>
       <c r="T383" s="3"/>
       <c r="U383" s="3"/>
@@ -5716,7 +5626,7 @@
       <c r="AA383" s="4"/>
       <c r="AB383" s="4"/>
     </row>
-    <row r="384" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="384" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q384"/>
       <c r="T384" s="3"/>
       <c r="U384" s="3"/>
@@ -5729,9 +5639,7 @@
       <c r="AB384" s="4"/>
     </row>
     <row r="385" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P385" s="3"/>
       <c r="Q385"/>
-      <c r="R385" s="12"/>
       <c r="T385" s="3"/>
       <c r="U385" s="3"/>
       <c r="V385" s="3"/>
@@ -5827,7 +5735,9 @@
       <c r="AB392" s="4"/>
     </row>
     <row r="393" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P393" s="3"/>
       <c r="Q393"/>
+      <c r="R393" s="12"/>
       <c r="T393" s="3"/>
       <c r="U393" s="3"/>
       <c r="V393" s="3"/>
@@ -5983,9 +5893,7 @@
       <c r="AB405" s="4"/>
     </row>
     <row r="406" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P406" s="3"/>
       <c r="Q406"/>
-      <c r="R406" s="12"/>
       <c r="T406" s="3"/>
       <c r="U406" s="3"/>
       <c r="V406" s="3"/>
@@ -6081,7 +5989,9 @@
       <c r="AB413" s="4"/>
     </row>
     <row r="414" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P414" s="3"/>
       <c r="Q414"/>
+      <c r="R414" s="12"/>
       <c r="T414" s="3"/>
       <c r="U414" s="3"/>
       <c r="V414" s="3"/>
@@ -6238,7 +6148,6 @@
     </row>
     <row r="427" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q427"/>
-      <c r="R427" s="12"/>
       <c r="T427" s="3"/>
       <c r="U427" s="3"/>
       <c r="V427" s="3"/>
@@ -6309,7 +6218,7 @@
       <c r="AA432" s="4"/>
       <c r="AB432" s="4"/>
     </row>
-    <row r="433" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="433" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q433"/>
       <c r="T433" s="3"/>
       <c r="U433" s="3"/>
@@ -6321,7 +6230,7 @@
       <c r="AA433" s="4"/>
       <c r="AB433" s="4"/>
     </row>
-    <row r="434" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="434" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q434"/>
       <c r="T434" s="3"/>
       <c r="U434" s="3"/>
@@ -6333,8 +6242,9 @@
       <c r="AA434" s="4"/>
       <c r="AB434" s="4"/>
     </row>
-    <row r="435" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="435" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q435"/>
+      <c r="R435" s="12"/>
       <c r="T435" s="3"/>
       <c r="U435" s="3"/>
       <c r="V435" s="3"/>
@@ -6345,7 +6255,7 @@
       <c r="AA435" s="4"/>
       <c r="AB435" s="4"/>
     </row>
-    <row r="436" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="436" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q436"/>
       <c r="T436" s="3"/>
       <c r="U436" s="3"/>
@@ -6357,7 +6267,7 @@
       <c r="AA436" s="4"/>
       <c r="AB436" s="4"/>
     </row>
-    <row r="437" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="437" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q437"/>
       <c r="T437" s="3"/>
       <c r="U437" s="3"/>
@@ -6369,7 +6279,7 @@
       <c r="AA437" s="4"/>
       <c r="AB437" s="4"/>
     </row>
-    <row r="438" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="438" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q438"/>
       <c r="T438" s="3"/>
       <c r="U438" s="3"/>
@@ -6381,7 +6291,7 @@
       <c r="AA438" s="4"/>
       <c r="AB438" s="4"/>
     </row>
-    <row r="439" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="439" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q439"/>
       <c r="T439" s="3"/>
       <c r="U439" s="3"/>
@@ -6393,7 +6303,7 @@
       <c r="AA439" s="4"/>
       <c r="AB439" s="4"/>
     </row>
-    <row r="440" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="440" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q440"/>
       <c r="T440" s="3"/>
       <c r="U440" s="3"/>
@@ -6405,7 +6315,7 @@
       <c r="AA440" s="4"/>
       <c r="AB440" s="4"/>
     </row>
-    <row r="441" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="441" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q441"/>
       <c r="T441" s="3"/>
       <c r="U441" s="3"/>
@@ -6417,7 +6327,7 @@
       <c r="AA441" s="4"/>
       <c r="AB441" s="4"/>
     </row>
-    <row r="442" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="442" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q442"/>
       <c r="T442" s="3"/>
       <c r="U442" s="3"/>
@@ -6429,7 +6339,7 @@
       <c r="AA442" s="4"/>
       <c r="AB442" s="4"/>
     </row>
-    <row r="443" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="443" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q443"/>
       <c r="T443" s="3"/>
       <c r="U443" s="3"/>
@@ -6441,7 +6351,7 @@
       <c r="AA443" s="4"/>
       <c r="AB443" s="4"/>
     </row>
-    <row r="444" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="444" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q444"/>
       <c r="T444" s="3"/>
       <c r="U444" s="3"/>
@@ -6453,7 +6363,7 @@
       <c r="AA444" s="4"/>
       <c r="AB444" s="4"/>
     </row>
-    <row r="445" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="445" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q445"/>
       <c r="T445" s="3"/>
       <c r="U445" s="3"/>
@@ -6465,10 +6375,8 @@
       <c r="AA445" s="4"/>
       <c r="AB445" s="4"/>
     </row>
-    <row r="446" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P446" s="3"/>
+    <row r="446" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q446"/>
-      <c r="R446" s="12"/>
       <c r="T446" s="3"/>
       <c r="U446" s="3"/>
       <c r="V446" s="3"/>
@@ -6479,7 +6387,7 @@
       <c r="AA446" s="4"/>
       <c r="AB446" s="4"/>
     </row>
-    <row r="447" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="447" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q447"/>
       <c r="T447" s="3"/>
       <c r="U447" s="3"/>
@@ -6491,7 +6399,7 @@
       <c r="AA447" s="4"/>
       <c r="AB447" s="4"/>
     </row>
-    <row r="448" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="448" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q448"/>
       <c r="T448" s="3"/>
       <c r="U448" s="3"/>
@@ -6503,7 +6411,7 @@
       <c r="AA448" s="4"/>
       <c r="AB448" s="4"/>
     </row>
-    <row r="449" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="449" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q449"/>
       <c r="T449" s="3"/>
       <c r="U449" s="3"/>
@@ -6515,7 +6423,7 @@
       <c r="AA449" s="4"/>
       <c r="AB449" s="4"/>
     </row>
-    <row r="450" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="450" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q450"/>
       <c r="T450" s="3"/>
       <c r="U450" s="3"/>
@@ -6527,7 +6435,7 @@
       <c r="AA450" s="4"/>
       <c r="AB450" s="4"/>
     </row>
-    <row r="451" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="451" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q451"/>
       <c r="T451" s="3"/>
       <c r="U451" s="3"/>
@@ -6539,7 +6447,7 @@
       <c r="AA451" s="4"/>
       <c r="AB451" s="4"/>
     </row>
-    <row r="452" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="452" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q452"/>
       <c r="T452" s="3"/>
       <c r="U452" s="3"/>
@@ -6551,7 +6459,7 @@
       <c r="AA452" s="4"/>
       <c r="AB452" s="4"/>
     </row>
-    <row r="453" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="453" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q453"/>
       <c r="T453" s="3"/>
       <c r="U453" s="3"/>
@@ -6563,8 +6471,10 @@
       <c r="AA453" s="4"/>
       <c r="AB453" s="4"/>
     </row>
-    <row r="454" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="454" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P454" s="3"/>
       <c r="Q454"/>
+      <c r="R454" s="12"/>
       <c r="T454" s="3"/>
       <c r="U454" s="3"/>
       <c r="V454" s="3"/>
@@ -6575,7 +6485,7 @@
       <c r="AA454" s="4"/>
       <c r="AB454" s="4"/>
     </row>
-    <row r="455" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="455" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q455"/>
       <c r="T455" s="3"/>
       <c r="U455" s="3"/>
@@ -6587,7 +6497,7 @@
       <c r="AA455" s="4"/>
       <c r="AB455" s="4"/>
     </row>
-    <row r="456" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="456" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q456"/>
       <c r="T456" s="3"/>
       <c r="U456" s="3"/>
@@ -6599,7 +6509,7 @@
       <c r="AA456" s="4"/>
       <c r="AB456" s="4"/>
     </row>
-    <row r="457" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="457" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q457"/>
       <c r="T457" s="3"/>
       <c r="U457" s="3"/>
@@ -6611,7 +6521,7 @@
       <c r="AA457" s="4"/>
       <c r="AB457" s="4"/>
     </row>
-    <row r="458" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="458" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q458"/>
       <c r="T458" s="3"/>
       <c r="U458" s="3"/>
@@ -6623,7 +6533,7 @@
       <c r="AA458" s="4"/>
       <c r="AB458" s="4"/>
     </row>
-    <row r="459" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="459" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q459"/>
       <c r="T459" s="3"/>
       <c r="U459" s="3"/>
@@ -6635,7 +6545,7 @@
       <c r="AA459" s="4"/>
       <c r="AB459" s="4"/>
     </row>
-    <row r="460" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="460" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q460"/>
       <c r="T460" s="3"/>
       <c r="U460" s="3"/>
@@ -6647,7 +6557,7 @@
       <c r="AA460" s="4"/>
       <c r="AB460" s="4"/>
     </row>
-    <row r="461" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="461" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q461"/>
       <c r="T461" s="3"/>
       <c r="U461" s="3"/>
@@ -6659,7 +6569,7 @@
       <c r="AA461" s="4"/>
       <c r="AB461" s="4"/>
     </row>
-    <row r="462" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="462" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q462"/>
       <c r="T462" s="3"/>
       <c r="U462" s="3"/>
@@ -6671,7 +6581,7 @@
       <c r="AA462" s="4"/>
       <c r="AB462" s="4"/>
     </row>
-    <row r="463" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="463" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q463"/>
       <c r="T463" s="3"/>
       <c r="U463" s="3"/>
@@ -6683,7 +6593,7 @@
       <c r="AA463" s="4"/>
       <c r="AB463" s="4"/>
     </row>
-    <row r="464" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="464" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q464"/>
       <c r="T464" s="3"/>
       <c r="U464" s="3"/>
@@ -6756,9 +6666,7 @@
       <c r="AB469" s="4"/>
     </row>
     <row r="470" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P470" s="3"/>
       <c r="Q470"/>
-      <c r="R470" s="12"/>
       <c r="T470" s="3"/>
       <c r="U470" s="3"/>
       <c r="V470" s="3"/>
@@ -6854,7 +6762,9 @@
       <c r="AB477" s="4"/>
     </row>
     <row r="478" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P478" s="3"/>
       <c r="Q478"/>
+      <c r="R478" s="12"/>
       <c r="T478" s="3"/>
       <c r="U478" s="3"/>
       <c r="V478" s="3"/>
@@ -6889,7 +6799,7 @@
       <c r="AA480" s="4"/>
       <c r="AB480" s="4"/>
     </row>
-    <row r="481" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="481" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q481"/>
       <c r="T481" s="3"/>
       <c r="U481" s="3"/>
@@ -6901,7 +6811,7 @@
       <c r="AA481" s="4"/>
       <c r="AB481" s="4"/>
     </row>
-    <row r="482" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="482" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q482"/>
       <c r="T482" s="3"/>
       <c r="U482" s="3"/>
@@ -6913,7 +6823,7 @@
       <c r="AA482" s="4"/>
       <c r="AB482" s="4"/>
     </row>
-    <row r="483" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="483" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q483"/>
       <c r="T483" s="3"/>
       <c r="U483" s="3"/>
@@ -6925,7 +6835,7 @@
       <c r="AA483" s="4"/>
       <c r="AB483" s="4"/>
     </row>
-    <row r="484" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="484" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q484"/>
       <c r="T484" s="3"/>
       <c r="U484" s="3"/>
@@ -6937,7 +6847,7 @@
       <c r="AA484" s="4"/>
       <c r="AB484" s="4"/>
     </row>
-    <row r="485" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="485" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q485"/>
       <c r="T485" s="3"/>
       <c r="U485" s="3"/>
@@ -6949,7 +6859,7 @@
       <c r="AA485" s="4"/>
       <c r="AB485" s="4"/>
     </row>
-    <row r="486" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="486" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q486"/>
       <c r="T486" s="3"/>
       <c r="U486" s="3"/>
@@ -6961,7 +6871,7 @@
       <c r="AA486" s="4"/>
       <c r="AB486" s="4"/>
     </row>
-    <row r="487" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="487" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q487"/>
       <c r="T487" s="3"/>
       <c r="U487" s="3"/>
@@ -6973,7 +6883,7 @@
       <c r="AA487" s="4"/>
       <c r="AB487" s="4"/>
     </row>
-    <row r="488" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="488" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q488"/>
       <c r="T488" s="3"/>
       <c r="U488" s="3"/>
@@ -6985,10 +6895,8 @@
       <c r="AA488" s="4"/>
       <c r="AB488" s="4"/>
     </row>
-    <row r="489" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P489" s="3"/>
+    <row r="489" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q489"/>
-      <c r="R489" s="12"/>
       <c r="T489" s="3"/>
       <c r="U489" s="3"/>
       <c r="V489" s="3"/>
@@ -6999,7 +6907,7 @@
       <c r="AA489" s="4"/>
       <c r="AB489" s="4"/>
     </row>
-    <row r="490" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="490" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q490"/>
       <c r="T490" s="3"/>
       <c r="U490" s="3"/>
@@ -7011,7 +6919,7 @@
       <c r="AA490" s="4"/>
       <c r="AB490" s="4"/>
     </row>
-    <row r="491" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="491" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q491"/>
       <c r="T491" s="3"/>
       <c r="U491" s="3"/>
@@ -7023,7 +6931,7 @@
       <c r="AA491" s="4"/>
       <c r="AB491" s="4"/>
     </row>
-    <row r="492" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="492" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q492"/>
       <c r="T492" s="3"/>
       <c r="U492" s="3"/>
@@ -7035,7 +6943,7 @@
       <c r="AA492" s="4"/>
       <c r="AB492" s="4"/>
     </row>
-    <row r="493" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="493" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q493"/>
       <c r="T493" s="3"/>
       <c r="U493" s="3"/>
@@ -7047,7 +6955,7 @@
       <c r="AA493" s="4"/>
       <c r="AB493" s="4"/>
     </row>
-    <row r="494" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="494" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q494"/>
       <c r="T494" s="3"/>
       <c r="U494" s="3"/>
@@ -7059,10 +6967,8 @@
       <c r="AA494" s="4"/>
       <c r="AB494" s="4"/>
     </row>
-    <row r="495" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P495" s="3"/>
+    <row r="495" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q495"/>
-      <c r="R495" s="12"/>
       <c r="T495" s="3"/>
       <c r="U495" s="3"/>
       <c r="V495" s="3"/>
@@ -7073,7 +6979,7 @@
       <c r="AA495" s="4"/>
       <c r="AB495" s="4"/>
     </row>
-    <row r="496" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="496" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q496"/>
       <c r="T496" s="3"/>
       <c r="U496" s="3"/>
@@ -7085,8 +6991,10 @@
       <c r="AA496" s="4"/>
       <c r="AB496" s="4"/>
     </row>
-    <row r="497" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="497" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P497" s="3"/>
       <c r="Q497"/>
+      <c r="R497" s="12"/>
       <c r="T497" s="3"/>
       <c r="U497" s="3"/>
       <c r="V497" s="3"/>
@@ -7097,7 +7005,7 @@
       <c r="AA497" s="4"/>
       <c r="AB497" s="4"/>
     </row>
-    <row r="498" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="498" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q498"/>
       <c r="T498" s="3"/>
       <c r="U498" s="3"/>
@@ -7109,7 +7017,7 @@
       <c r="AA498" s="4"/>
       <c r="AB498" s="4"/>
     </row>
-    <row r="499" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="499" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q499"/>
       <c r="T499" s="3"/>
       <c r="U499" s="3"/>
@@ -7121,7 +7029,7 @@
       <c r="AA499" s="4"/>
       <c r="AB499" s="4"/>
     </row>
-    <row r="500" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="500" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q500"/>
       <c r="T500" s="3"/>
       <c r="U500" s="3"/>
@@ -7133,7 +7041,7 @@
       <c r="AA500" s="4"/>
       <c r="AB500" s="4"/>
     </row>
-    <row r="501" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="501" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q501"/>
       <c r="T501" s="3"/>
       <c r="U501" s="3"/>
@@ -7145,7 +7053,7 @@
       <c r="AA501" s="4"/>
       <c r="AB501" s="4"/>
     </row>
-    <row r="502" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="502" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q502"/>
       <c r="T502" s="3"/>
       <c r="U502" s="3"/>
@@ -7157,8 +7065,10 @@
       <c r="AA502" s="4"/>
       <c r="AB502" s="4"/>
     </row>
-    <row r="503" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="503" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P503" s="3"/>
       <c r="Q503"/>
+      <c r="R503" s="12"/>
       <c r="T503" s="3"/>
       <c r="U503" s="3"/>
       <c r="V503" s="3"/>
@@ -7169,7 +7079,7 @@
       <c r="AA503" s="4"/>
       <c r="AB503" s="4"/>
     </row>
-    <row r="504" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="504" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q504"/>
       <c r="T504" s="3"/>
       <c r="U504" s="3"/>
@@ -7181,7 +7091,7 @@
       <c r="AA504" s="4"/>
       <c r="AB504" s="4"/>
     </row>
-    <row r="505" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="505" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q505"/>
       <c r="T505" s="3"/>
       <c r="U505" s="3"/>
@@ -7193,7 +7103,7 @@
       <c r="AA505" s="4"/>
       <c r="AB505" s="4"/>
     </row>
-    <row r="506" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="506" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q506"/>
       <c r="T506" s="3"/>
       <c r="U506" s="3"/>
@@ -7205,7 +7115,7 @@
       <c r="AA506" s="4"/>
       <c r="AB506" s="4"/>
     </row>
-    <row r="507" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="507" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q507"/>
       <c r="T507" s="3"/>
       <c r="U507" s="3"/>
@@ -7217,9 +7127,8 @@
       <c r="AA507" s="4"/>
       <c r="AB507" s="4"/>
     </row>
-    <row r="508" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="508" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q508"/>
-      <c r="R508" s="12"/>
       <c r="T508" s="3"/>
       <c r="U508" s="3"/>
       <c r="V508" s="3"/>
@@ -7230,7 +7139,7 @@
       <c r="AA508" s="4"/>
       <c r="AB508" s="4"/>
     </row>
-    <row r="509" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="509" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q509"/>
       <c r="T509" s="3"/>
       <c r="U509" s="3"/>
@@ -7242,7 +7151,7 @@
       <c r="AA509" s="4"/>
       <c r="AB509" s="4"/>
     </row>
-    <row r="510" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="510" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q510"/>
       <c r="T510" s="3"/>
       <c r="U510" s="3"/>
@@ -7254,7 +7163,7 @@
       <c r="AA510" s="4"/>
       <c r="AB510" s="4"/>
     </row>
-    <row r="511" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="511" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q511"/>
       <c r="T511" s="3"/>
       <c r="U511" s="3"/>
@@ -7266,7 +7175,7 @@
       <c r="AA511" s="4"/>
       <c r="AB511" s="4"/>
     </row>
-    <row r="512" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="512" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q512"/>
       <c r="T512" s="3"/>
       <c r="U512" s="3"/>
@@ -7316,6 +7225,7 @@
     </row>
     <row r="516" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q516"/>
+      <c r="R516" s="12"/>
       <c r="T516" s="3"/>
       <c r="U516" s="3"/>
       <c r="V516" s="3"/>
@@ -7351,9 +7261,7 @@
       <c r="AB518" s="4"/>
     </row>
     <row r="519" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P519" s="3"/>
       <c r="Q519"/>
-      <c r="R519" s="12"/>
       <c r="T519" s="3"/>
       <c r="U519" s="3"/>
       <c r="V519" s="3"/>
@@ -7449,7 +7357,9 @@
       <c r="AB526" s="4"/>
     </row>
     <row r="527" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P527" s="3"/>
       <c r="Q527"/>
+      <c r="R527" s="12"/>
       <c r="T527" s="3"/>
       <c r="U527" s="3"/>
       <c r="V527" s="3"/>
@@ -7497,9 +7407,7 @@
       <c r="AB530" s="4"/>
     </row>
     <row r="531" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P531" s="3"/>
       <c r="Q531"/>
-      <c r="R531" s="12"/>
       <c r="T531" s="3"/>
       <c r="U531" s="3"/>
       <c r="V531" s="3"/>
@@ -7693,7 +7601,9 @@
       <c r="AB546" s="4"/>
     </row>
     <row r="547" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P547" s="3"/>
       <c r="Q547"/>
+      <c r="R547" s="12"/>
       <c r="T547" s="3"/>
       <c r="U547" s="3"/>
       <c r="V547" s="3"/>
@@ -7801,9 +7711,7 @@
       <c r="AB555" s="4"/>
     </row>
     <row r="556" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P556" s="3"/>
       <c r="Q556"/>
-      <c r="R556" s="12"/>
       <c r="T556" s="3"/>
       <c r="U556" s="3"/>
       <c r="V556" s="3"/>
@@ -7899,7 +7807,9 @@
       <c r="AB563" s="4"/>
     </row>
     <row r="564" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P564" s="3"/>
       <c r="Q564"/>
+      <c r="R564" s="12"/>
       <c r="T564" s="3"/>
       <c r="U564" s="3"/>
       <c r="V564" s="3"/>
@@ -7924,7 +7834,6 @@
     </row>
     <row r="566" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q566"/>
-      <c r="R566" s="12"/>
       <c r="T566" s="3"/>
       <c r="U566" s="3"/>
       <c r="V566" s="3"/>
@@ -7984,9 +7893,7 @@
       <c r="AB570" s="4"/>
     </row>
     <row r="571" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P571" s="3"/>
       <c r="Q571"/>
-      <c r="R571" s="12"/>
       <c r="T571" s="3"/>
       <c r="U571" s="3"/>
       <c r="V571" s="3"/>
@@ -8023,6 +7930,7 @@
     </row>
     <row r="574" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q574"/>
+      <c r="R574" s="12"/>
       <c r="T574" s="3"/>
       <c r="U574" s="3"/>
       <c r="V574" s="3"/>
@@ -8057,7 +7965,7 @@
       <c r="AA576" s="4"/>
       <c r="AB576" s="4"/>
     </row>
-    <row r="577" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="577" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q577"/>
       <c r="T577" s="3"/>
       <c r="U577" s="3"/>
@@ -8069,7 +7977,7 @@
       <c r="AA577" s="4"/>
       <c r="AB577" s="4"/>
     </row>
-    <row r="578" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="578" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q578"/>
       <c r="T578" s="3"/>
       <c r="U578" s="3"/>
@@ -8081,8 +7989,10 @@
       <c r="AA578" s="4"/>
       <c r="AB578" s="4"/>
     </row>
-    <row r="579" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="579" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P579" s="3"/>
       <c r="Q579"/>
+      <c r="R579" s="12"/>
       <c r="T579" s="3"/>
       <c r="U579" s="3"/>
       <c r="V579" s="3"/>
@@ -8093,7 +8003,7 @@
       <c r="AA579" s="4"/>
       <c r="AB579" s="4"/>
     </row>
-    <row r="580" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="580" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q580"/>
       <c r="T580" s="3"/>
       <c r="U580" s="3"/>
@@ -8105,7 +8015,7 @@
       <c r="AA580" s="4"/>
       <c r="AB580" s="4"/>
     </row>
-    <row r="581" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="581" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q581"/>
       <c r="T581" s="3"/>
       <c r="U581" s="3"/>
@@ -8117,7 +8027,7 @@
       <c r="AA581" s="4"/>
       <c r="AB581" s="4"/>
     </row>
-    <row r="582" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="582" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q582"/>
       <c r="T582" s="3"/>
       <c r="U582" s="3"/>
@@ -8129,7 +8039,7 @@
       <c r="AA582" s="4"/>
       <c r="AB582" s="4"/>
     </row>
-    <row r="583" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="583" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q583"/>
       <c r="T583" s="3"/>
       <c r="U583" s="3"/>
@@ -8141,7 +8051,7 @@
       <c r="AA583" s="4"/>
       <c r="AB583" s="4"/>
     </row>
-    <row r="584" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="584" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q584"/>
       <c r="T584" s="3"/>
       <c r="U584" s="3"/>
@@ -8153,7 +8063,7 @@
       <c r="AA584" s="4"/>
       <c r="AB584" s="4"/>
     </row>
-    <row r="585" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="585" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q585"/>
       <c r="T585" s="3"/>
       <c r="U585" s="3"/>
@@ -8165,7 +8075,7 @@
       <c r="AA585" s="4"/>
       <c r="AB585" s="4"/>
     </row>
-    <row r="586" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="586" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q586"/>
       <c r="T586" s="3"/>
       <c r="U586" s="3"/>
@@ -8177,7 +8087,7 @@
       <c r="AA586" s="4"/>
       <c r="AB586" s="4"/>
     </row>
-    <row r="587" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="587" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q587"/>
       <c r="T587" s="3"/>
       <c r="U587" s="3"/>
@@ -8189,7 +8099,7 @@
       <c r="AA587" s="4"/>
       <c r="AB587" s="4"/>
     </row>
-    <row r="588" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="588" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q588"/>
       <c r="T588" s="3"/>
       <c r="U588" s="3"/>
@@ -8201,7 +8111,7 @@
       <c r="AA588" s="4"/>
       <c r="AB588" s="4"/>
     </row>
-    <row r="589" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="589" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q589"/>
       <c r="T589" s="3"/>
       <c r="U589" s="3"/>
@@ -8213,7 +8123,7 @@
       <c r="AA589" s="4"/>
       <c r="AB589" s="4"/>
     </row>
-    <row r="590" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="590" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q590"/>
       <c r="T590" s="3"/>
       <c r="U590" s="3"/>
@@ -8225,7 +8135,7 @@
       <c r="AA590" s="4"/>
       <c r="AB590" s="4"/>
     </row>
-    <row r="591" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="591" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q591"/>
       <c r="T591" s="3"/>
       <c r="U591" s="3"/>
@@ -8237,7 +8147,7 @@
       <c r="AA591" s="4"/>
       <c r="AB591" s="4"/>
     </row>
-    <row r="592" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="592" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q592"/>
       <c r="T592" s="3"/>
       <c r="U592" s="3"/>
@@ -8322,36 +8232,100 @@
       <c r="AB598" s="4"/>
     </row>
     <row r="599" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T599" s="6"/>
-      <c r="U599" s="6"/>
+      <c r="Q599"/>
+      <c r="T599" s="3"/>
+      <c r="U599" s="3"/>
+      <c r="V599" s="3"/>
+      <c r="W599"/>
+      <c r="X599" s="10"/>
+      <c r="Y599"/>
+      <c r="Z599"/>
+      <c r="AA599" s="4"/>
+      <c r="AB599" s="4"/>
     </row>
     <row r="600" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T600" s="6"/>
-      <c r="U600" s="6"/>
+      <c r="Q600"/>
+      <c r="T600" s="3"/>
+      <c r="U600" s="3"/>
+      <c r="V600" s="3"/>
+      <c r="W600"/>
+      <c r="X600" s="10"/>
+      <c r="Y600"/>
+      <c r="Z600"/>
+      <c r="AA600" s="4"/>
+      <c r="AB600" s="4"/>
     </row>
     <row r="601" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T601" s="6"/>
-      <c r="U601" s="6"/>
+      <c r="Q601"/>
+      <c r="T601" s="3"/>
+      <c r="U601" s="3"/>
+      <c r="V601" s="3"/>
+      <c r="W601"/>
+      <c r="X601" s="10"/>
+      <c r="Y601"/>
+      <c r="Z601"/>
+      <c r="AA601" s="4"/>
+      <c r="AB601" s="4"/>
     </row>
     <row r="602" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T602" s="6"/>
-      <c r="U602" s="6"/>
+      <c r="Q602"/>
+      <c r="T602" s="3"/>
+      <c r="U602" s="3"/>
+      <c r="V602" s="3"/>
+      <c r="W602"/>
+      <c r="X602" s="10"/>
+      <c r="Y602"/>
+      <c r="Z602"/>
+      <c r="AA602" s="4"/>
+      <c r="AB602" s="4"/>
     </row>
     <row r="603" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T603" s="6"/>
-      <c r="U603" s="6"/>
+      <c r="Q603"/>
+      <c r="T603" s="3"/>
+      <c r="U603" s="3"/>
+      <c r="V603" s="3"/>
+      <c r="W603"/>
+      <c r="X603" s="10"/>
+      <c r="Y603"/>
+      <c r="Z603"/>
+      <c r="AA603" s="4"/>
+      <c r="AB603" s="4"/>
     </row>
     <row r="604" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T604" s="6"/>
-      <c r="U604" s="6"/>
+      <c r="Q604"/>
+      <c r="T604" s="3"/>
+      <c r="U604" s="3"/>
+      <c r="V604" s="3"/>
+      <c r="W604"/>
+      <c r="X604" s="10"/>
+      <c r="Y604"/>
+      <c r="Z604"/>
+      <c r="AA604" s="4"/>
+      <c r="AB604" s="4"/>
     </row>
     <row r="605" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T605" s="6"/>
-      <c r="U605" s="6"/>
+      <c r="Q605"/>
+      <c r="T605" s="3"/>
+      <c r="U605" s="3"/>
+      <c r="V605" s="3"/>
+      <c r="W605"/>
+      <c r="X605" s="10"/>
+      <c r="Y605"/>
+      <c r="Z605"/>
+      <c r="AA605" s="4"/>
+      <c r="AB605" s="4"/>
     </row>
     <row r="606" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T606" s="6"/>
-      <c r="U606" s="6"/>
+      <c r="Q606"/>
+      <c r="T606" s="3"/>
+      <c r="U606" s="3"/>
+      <c r="V606" s="3"/>
+      <c r="W606"/>
+      <c r="X606" s="10"/>
+      <c r="Y606"/>
+      <c r="Z606"/>
+      <c r="AA606" s="4"/>
+      <c r="AB606" s="4"/>
     </row>
     <row r="607" spans="17:28" x14ac:dyDescent="0.2">
       <c r="T607" s="6"/>
@@ -8440,6 +8414,38 @@
     <row r="628" spans="20:21" x14ac:dyDescent="0.2">
       <c r="T628" s="6"/>
       <c r="U628" s="6"/>
+    </row>
+    <row r="629" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T629" s="6"/>
+      <c r="U629" s="6"/>
+    </row>
+    <row r="630" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T630" s="6"/>
+      <c r="U630" s="6"/>
+    </row>
+    <row r="631" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T631" s="6"/>
+      <c r="U631" s="6"/>
+    </row>
+    <row r="632" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T632" s="6"/>
+      <c r="U632" s="6"/>
+    </row>
+    <row r="633" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T633" s="6"/>
+      <c r="U633" s="6"/>
+    </row>
+    <row r="634" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T634" s="6"/>
+      <c r="U634" s="6"/>
+    </row>
+    <row r="635" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T635" s="6"/>
+      <c r="U635" s="6"/>
+    </row>
+    <row r="636" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T636" s="6"/>
+      <c r="U636" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -8451,12 +8457,9 @@
     <hyperlink ref="F7" r:id="rId5"/>
     <hyperlink ref="F8" r:id="rId6"/>
     <hyperlink ref="F11" r:id="rId7"/>
-    <hyperlink ref="F12" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add inputtypes & orientation index
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Customers.xlsx
+++ b/EDI/Web/wwwroot/Upload/Customers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>School Name</t>
   </si>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB628"/>
+  <dimension ref="A1:AB636"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1116,36 +1116,6 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="20">
-        <v>42299</v>
-      </c>
-      <c r="K12" s="21">
-        <v>200122609501901</v>
-      </c>
       <c r="Q12"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -1158,36 +1128,6 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="20">
-        <v>41876</v>
-      </c>
-      <c r="K13" s="21">
-        <v>200122604903901</v>
-      </c>
       <c r="Q13"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -1199,37 +1139,7 @@
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="20">
-        <v>42113</v>
-      </c>
-      <c r="K14" s="21">
-        <v>200122699902901</v>
-      </c>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Q14"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1399,7 +1309,6 @@
     </row>
     <row r="28" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q28"/>
-      <c r="R28" s="12"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -1496,6 +1405,7 @@
     </row>
     <row r="36" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q36"/>
+      <c r="R36" s="12"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -1687,9 +1597,7 @@
       <c r="AB51" s="4"/>
     </row>
     <row r="52" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P52" s="3"/>
       <c r="Q52"/>
-      <c r="R52" s="12"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -1785,7 +1693,9 @@
       <c r="AB59" s="4"/>
     </row>
     <row r="60" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P60" s="3"/>
       <c r="Q60"/>
+      <c r="R60" s="12"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="3"/>
@@ -1929,9 +1839,7 @@
       <c r="AB71" s="4"/>
     </row>
     <row r="72" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P72" s="3"/>
       <c r="Q72"/>
-      <c r="R72" s="12"/>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
@@ -2016,7 +1924,6 @@
     </row>
     <row r="79" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q79"/>
-      <c r="R79" s="12"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
@@ -2028,7 +1935,9 @@
       <c r="AB79" s="4"/>
     </row>
     <row r="80" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P80" s="3"/>
       <c r="Q80"/>
+      <c r="R80" s="12"/>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
@@ -2112,7 +2021,6 @@
       <c r="AB86" s="4"/>
     </row>
     <row r="87" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P87" s="3"/>
       <c r="Q87"/>
       <c r="R87" s="12"/>
       <c r="T87" s="3"/>
@@ -2210,7 +2118,9 @@
       <c r="AB94" s="4"/>
     </row>
     <row r="95" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P95" s="3"/>
       <c r="Q95"/>
+      <c r="R95" s="12"/>
       <c r="T95" s="3"/>
       <c r="U95" s="3"/>
       <c r="V95" s="3"/>
@@ -2233,7 +2143,7 @@
       <c r="AA96" s="4"/>
       <c r="AB96" s="4"/>
     </row>
-    <row r="97" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q97"/>
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
@@ -2245,7 +2155,7 @@
       <c r="AA97" s="4"/>
       <c r="AB97" s="4"/>
     </row>
-    <row r="98" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q98"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -2257,7 +2167,7 @@
       <c r="AA98" s="4"/>
       <c r="AB98" s="4"/>
     </row>
-    <row r="99" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q99"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -2269,9 +2179,8 @@
       <c r="AA99" s="4"/>
       <c r="AB99" s="4"/>
     </row>
-    <row r="100" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="100" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q100"/>
-      <c r="R100" s="12"/>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
       <c r="V100" s="3"/>
@@ -2282,7 +2191,7 @@
       <c r="AA100" s="4"/>
       <c r="AB100" s="4"/>
     </row>
-    <row r="101" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q101"/>
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
@@ -2294,7 +2203,7 @@
       <c r="AA101" s="4"/>
       <c r="AB101" s="4"/>
     </row>
-    <row r="102" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q102"/>
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
@@ -2306,7 +2215,7 @@
       <c r="AA102" s="4"/>
       <c r="AB102" s="4"/>
     </row>
-    <row r="103" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q103"/>
       <c r="T103" s="3"/>
       <c r="U103" s="3"/>
@@ -2318,7 +2227,7 @@
       <c r="AA103" s="4"/>
       <c r="AB103" s="4"/>
     </row>
-    <row r="104" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q104"/>
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
@@ -2330,7 +2239,7 @@
       <c r="AA104" s="4"/>
       <c r="AB104" s="4"/>
     </row>
-    <row r="105" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q105"/>
       <c r="T105" s="3"/>
       <c r="U105" s="3"/>
@@ -2342,7 +2251,7 @@
       <c r="AA105" s="4"/>
       <c r="AB105" s="4"/>
     </row>
-    <row r="106" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q106"/>
       <c r="T106" s="3"/>
       <c r="U106" s="3"/>
@@ -2354,7 +2263,7 @@
       <c r="AA106" s="4"/>
       <c r="AB106" s="4"/>
     </row>
-    <row r="107" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q107"/>
       <c r="T107" s="3"/>
       <c r="U107" s="3"/>
@@ -2366,8 +2275,7 @@
       <c r="AA107" s="4"/>
       <c r="AB107" s="4"/>
     </row>
-    <row r="108" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P108" s="3"/>
+    <row r="108" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q108"/>
       <c r="R108" s="12"/>
       <c r="T108" s="3"/>
@@ -2380,7 +2288,7 @@
       <c r="AA108" s="4"/>
       <c r="AB108" s="4"/>
     </row>
-    <row r="109" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q109"/>
       <c r="T109" s="3"/>
       <c r="U109" s="3"/>
@@ -2392,7 +2300,7 @@
       <c r="AA109" s="4"/>
       <c r="AB109" s="4"/>
     </row>
-    <row r="110" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q110"/>
       <c r="T110" s="3"/>
       <c r="U110" s="3"/>
@@ -2404,7 +2312,7 @@
       <c r="AA110" s="4"/>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q111"/>
       <c r="T111" s="3"/>
       <c r="U111" s="3"/>
@@ -2416,7 +2324,7 @@
       <c r="AA111" s="4"/>
       <c r="AB111" s="4"/>
     </row>
-    <row r="112" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q112"/>
       <c r="T112" s="3"/>
       <c r="U112" s="3"/>
@@ -2428,7 +2336,7 @@
       <c r="AA112" s="4"/>
       <c r="AB112" s="4"/>
     </row>
-    <row r="113" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q113"/>
       <c r="T113" s="3"/>
       <c r="U113" s="3"/>
@@ -2440,7 +2348,7 @@
       <c r="AA113" s="4"/>
       <c r="AB113" s="4"/>
     </row>
-    <row r="114" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q114"/>
       <c r="T114" s="3"/>
       <c r="U114" s="3"/>
@@ -2452,7 +2360,7 @@
       <c r="AA114" s="4"/>
       <c r="AB114" s="4"/>
     </row>
-    <row r="115" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q115"/>
       <c r="T115" s="3"/>
       <c r="U115" s="3"/>
@@ -2464,8 +2372,10 @@
       <c r="AA115" s="4"/>
       <c r="AB115" s="4"/>
     </row>
-    <row r="116" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P116" s="3"/>
       <c r="Q116"/>
+      <c r="R116" s="12"/>
       <c r="T116" s="3"/>
       <c r="U116" s="3"/>
       <c r="V116" s="3"/>
@@ -2476,7 +2386,7 @@
       <c r="AA116" s="4"/>
       <c r="AB116" s="4"/>
     </row>
-    <row r="117" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q117"/>
       <c r="T117" s="3"/>
       <c r="U117" s="3"/>
@@ -2488,7 +2398,7 @@
       <c r="AA117" s="4"/>
       <c r="AB117" s="4"/>
     </row>
-    <row r="118" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q118"/>
       <c r="T118" s="3"/>
       <c r="U118" s="3"/>
@@ -2500,7 +2410,7 @@
       <c r="AA118" s="4"/>
       <c r="AB118" s="4"/>
     </row>
-    <row r="119" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q119"/>
       <c r="T119" s="3"/>
       <c r="U119" s="3"/>
@@ -2512,7 +2422,7 @@
       <c r="AA119" s="4"/>
       <c r="AB119" s="4"/>
     </row>
-    <row r="120" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q120"/>
       <c r="T120" s="3"/>
       <c r="U120" s="3"/>
@@ -2524,9 +2434,8 @@
       <c r="AA120" s="4"/>
       <c r="AB120" s="4"/>
     </row>
-    <row r="121" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q121"/>
-      <c r="R121" s="12"/>
       <c r="T121" s="3"/>
       <c r="U121" s="3"/>
       <c r="V121" s="3"/>
@@ -2537,7 +2446,7 @@
       <c r="AA121" s="4"/>
       <c r="AB121" s="4"/>
     </row>
-    <row r="122" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q122"/>
       <c r="T122" s="3"/>
       <c r="U122" s="3"/>
@@ -2549,7 +2458,7 @@
       <c r="AA122" s="4"/>
       <c r="AB122" s="4"/>
     </row>
-    <row r="123" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q123"/>
       <c r="T123" s="3"/>
       <c r="U123" s="3"/>
@@ -2561,7 +2470,7 @@
       <c r="AA123" s="4"/>
       <c r="AB123" s="4"/>
     </row>
-    <row r="124" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q124"/>
       <c r="T124" s="3"/>
       <c r="U124" s="3"/>
@@ -2573,7 +2482,7 @@
       <c r="AA124" s="4"/>
       <c r="AB124" s="4"/>
     </row>
-    <row r="125" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q125"/>
       <c r="T125" s="3"/>
       <c r="U125" s="3"/>
@@ -2585,7 +2494,7 @@
       <c r="AA125" s="4"/>
       <c r="AB125" s="4"/>
     </row>
-    <row r="126" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q126"/>
       <c r="T126" s="3"/>
       <c r="U126" s="3"/>
@@ -2597,7 +2506,7 @@
       <c r="AA126" s="4"/>
       <c r="AB126" s="4"/>
     </row>
-    <row r="127" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q127"/>
       <c r="T127" s="3"/>
       <c r="U127" s="3"/>
@@ -2609,7 +2518,7 @@
       <c r="AA127" s="4"/>
       <c r="AB127" s="4"/>
     </row>
-    <row r="128" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q128"/>
       <c r="T128" s="3"/>
       <c r="U128" s="3"/>
@@ -2623,6 +2532,7 @@
     </row>
     <row r="129" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q129"/>
+      <c r="R129" s="12"/>
       <c r="T129" s="3"/>
       <c r="U129" s="3"/>
       <c r="V129" s="3"/>
@@ -2694,9 +2604,7 @@
       <c r="AB134" s="4"/>
     </row>
     <row r="135" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P135" s="3"/>
       <c r="Q135"/>
-      <c r="R135" s="12"/>
       <c r="T135" s="3"/>
       <c r="U135" s="3"/>
       <c r="V135" s="3"/>
@@ -2792,7 +2700,9 @@
       <c r="AB142" s="4"/>
     </row>
     <row r="143" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P143" s="3"/>
       <c r="Q143"/>
+      <c r="R143" s="12"/>
       <c r="T143" s="3"/>
       <c r="U143" s="3"/>
       <c r="V143" s="3"/>
@@ -2840,9 +2750,7 @@
       <c r="AB146" s="4"/>
     </row>
     <row r="147" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P147" s="3"/>
       <c r="Q147"/>
-      <c r="R147" s="12"/>
       <c r="T147" s="3"/>
       <c r="U147" s="3"/>
       <c r="V147" s="3"/>
@@ -2938,7 +2846,9 @@
       <c r="AB154" s="4"/>
     </row>
     <row r="155" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P155" s="3"/>
       <c r="Q155"/>
+      <c r="R155" s="12"/>
       <c r="T155" s="3"/>
       <c r="U155" s="3"/>
       <c r="V155" s="3"/>
@@ -3009,9 +2919,8 @@
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
     </row>
-    <row r="161" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="161" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q161"/>
-      <c r="R161" s="12"/>
       <c r="T161" s="3"/>
       <c r="U161" s="3"/>
       <c r="V161" s="3"/>
@@ -3022,7 +2931,7 @@
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
     </row>
-    <row r="162" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="162" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q162"/>
       <c r="T162" s="3"/>
       <c r="U162" s="3"/>
@@ -3034,7 +2943,7 @@
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
     </row>
-    <row r="163" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="163" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q163"/>
       <c r="T163" s="3"/>
       <c r="U163" s="3"/>
@@ -3046,7 +2955,7 @@
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
     </row>
-    <row r="164" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="164" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q164"/>
       <c r="T164" s="3"/>
       <c r="U164" s="3"/>
@@ -3058,7 +2967,7 @@
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
     </row>
-    <row r="165" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="165" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q165"/>
       <c r="T165" s="3"/>
       <c r="U165" s="3"/>
@@ -3070,7 +2979,7 @@
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
     </row>
-    <row r="166" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="166" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q166"/>
       <c r="T166" s="3"/>
       <c r="U166" s="3"/>
@@ -3082,7 +2991,7 @@
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
     </row>
-    <row r="167" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="167" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q167"/>
       <c r="T167" s="3"/>
       <c r="U167" s="3"/>
@@ -3094,7 +3003,7 @@
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
     </row>
-    <row r="168" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="168" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q168"/>
       <c r="T168" s="3"/>
       <c r="U168" s="3"/>
@@ -3106,8 +3015,9 @@
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
     </row>
-    <row r="169" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="169" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q169"/>
+      <c r="R169" s="12"/>
       <c r="T169" s="3"/>
       <c r="U169" s="3"/>
       <c r="V169" s="3"/>
@@ -3118,7 +3028,7 @@
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
     </row>
-    <row r="170" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="170" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q170"/>
       <c r="T170" s="3"/>
       <c r="U170" s="3"/>
@@ -3130,7 +3040,7 @@
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
     </row>
-    <row r="171" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="171" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q171"/>
       <c r="T171" s="3"/>
       <c r="U171" s="3"/>
@@ -3142,7 +3052,7 @@
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
     </row>
-    <row r="172" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="172" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q172"/>
       <c r="T172" s="3"/>
       <c r="U172" s="3"/>
@@ -3154,10 +3064,8 @@
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
     </row>
-    <row r="173" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P173" s="3"/>
+    <row r="173" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q173"/>
-      <c r="R173" s="12"/>
       <c r="T173" s="3"/>
       <c r="U173" s="3"/>
       <c r="V173" s="3"/>
@@ -3168,7 +3076,7 @@
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
     </row>
-    <row r="174" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="174" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q174"/>
       <c r="T174" s="3"/>
       <c r="U174" s="3"/>
@@ -3180,7 +3088,7 @@
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
     </row>
-    <row r="175" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="175" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q175"/>
       <c r="T175" s="3"/>
       <c r="U175" s="3"/>
@@ -3192,7 +3100,7 @@
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
     </row>
-    <row r="176" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="176" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q176"/>
       <c r="T176" s="3"/>
       <c r="U176" s="3"/>
@@ -3253,7 +3161,9 @@
       <c r="AB180" s="4"/>
     </row>
     <row r="181" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P181" s="3"/>
       <c r="Q181"/>
+      <c r="R181" s="12"/>
       <c r="T181" s="3"/>
       <c r="U181" s="3"/>
       <c r="V181" s="3"/>
@@ -3313,9 +3223,7 @@
       <c r="AB185" s="4"/>
     </row>
     <row r="186" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P186" s="3"/>
       <c r="Q186"/>
-      <c r="R186" s="12"/>
       <c r="T186" s="3"/>
       <c r="U186" s="3"/>
       <c r="V186" s="3"/>
@@ -3398,7 +3306,7 @@
       <c r="AA192" s="4"/>
       <c r="AB192" s="4"/>
     </row>
-    <row r="193" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="193" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q193"/>
       <c r="T193" s="3"/>
       <c r="U193" s="3"/>
@@ -3410,8 +3318,10 @@
       <c r="AA193" s="4"/>
       <c r="AB193" s="4"/>
     </row>
-    <row r="194" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="194" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P194" s="3"/>
       <c r="Q194"/>
+      <c r="R194" s="12"/>
       <c r="T194" s="3"/>
       <c r="U194" s="3"/>
       <c r="V194" s="3"/>
@@ -3422,9 +3332,8 @@
       <c r="AA194" s="4"/>
       <c r="AB194" s="4"/>
     </row>
-    <row r="195" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="195" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q195"/>
-      <c r="R195" s="12"/>
       <c r="T195" s="3"/>
       <c r="U195" s="3"/>
       <c r="V195" s="3"/>
@@ -3435,7 +3344,7 @@
       <c r="AA195" s="4"/>
       <c r="AB195" s="4"/>
     </row>
-    <row r="196" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="196" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q196"/>
       <c r="T196" s="3"/>
       <c r="U196" s="3"/>
@@ -3447,7 +3356,7 @@
       <c r="AA196" s="4"/>
       <c r="AB196" s="4"/>
     </row>
-    <row r="197" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="197" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q197"/>
       <c r="T197" s="3"/>
       <c r="U197" s="3"/>
@@ -3459,7 +3368,7 @@
       <c r="AA197" s="4"/>
       <c r="AB197" s="4"/>
     </row>
-    <row r="198" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="198" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q198"/>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
@@ -3471,7 +3380,7 @@
       <c r="AA198" s="4"/>
       <c r="AB198" s="4"/>
     </row>
-    <row r="199" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="199" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q199"/>
       <c r="T199" s="3"/>
       <c r="U199" s="3"/>
@@ -3483,7 +3392,7 @@
       <c r="AA199" s="4"/>
       <c r="AB199" s="4"/>
     </row>
-    <row r="200" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="200" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q200"/>
       <c r="T200" s="3"/>
       <c r="U200" s="3"/>
@@ -3495,7 +3404,7 @@
       <c r="AA200" s="4"/>
       <c r="AB200" s="4"/>
     </row>
-    <row r="201" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="201" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q201"/>
       <c r="T201" s="3"/>
       <c r="U201" s="3"/>
@@ -3507,7 +3416,7 @@
       <c r="AA201" s="4"/>
       <c r="AB201" s="4"/>
     </row>
-    <row r="202" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="202" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q202"/>
       <c r="T202" s="3"/>
       <c r="U202" s="3"/>
@@ -3519,8 +3428,9 @@
       <c r="AA202" s="4"/>
       <c r="AB202" s="4"/>
     </row>
-    <row r="203" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="203" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q203"/>
+      <c r="R203" s="12"/>
       <c r="T203" s="3"/>
       <c r="U203" s="3"/>
       <c r="V203" s="3"/>
@@ -3531,7 +3441,7 @@
       <c r="AA203" s="4"/>
       <c r="AB203" s="4"/>
     </row>
-    <row r="204" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="204" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q204"/>
       <c r="T204" s="3"/>
       <c r="U204" s="3"/>
@@ -3543,7 +3453,7 @@
       <c r="AA204" s="4"/>
       <c r="AB204" s="4"/>
     </row>
-    <row r="205" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="205" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q205"/>
       <c r="T205" s="3"/>
       <c r="U205" s="3"/>
@@ -3555,7 +3465,7 @@
       <c r="AA205" s="4"/>
       <c r="AB205" s="4"/>
     </row>
-    <row r="206" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="206" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q206"/>
       <c r="T206" s="3"/>
       <c r="U206" s="3"/>
@@ -3567,7 +3477,7 @@
       <c r="AA206" s="4"/>
       <c r="AB206" s="4"/>
     </row>
-    <row r="207" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="207" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q207"/>
       <c r="T207" s="3"/>
       <c r="U207" s="3"/>
@@ -3579,7 +3489,7 @@
       <c r="AA207" s="4"/>
       <c r="AB207" s="4"/>
     </row>
-    <row r="208" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="208" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q208"/>
       <c r="T208" s="3"/>
       <c r="U208" s="3"/>
@@ -3591,7 +3501,7 @@
       <c r="AA208" s="4"/>
       <c r="AB208" s="4"/>
     </row>
-    <row r="209" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="209" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q209"/>
       <c r="T209" s="3"/>
       <c r="U209" s="3"/>
@@ -3603,7 +3513,7 @@
       <c r="AA209" s="4"/>
       <c r="AB209" s="4"/>
     </row>
-    <row r="210" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="210" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q210"/>
       <c r="T210" s="3"/>
       <c r="U210" s="3"/>
@@ -3615,7 +3525,7 @@
       <c r="AA210" s="4"/>
       <c r="AB210" s="4"/>
     </row>
-    <row r="211" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="211" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q211"/>
       <c r="T211" s="3"/>
       <c r="U211" s="3"/>
@@ -3627,7 +3537,7 @@
       <c r="AA211" s="4"/>
       <c r="AB211" s="4"/>
     </row>
-    <row r="212" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="212" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q212"/>
       <c r="T212" s="3"/>
       <c r="U212" s="3"/>
@@ -3639,7 +3549,7 @@
       <c r="AA212" s="4"/>
       <c r="AB212" s="4"/>
     </row>
-    <row r="213" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="213" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q213"/>
       <c r="T213" s="3"/>
       <c r="U213" s="3"/>
@@ -3651,7 +3561,7 @@
       <c r="AA213" s="4"/>
       <c r="AB213" s="4"/>
     </row>
-    <row r="214" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="214" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q214"/>
       <c r="T214" s="3"/>
       <c r="U214" s="3"/>
@@ -3663,7 +3573,7 @@
       <c r="AA214" s="4"/>
       <c r="AB214" s="4"/>
     </row>
-    <row r="215" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="215" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q215"/>
       <c r="T215" s="3"/>
       <c r="U215" s="3"/>
@@ -3675,7 +3585,7 @@
       <c r="AA215" s="4"/>
       <c r="AB215" s="4"/>
     </row>
-    <row r="216" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="216" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q216"/>
       <c r="T216" s="3"/>
       <c r="U216" s="3"/>
@@ -3687,10 +3597,8 @@
       <c r="AA216" s="4"/>
       <c r="AB216" s="4"/>
     </row>
-    <row r="217" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P217" s="3"/>
+    <row r="217" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q217"/>
-      <c r="R217" s="12"/>
       <c r="T217" s="3"/>
       <c r="U217" s="3"/>
       <c r="V217" s="3"/>
@@ -3701,7 +3609,7 @@
       <c r="AA217" s="4"/>
       <c r="AB217" s="4"/>
     </row>
-    <row r="218" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="218" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q218"/>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
@@ -3713,7 +3621,7 @@
       <c r="AA218" s="4"/>
       <c r="AB218" s="4"/>
     </row>
-    <row r="219" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="219" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q219"/>
       <c r="T219" s="3"/>
       <c r="U219" s="3"/>
@@ -3725,7 +3633,7 @@
       <c r="AA219" s="4"/>
       <c r="AB219" s="4"/>
     </row>
-    <row r="220" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="220" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q220"/>
       <c r="T220" s="3"/>
       <c r="U220" s="3"/>
@@ -3737,7 +3645,7 @@
       <c r="AA220" s="4"/>
       <c r="AB220" s="4"/>
     </row>
-    <row r="221" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="221" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q221"/>
       <c r="T221" s="3"/>
       <c r="U221" s="3"/>
@@ -3749,7 +3657,7 @@
       <c r="AA221" s="4"/>
       <c r="AB221" s="4"/>
     </row>
-    <row r="222" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="222" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q222"/>
       <c r="T222" s="3"/>
       <c r="U222" s="3"/>
@@ -3761,7 +3669,7 @@
       <c r="AA222" s="4"/>
       <c r="AB222" s="4"/>
     </row>
-    <row r="223" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="223" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q223"/>
       <c r="T223" s="3"/>
       <c r="U223" s="3"/>
@@ -3773,7 +3681,7 @@
       <c r="AA223" s="4"/>
       <c r="AB223" s="4"/>
     </row>
-    <row r="224" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="224" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q224"/>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
@@ -3786,7 +3694,9 @@
       <c r="AB224" s="4"/>
     </row>
     <row r="225" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P225" s="3"/>
       <c r="Q225"/>
+      <c r="R225" s="12"/>
       <c r="T225" s="3"/>
       <c r="U225" s="3"/>
       <c r="V225" s="3"/>
@@ -3906,9 +3816,7 @@
       <c r="AB234" s="4"/>
     </row>
     <row r="235" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P235" s="3"/>
       <c r="Q235"/>
-      <c r="R235" s="12"/>
       <c r="T235" s="3"/>
       <c r="U235" s="3"/>
       <c r="V235" s="3"/>
@@ -3993,7 +3901,6 @@
     </row>
     <row r="242" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q242"/>
-      <c r="R242" s="12"/>
       <c r="T242" s="3"/>
       <c r="U242" s="3"/>
       <c r="V242" s="3"/>
@@ -4005,7 +3912,9 @@
       <c r="AB242" s="4"/>
     </row>
     <row r="243" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P243" s="3"/>
       <c r="Q243"/>
+      <c r="R243" s="12"/>
       <c r="T243" s="3"/>
       <c r="U243" s="3"/>
       <c r="V243" s="3"/>
@@ -4090,6 +3999,7 @@
     </row>
     <row r="250" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q250"/>
+      <c r="R250" s="12"/>
       <c r="T250" s="3"/>
       <c r="U250" s="3"/>
       <c r="V250" s="3"/>
@@ -4113,9 +4023,7 @@
       <c r="AB251" s="4"/>
     </row>
     <row r="252" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P252" s="3"/>
       <c r="Q252"/>
-      <c r="R252" s="12"/>
       <c r="T252" s="3"/>
       <c r="U252" s="3"/>
       <c r="V252" s="3"/>
@@ -4211,7 +4119,9 @@
       <c r="AB259" s="4"/>
     </row>
     <row r="260" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P260" s="3"/>
       <c r="Q260"/>
+      <c r="R260" s="12"/>
       <c r="T260" s="3"/>
       <c r="U260" s="3"/>
       <c r="V260" s="3"/>
@@ -4223,9 +4133,7 @@
       <c r="AB260" s="4"/>
     </row>
     <row r="261" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P261" s="3"/>
       <c r="Q261"/>
-      <c r="R261" s="12"/>
       <c r="T261" s="3"/>
       <c r="U261" s="3"/>
       <c r="V261" s="3"/>
@@ -4321,7 +4229,9 @@
       <c r="AB268" s="4"/>
     </row>
     <row r="269" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P269" s="3"/>
       <c r="Q269"/>
+      <c r="R269" s="12"/>
       <c r="T269" s="3"/>
       <c r="U269" s="3"/>
       <c r="V269" s="3"/>
@@ -4334,7 +4244,6 @@
     </row>
     <row r="270" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q270"/>
-      <c r="R270" s="12"/>
       <c r="T270" s="3"/>
       <c r="U270" s="3"/>
       <c r="V270" s="3"/>
@@ -4369,7 +4278,7 @@
       <c r="AA272" s="4"/>
       <c r="AB272" s="4"/>
     </row>
-    <row r="273" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="273" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q273"/>
       <c r="T273" s="3"/>
       <c r="U273" s="3"/>
@@ -4381,7 +4290,7 @@
       <c r="AA273" s="4"/>
       <c r="AB273" s="4"/>
     </row>
-    <row r="274" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="274" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q274"/>
       <c r="T274" s="3"/>
       <c r="U274" s="3"/>
@@ -4393,7 +4302,7 @@
       <c r="AA274" s="4"/>
       <c r="AB274" s="4"/>
     </row>
-    <row r="275" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="275" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q275"/>
       <c r="T275" s="3"/>
       <c r="U275" s="3"/>
@@ -4405,7 +4314,7 @@
       <c r="AA275" s="4"/>
       <c r="AB275" s="4"/>
     </row>
-    <row r="276" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="276" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q276"/>
       <c r="T276" s="3"/>
       <c r="U276" s="3"/>
@@ -4417,7 +4326,7 @@
       <c r="AA276" s="4"/>
       <c r="AB276" s="4"/>
     </row>
-    <row r="277" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="277" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q277"/>
       <c r="T277" s="3"/>
       <c r="U277" s="3"/>
@@ -4429,8 +4338,9 @@
       <c r="AA277" s="4"/>
       <c r="AB277" s="4"/>
     </row>
-    <row r="278" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="278" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q278"/>
+      <c r="R278" s="12"/>
       <c r="T278" s="3"/>
       <c r="U278" s="3"/>
       <c r="V278" s="3"/>
@@ -4441,7 +4351,7 @@
       <c r="AA278" s="4"/>
       <c r="AB278" s="4"/>
     </row>
-    <row r="279" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="279" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q279"/>
       <c r="T279" s="3"/>
       <c r="U279" s="3"/>
@@ -4453,7 +4363,7 @@
       <c r="AA279" s="4"/>
       <c r="AB279" s="4"/>
     </row>
-    <row r="280" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="280" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q280"/>
       <c r="T280" s="3"/>
       <c r="U280" s="3"/>
@@ -4465,10 +4375,8 @@
       <c r="AA280" s="4"/>
       <c r="AB280" s="4"/>
     </row>
-    <row r="281" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P281" s="3"/>
+    <row r="281" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q281"/>
-      <c r="R281" s="12"/>
       <c r="T281" s="3"/>
       <c r="U281" s="3"/>
       <c r="V281" s="3"/>
@@ -4479,7 +4387,7 @@
       <c r="AA281" s="4"/>
       <c r="AB281" s="4"/>
     </row>
-    <row r="282" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="282" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q282"/>
       <c r="T282" s="3"/>
       <c r="U282" s="3"/>
@@ -4491,7 +4399,7 @@
       <c r="AA282" s="4"/>
       <c r="AB282" s="4"/>
     </row>
-    <row r="283" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="283" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q283"/>
       <c r="T283" s="3"/>
       <c r="U283" s="3"/>
@@ -4503,7 +4411,7 @@
       <c r="AA283" s="4"/>
       <c r="AB283" s="4"/>
     </row>
-    <row r="284" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="284" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q284"/>
       <c r="T284" s="3"/>
       <c r="U284" s="3"/>
@@ -4515,7 +4423,7 @@
       <c r="AA284" s="4"/>
       <c r="AB284" s="4"/>
     </row>
-    <row r="285" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="285" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q285"/>
       <c r="T285" s="3"/>
       <c r="U285" s="3"/>
@@ -4527,7 +4435,7 @@
       <c r="AA285" s="4"/>
       <c r="AB285" s="4"/>
     </row>
-    <row r="286" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="286" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q286"/>
       <c r="T286" s="3"/>
       <c r="U286" s="3"/>
@@ -4539,7 +4447,7 @@
       <c r="AA286" s="4"/>
       <c r="AB286" s="4"/>
     </row>
-    <row r="287" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="287" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q287"/>
       <c r="T287" s="3"/>
       <c r="U287" s="3"/>
@@ -4551,7 +4459,7 @@
       <c r="AA287" s="4"/>
       <c r="AB287" s="4"/>
     </row>
-    <row r="288" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="288" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q288"/>
       <c r="T288" s="3"/>
       <c r="U288" s="3"/>
@@ -4564,7 +4472,9 @@
       <c r="AB288" s="4"/>
     </row>
     <row r="289" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P289" s="3"/>
       <c r="Q289"/>
+      <c r="R289" s="12"/>
       <c r="T289" s="3"/>
       <c r="U289" s="3"/>
       <c r="V289" s="3"/>
@@ -4708,9 +4618,7 @@
       <c r="AB300" s="4"/>
     </row>
     <row r="301" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P301" s="3"/>
       <c r="Q301"/>
-      <c r="R301" s="12"/>
       <c r="T301" s="3"/>
       <c r="U301" s="3"/>
       <c r="V301" s="3"/>
@@ -4806,7 +4714,9 @@
       <c r="AB308" s="4"/>
     </row>
     <row r="309" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P309" s="3"/>
       <c r="Q309"/>
+      <c r="R309" s="12"/>
       <c r="T309" s="3"/>
       <c r="U309" s="3"/>
       <c r="V309" s="3"/>
@@ -4830,9 +4740,7 @@
       <c r="AB310" s="4"/>
     </row>
     <row r="311" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P311" s="3"/>
       <c r="Q311"/>
-      <c r="R311" s="12"/>
       <c r="T311" s="3"/>
       <c r="U311" s="3"/>
       <c r="V311" s="3"/>
@@ -4928,7 +4836,9 @@
       <c r="AB318" s="4"/>
     </row>
     <row r="319" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P319" s="3"/>
       <c r="Q319"/>
+      <c r="R319" s="12"/>
       <c r="T319" s="3"/>
       <c r="U319" s="3"/>
       <c r="V319" s="3"/>
@@ -5061,7 +4971,6 @@
     </row>
     <row r="330" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q330"/>
-      <c r="R330" s="12"/>
       <c r="T330" s="3"/>
       <c r="U330" s="3"/>
       <c r="V330" s="3"/>
@@ -5144,9 +5053,8 @@
       <c r="AA336" s="4"/>
       <c r="AB336" s="4"/>
     </row>
-    <row r="337" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="337" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q337"/>
-      <c r="R337" s="12"/>
       <c r="T337" s="3"/>
       <c r="U337" s="3"/>
       <c r="V337" s="3"/>
@@ -5157,8 +5065,9 @@
       <c r="AA337" s="4"/>
       <c r="AB337" s="4"/>
     </row>
-    <row r="338" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="338" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q338"/>
+      <c r="R338" s="12"/>
       <c r="T338" s="3"/>
       <c r="U338" s="3"/>
       <c r="V338" s="3"/>
@@ -5169,7 +5078,7 @@
       <c r="AA338" s="4"/>
       <c r="AB338" s="4"/>
     </row>
-    <row r="339" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="339" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q339"/>
       <c r="T339" s="3"/>
       <c r="U339" s="3"/>
@@ -5181,7 +5090,7 @@
       <c r="AA339" s="4"/>
       <c r="AB339" s="4"/>
     </row>
-    <row r="340" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="340" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q340"/>
       <c r="T340" s="3"/>
       <c r="U340" s="3"/>
@@ -5193,7 +5102,7 @@
       <c r="AA340" s="4"/>
       <c r="AB340" s="4"/>
     </row>
-    <row r="341" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="341" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q341"/>
       <c r="T341" s="3"/>
       <c r="U341" s="3"/>
@@ -5205,7 +5114,7 @@
       <c r="AA341" s="4"/>
       <c r="AB341" s="4"/>
     </row>
-    <row r="342" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="342" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q342"/>
       <c r="T342" s="3"/>
       <c r="U342" s="3"/>
@@ -5217,7 +5126,7 @@
       <c r="AA342" s="4"/>
       <c r="AB342" s="4"/>
     </row>
-    <row r="343" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="343" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q343"/>
       <c r="T343" s="3"/>
       <c r="U343" s="3"/>
@@ -5229,7 +5138,7 @@
       <c r="AA343" s="4"/>
       <c r="AB343" s="4"/>
     </row>
-    <row r="344" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="344" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q344"/>
       <c r="T344" s="3"/>
       <c r="U344" s="3"/>
@@ -5241,8 +5150,7 @@
       <c r="AA344" s="4"/>
       <c r="AB344" s="4"/>
     </row>
-    <row r="345" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P345" s="3"/>
+    <row r="345" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q345"/>
       <c r="R345" s="12"/>
       <c r="T345" s="3"/>
@@ -5255,7 +5163,7 @@
       <c r="AA345" s="4"/>
       <c r="AB345" s="4"/>
     </row>
-    <row r="346" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="346" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q346"/>
       <c r="T346" s="3"/>
       <c r="U346" s="3"/>
@@ -5267,7 +5175,7 @@
       <c r="AA346" s="4"/>
       <c r="AB346" s="4"/>
     </row>
-    <row r="347" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="347" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q347"/>
       <c r="T347" s="3"/>
       <c r="U347" s="3"/>
@@ -5279,7 +5187,7 @@
       <c r="AA347" s="4"/>
       <c r="AB347" s="4"/>
     </row>
-    <row r="348" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="348" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q348"/>
       <c r="T348" s="3"/>
       <c r="U348" s="3"/>
@@ -5291,7 +5199,7 @@
       <c r="AA348" s="4"/>
       <c r="AB348" s="4"/>
     </row>
-    <row r="349" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="349" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q349"/>
       <c r="T349" s="3"/>
       <c r="U349" s="3"/>
@@ -5303,7 +5211,7 @@
       <c r="AA349" s="4"/>
       <c r="AB349" s="4"/>
     </row>
-    <row r="350" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="350" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q350"/>
       <c r="T350" s="3"/>
       <c r="U350" s="3"/>
@@ -5315,9 +5223,8 @@
       <c r="AA350" s="4"/>
       <c r="AB350" s="4"/>
     </row>
-    <row r="351" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="351" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q351"/>
-      <c r="R351" s="12"/>
       <c r="T351" s="3"/>
       <c r="U351" s="3"/>
       <c r="V351" s="3"/>
@@ -5328,7 +5235,7 @@
       <c r="AA351" s="4"/>
       <c r="AB351" s="4"/>
     </row>
-    <row r="352" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="352" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q352"/>
       <c r="T352" s="3"/>
       <c r="U352" s="3"/>
@@ -5341,7 +5248,9 @@
       <c r="AB352" s="4"/>
     </row>
     <row r="353" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P353" s="3"/>
       <c r="Q353"/>
+      <c r="R353" s="12"/>
       <c r="T353" s="3"/>
       <c r="U353" s="3"/>
       <c r="V353" s="3"/>
@@ -5377,9 +5286,7 @@
       <c r="AB355" s="4"/>
     </row>
     <row r="356" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P356" s="3"/>
       <c r="Q356"/>
-      <c r="R356" s="12"/>
       <c r="T356" s="3"/>
       <c r="U356" s="3"/>
       <c r="V356" s="3"/>
@@ -5416,6 +5323,7 @@
     </row>
     <row r="359" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q359"/>
+      <c r="R359" s="12"/>
       <c r="T359" s="3"/>
       <c r="U359" s="3"/>
       <c r="V359" s="3"/>
@@ -5475,7 +5383,9 @@
       <c r="AB363" s="4"/>
     </row>
     <row r="364" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P364" s="3"/>
       <c r="Q364"/>
+      <c r="R364" s="12"/>
       <c r="T364" s="3"/>
       <c r="U364" s="3"/>
       <c r="V364" s="3"/>
@@ -5499,9 +5409,7 @@
       <c r="AB365" s="4"/>
     </row>
     <row r="366" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P366" s="3"/>
       <c r="Q366"/>
-      <c r="R366" s="12"/>
       <c r="T366" s="3"/>
       <c r="U366" s="3"/>
       <c r="V366" s="3"/>
@@ -5536,7 +5444,7 @@
       <c r="AA368" s="4"/>
       <c r="AB368" s="4"/>
     </row>
-    <row r="369" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="369" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q369"/>
       <c r="T369" s="3"/>
       <c r="U369" s="3"/>
@@ -5548,7 +5456,7 @@
       <c r="AA369" s="4"/>
       <c r="AB369" s="4"/>
     </row>
-    <row r="370" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="370" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q370"/>
       <c r="T370" s="3"/>
       <c r="U370" s="3"/>
@@ -5560,7 +5468,7 @@
       <c r="AA370" s="4"/>
       <c r="AB370" s="4"/>
     </row>
-    <row r="371" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="371" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q371"/>
       <c r="T371" s="3"/>
       <c r="U371" s="3"/>
@@ -5572,7 +5480,7 @@
       <c r="AA371" s="4"/>
       <c r="AB371" s="4"/>
     </row>
-    <row r="372" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="372" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q372"/>
       <c r="T372" s="3"/>
       <c r="U372" s="3"/>
@@ -5584,7 +5492,7 @@
       <c r="AA372" s="4"/>
       <c r="AB372" s="4"/>
     </row>
-    <row r="373" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="373" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q373"/>
       <c r="T373" s="3"/>
       <c r="U373" s="3"/>
@@ -5596,8 +5504,10 @@
       <c r="AA373" s="4"/>
       <c r="AB373" s="4"/>
     </row>
-    <row r="374" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="374" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P374" s="3"/>
       <c r="Q374"/>
+      <c r="R374" s="12"/>
       <c r="T374" s="3"/>
       <c r="U374" s="3"/>
       <c r="V374" s="3"/>
@@ -5608,7 +5518,7 @@
       <c r="AA374" s="4"/>
       <c r="AB374" s="4"/>
     </row>
-    <row r="375" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="375" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q375"/>
       <c r="T375" s="3"/>
       <c r="U375" s="3"/>
@@ -5620,7 +5530,7 @@
       <c r="AA375" s="4"/>
       <c r="AB375" s="4"/>
     </row>
-    <row r="376" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="376" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q376"/>
       <c r="T376" s="3"/>
       <c r="U376" s="3"/>
@@ -5632,7 +5542,7 @@
       <c r="AA376" s="4"/>
       <c r="AB376" s="4"/>
     </row>
-    <row r="377" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="377" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q377"/>
       <c r="T377" s="3"/>
       <c r="U377" s="3"/>
@@ -5644,7 +5554,7 @@
       <c r="AA377" s="4"/>
       <c r="AB377" s="4"/>
     </row>
-    <row r="378" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="378" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q378"/>
       <c r="T378" s="3"/>
       <c r="U378" s="3"/>
@@ -5656,7 +5566,7 @@
       <c r="AA378" s="4"/>
       <c r="AB378" s="4"/>
     </row>
-    <row r="379" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="379" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q379"/>
       <c r="T379" s="3"/>
       <c r="U379" s="3"/>
@@ -5668,7 +5578,7 @@
       <c r="AA379" s="4"/>
       <c r="AB379" s="4"/>
     </row>
-    <row r="380" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="380" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q380"/>
       <c r="T380" s="3"/>
       <c r="U380" s="3"/>
@@ -5680,7 +5590,7 @@
       <c r="AA380" s="4"/>
       <c r="AB380" s="4"/>
     </row>
-    <row r="381" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="381" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q381"/>
       <c r="T381" s="3"/>
       <c r="U381" s="3"/>
@@ -5692,7 +5602,7 @@
       <c r="AA381" s="4"/>
       <c r="AB381" s="4"/>
     </row>
-    <row r="382" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="382" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q382"/>
       <c r="T382" s="3"/>
       <c r="U382" s="3"/>
@@ -5704,7 +5614,7 @@
       <c r="AA382" s="4"/>
       <c r="AB382" s="4"/>
     </row>
-    <row r="383" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="383" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q383"/>
       <c r="T383" s="3"/>
       <c r="U383" s="3"/>
@@ -5716,7 +5626,7 @@
       <c r="AA383" s="4"/>
       <c r="AB383" s="4"/>
     </row>
-    <row r="384" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="384" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q384"/>
       <c r="T384" s="3"/>
       <c r="U384" s="3"/>
@@ -5729,9 +5639,7 @@
       <c r="AB384" s="4"/>
     </row>
     <row r="385" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P385" s="3"/>
       <c r="Q385"/>
-      <c r="R385" s="12"/>
       <c r="T385" s="3"/>
       <c r="U385" s="3"/>
       <c r="V385" s="3"/>
@@ -5827,7 +5735,9 @@
       <c r="AB392" s="4"/>
     </row>
     <row r="393" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P393" s="3"/>
       <c r="Q393"/>
+      <c r="R393" s="12"/>
       <c r="T393" s="3"/>
       <c r="U393" s="3"/>
       <c r="V393" s="3"/>
@@ -5983,9 +5893,7 @@
       <c r="AB405" s="4"/>
     </row>
     <row r="406" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P406" s="3"/>
       <c r="Q406"/>
-      <c r="R406" s="12"/>
       <c r="T406" s="3"/>
       <c r="U406" s="3"/>
       <c r="V406" s="3"/>
@@ -6081,7 +5989,9 @@
       <c r="AB413" s="4"/>
     </row>
     <row r="414" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P414" s="3"/>
       <c r="Q414"/>
+      <c r="R414" s="12"/>
       <c r="T414" s="3"/>
       <c r="U414" s="3"/>
       <c r="V414" s="3"/>
@@ -6238,7 +6148,6 @@
     </row>
     <row r="427" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q427"/>
-      <c r="R427" s="12"/>
       <c r="T427" s="3"/>
       <c r="U427" s="3"/>
       <c r="V427" s="3"/>
@@ -6309,7 +6218,7 @@
       <c r="AA432" s="4"/>
       <c r="AB432" s="4"/>
     </row>
-    <row r="433" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="433" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q433"/>
       <c r="T433" s="3"/>
       <c r="U433" s="3"/>
@@ -6321,7 +6230,7 @@
       <c r="AA433" s="4"/>
       <c r="AB433" s="4"/>
     </row>
-    <row r="434" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="434" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q434"/>
       <c r="T434" s="3"/>
       <c r="U434" s="3"/>
@@ -6333,8 +6242,9 @@
       <c r="AA434" s="4"/>
       <c r="AB434" s="4"/>
     </row>
-    <row r="435" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="435" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q435"/>
+      <c r="R435" s="12"/>
       <c r="T435" s="3"/>
       <c r="U435" s="3"/>
       <c r="V435" s="3"/>
@@ -6345,7 +6255,7 @@
       <c r="AA435" s="4"/>
       <c r="AB435" s="4"/>
     </row>
-    <row r="436" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="436" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q436"/>
       <c r="T436" s="3"/>
       <c r="U436" s="3"/>
@@ -6357,7 +6267,7 @@
       <c r="AA436" s="4"/>
       <c r="AB436" s="4"/>
     </row>
-    <row r="437" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="437" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q437"/>
       <c r="T437" s="3"/>
       <c r="U437" s="3"/>
@@ -6369,7 +6279,7 @@
       <c r="AA437" s="4"/>
       <c r="AB437" s="4"/>
     </row>
-    <row r="438" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="438" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q438"/>
       <c r="T438" s="3"/>
       <c r="U438" s="3"/>
@@ -6381,7 +6291,7 @@
       <c r="AA438" s="4"/>
       <c r="AB438" s="4"/>
     </row>
-    <row r="439" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="439" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q439"/>
       <c r="T439" s="3"/>
       <c r="U439" s="3"/>
@@ -6393,7 +6303,7 @@
       <c r="AA439" s="4"/>
       <c r="AB439" s="4"/>
     </row>
-    <row r="440" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="440" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q440"/>
       <c r="T440" s="3"/>
       <c r="U440" s="3"/>
@@ -6405,7 +6315,7 @@
       <c r="AA440" s="4"/>
       <c r="AB440" s="4"/>
     </row>
-    <row r="441" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="441" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q441"/>
       <c r="T441" s="3"/>
       <c r="U441" s="3"/>
@@ -6417,7 +6327,7 @@
       <c r="AA441" s="4"/>
       <c r="AB441" s="4"/>
     </row>
-    <row r="442" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="442" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q442"/>
       <c r="T442" s="3"/>
       <c r="U442" s="3"/>
@@ -6429,7 +6339,7 @@
       <c r="AA442" s="4"/>
       <c r="AB442" s="4"/>
     </row>
-    <row r="443" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="443" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q443"/>
       <c r="T443" s="3"/>
       <c r="U443" s="3"/>
@@ -6441,7 +6351,7 @@
       <c r="AA443" s="4"/>
       <c r="AB443" s="4"/>
     </row>
-    <row r="444" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="444" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q444"/>
       <c r="T444" s="3"/>
       <c r="U444" s="3"/>
@@ -6453,7 +6363,7 @@
       <c r="AA444" s="4"/>
       <c r="AB444" s="4"/>
     </row>
-    <row r="445" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="445" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q445"/>
       <c r="T445" s="3"/>
       <c r="U445" s="3"/>
@@ -6465,10 +6375,8 @@
       <c r="AA445" s="4"/>
       <c r="AB445" s="4"/>
     </row>
-    <row r="446" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P446" s="3"/>
+    <row r="446" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q446"/>
-      <c r="R446" s="12"/>
       <c r="T446" s="3"/>
       <c r="U446" s="3"/>
       <c r="V446" s="3"/>
@@ -6479,7 +6387,7 @@
       <c r="AA446" s="4"/>
       <c r="AB446" s="4"/>
     </row>
-    <row r="447" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="447" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q447"/>
       <c r="T447" s="3"/>
       <c r="U447" s="3"/>
@@ -6491,7 +6399,7 @@
       <c r="AA447" s="4"/>
       <c r="AB447" s="4"/>
     </row>
-    <row r="448" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="448" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q448"/>
       <c r="T448" s="3"/>
       <c r="U448" s="3"/>
@@ -6503,7 +6411,7 @@
       <c r="AA448" s="4"/>
       <c r="AB448" s="4"/>
     </row>
-    <row r="449" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="449" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q449"/>
       <c r="T449" s="3"/>
       <c r="U449" s="3"/>
@@ -6515,7 +6423,7 @@
       <c r="AA449" s="4"/>
       <c r="AB449" s="4"/>
     </row>
-    <row r="450" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="450" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q450"/>
       <c r="T450" s="3"/>
       <c r="U450" s="3"/>
@@ -6527,7 +6435,7 @@
       <c r="AA450" s="4"/>
       <c r="AB450" s="4"/>
     </row>
-    <row r="451" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="451" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q451"/>
       <c r="T451" s="3"/>
       <c r="U451" s="3"/>
@@ -6539,7 +6447,7 @@
       <c r="AA451" s="4"/>
       <c r="AB451" s="4"/>
     </row>
-    <row r="452" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="452" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q452"/>
       <c r="T452" s="3"/>
       <c r="U452" s="3"/>
@@ -6551,7 +6459,7 @@
       <c r="AA452" s="4"/>
       <c r="AB452" s="4"/>
     </row>
-    <row r="453" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="453" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q453"/>
       <c r="T453" s="3"/>
       <c r="U453" s="3"/>
@@ -6563,8 +6471,10 @@
       <c r="AA453" s="4"/>
       <c r="AB453" s="4"/>
     </row>
-    <row r="454" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="454" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P454" s="3"/>
       <c r="Q454"/>
+      <c r="R454" s="12"/>
       <c r="T454" s="3"/>
       <c r="U454" s="3"/>
       <c r="V454" s="3"/>
@@ -6575,7 +6485,7 @@
       <c r="AA454" s="4"/>
       <c r="AB454" s="4"/>
     </row>
-    <row r="455" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="455" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q455"/>
       <c r="T455" s="3"/>
       <c r="U455" s="3"/>
@@ -6587,7 +6497,7 @@
       <c r="AA455" s="4"/>
       <c r="AB455" s="4"/>
     </row>
-    <row r="456" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="456" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q456"/>
       <c r="T456" s="3"/>
       <c r="U456" s="3"/>
@@ -6599,7 +6509,7 @@
       <c r="AA456" s="4"/>
       <c r="AB456" s="4"/>
     </row>
-    <row r="457" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="457" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q457"/>
       <c r="T457" s="3"/>
       <c r="U457" s="3"/>
@@ -6611,7 +6521,7 @@
       <c r="AA457" s="4"/>
       <c r="AB457" s="4"/>
     </row>
-    <row r="458" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="458" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q458"/>
       <c r="T458" s="3"/>
       <c r="U458" s="3"/>
@@ -6623,7 +6533,7 @@
       <c r="AA458" s="4"/>
       <c r="AB458" s="4"/>
     </row>
-    <row r="459" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="459" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q459"/>
       <c r="T459" s="3"/>
       <c r="U459" s="3"/>
@@ -6635,7 +6545,7 @@
       <c r="AA459" s="4"/>
       <c r="AB459" s="4"/>
     </row>
-    <row r="460" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="460" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q460"/>
       <c r="T460" s="3"/>
       <c r="U460" s="3"/>
@@ -6647,7 +6557,7 @@
       <c r="AA460" s="4"/>
       <c r="AB460" s="4"/>
     </row>
-    <row r="461" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="461" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q461"/>
       <c r="T461" s="3"/>
       <c r="U461" s="3"/>
@@ -6659,7 +6569,7 @@
       <c r="AA461" s="4"/>
       <c r="AB461" s="4"/>
     </row>
-    <row r="462" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="462" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q462"/>
       <c r="T462" s="3"/>
       <c r="U462" s="3"/>
@@ -6671,7 +6581,7 @@
       <c r="AA462" s="4"/>
       <c r="AB462" s="4"/>
     </row>
-    <row r="463" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="463" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q463"/>
       <c r="T463" s="3"/>
       <c r="U463" s="3"/>
@@ -6683,7 +6593,7 @@
       <c r="AA463" s="4"/>
       <c r="AB463" s="4"/>
     </row>
-    <row r="464" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="464" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q464"/>
       <c r="T464" s="3"/>
       <c r="U464" s="3"/>
@@ -6756,9 +6666,7 @@
       <c r="AB469" s="4"/>
     </row>
     <row r="470" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P470" s="3"/>
       <c r="Q470"/>
-      <c r="R470" s="12"/>
       <c r="T470" s="3"/>
       <c r="U470" s="3"/>
       <c r="V470" s="3"/>
@@ -6854,7 +6762,9 @@
       <c r="AB477" s="4"/>
     </row>
     <row r="478" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P478" s="3"/>
       <c r="Q478"/>
+      <c r="R478" s="12"/>
       <c r="T478" s="3"/>
       <c r="U478" s="3"/>
       <c r="V478" s="3"/>
@@ -6889,7 +6799,7 @@
       <c r="AA480" s="4"/>
       <c r="AB480" s="4"/>
     </row>
-    <row r="481" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="481" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q481"/>
       <c r="T481" s="3"/>
       <c r="U481" s="3"/>
@@ -6901,7 +6811,7 @@
       <c r="AA481" s="4"/>
       <c r="AB481" s="4"/>
     </row>
-    <row r="482" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="482" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q482"/>
       <c r="T482" s="3"/>
       <c r="U482" s="3"/>
@@ -6913,7 +6823,7 @@
       <c r="AA482" s="4"/>
       <c r="AB482" s="4"/>
     </row>
-    <row r="483" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="483" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q483"/>
       <c r="T483" s="3"/>
       <c r="U483" s="3"/>
@@ -6925,7 +6835,7 @@
       <c r="AA483" s="4"/>
       <c r="AB483" s="4"/>
     </row>
-    <row r="484" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="484" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q484"/>
       <c r="T484" s="3"/>
       <c r="U484" s="3"/>
@@ -6937,7 +6847,7 @@
       <c r="AA484" s="4"/>
       <c r="AB484" s="4"/>
     </row>
-    <row r="485" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="485" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q485"/>
       <c r="T485" s="3"/>
       <c r="U485" s="3"/>
@@ -6949,7 +6859,7 @@
       <c r="AA485" s="4"/>
       <c r="AB485" s="4"/>
     </row>
-    <row r="486" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="486" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q486"/>
       <c r="T486" s="3"/>
       <c r="U486" s="3"/>
@@ -6961,7 +6871,7 @@
       <c r="AA486" s="4"/>
       <c r="AB486" s="4"/>
     </row>
-    <row r="487" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="487" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q487"/>
       <c r="T487" s="3"/>
       <c r="U487" s="3"/>
@@ -6973,7 +6883,7 @@
       <c r="AA487" s="4"/>
       <c r="AB487" s="4"/>
     </row>
-    <row r="488" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="488" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q488"/>
       <c r="T488" s="3"/>
       <c r="U488" s="3"/>
@@ -6985,10 +6895,8 @@
       <c r="AA488" s="4"/>
       <c r="AB488" s="4"/>
     </row>
-    <row r="489" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P489" s="3"/>
+    <row r="489" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q489"/>
-      <c r="R489" s="12"/>
       <c r="T489" s="3"/>
       <c r="U489" s="3"/>
       <c r="V489" s="3"/>
@@ -6999,7 +6907,7 @@
       <c r="AA489" s="4"/>
       <c r="AB489" s="4"/>
     </row>
-    <row r="490" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="490" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q490"/>
       <c r="T490" s="3"/>
       <c r="U490" s="3"/>
@@ -7011,7 +6919,7 @@
       <c r="AA490" s="4"/>
       <c r="AB490" s="4"/>
     </row>
-    <row r="491" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="491" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q491"/>
       <c r="T491" s="3"/>
       <c r="U491" s="3"/>
@@ -7023,7 +6931,7 @@
       <c r="AA491" s="4"/>
       <c r="AB491" s="4"/>
     </row>
-    <row r="492" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="492" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q492"/>
       <c r="T492" s="3"/>
       <c r="U492" s="3"/>
@@ -7035,7 +6943,7 @@
       <c r="AA492" s="4"/>
       <c r="AB492" s="4"/>
     </row>
-    <row r="493" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="493" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q493"/>
       <c r="T493" s="3"/>
       <c r="U493" s="3"/>
@@ -7047,7 +6955,7 @@
       <c r="AA493" s="4"/>
       <c r="AB493" s="4"/>
     </row>
-    <row r="494" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="494" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q494"/>
       <c r="T494" s="3"/>
       <c r="U494" s="3"/>
@@ -7059,10 +6967,8 @@
       <c r="AA494" s="4"/>
       <c r="AB494" s="4"/>
     </row>
-    <row r="495" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P495" s="3"/>
+    <row r="495" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q495"/>
-      <c r="R495" s="12"/>
       <c r="T495" s="3"/>
       <c r="U495" s="3"/>
       <c r="V495" s="3"/>
@@ -7073,7 +6979,7 @@
       <c r="AA495" s="4"/>
       <c r="AB495" s="4"/>
     </row>
-    <row r="496" spans="16:28" x14ac:dyDescent="0.2">
+    <row r="496" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q496"/>
       <c r="T496" s="3"/>
       <c r="U496" s="3"/>
@@ -7085,8 +6991,10 @@
       <c r="AA496" s="4"/>
       <c r="AB496" s="4"/>
     </row>
-    <row r="497" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="497" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P497" s="3"/>
       <c r="Q497"/>
+      <c r="R497" s="12"/>
       <c r="T497" s="3"/>
       <c r="U497" s="3"/>
       <c r="V497" s="3"/>
@@ -7097,7 +7005,7 @@
       <c r="AA497" s="4"/>
       <c r="AB497" s="4"/>
     </row>
-    <row r="498" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="498" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q498"/>
       <c r="T498" s="3"/>
       <c r="U498" s="3"/>
@@ -7109,7 +7017,7 @@
       <c r="AA498" s="4"/>
       <c r="AB498" s="4"/>
     </row>
-    <row r="499" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="499" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q499"/>
       <c r="T499" s="3"/>
       <c r="U499" s="3"/>
@@ -7121,7 +7029,7 @@
       <c r="AA499" s="4"/>
       <c r="AB499" s="4"/>
     </row>
-    <row r="500" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="500" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q500"/>
       <c r="T500" s="3"/>
       <c r="U500" s="3"/>
@@ -7133,7 +7041,7 @@
       <c r="AA500" s="4"/>
       <c r="AB500" s="4"/>
     </row>
-    <row r="501" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="501" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q501"/>
       <c r="T501" s="3"/>
       <c r="U501" s="3"/>
@@ -7145,7 +7053,7 @@
       <c r="AA501" s="4"/>
       <c r="AB501" s="4"/>
     </row>
-    <row r="502" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="502" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q502"/>
       <c r="T502" s="3"/>
       <c r="U502" s="3"/>
@@ -7157,8 +7065,10 @@
       <c r="AA502" s="4"/>
       <c r="AB502" s="4"/>
     </row>
-    <row r="503" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="503" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P503" s="3"/>
       <c r="Q503"/>
+      <c r="R503" s="12"/>
       <c r="T503" s="3"/>
       <c r="U503" s="3"/>
       <c r="V503" s="3"/>
@@ -7169,7 +7079,7 @@
       <c r="AA503" s="4"/>
       <c r="AB503" s="4"/>
     </row>
-    <row r="504" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="504" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q504"/>
       <c r="T504" s="3"/>
       <c r="U504" s="3"/>
@@ -7181,7 +7091,7 @@
       <c r="AA504" s="4"/>
       <c r="AB504" s="4"/>
     </row>
-    <row r="505" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="505" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q505"/>
       <c r="T505" s="3"/>
       <c r="U505" s="3"/>
@@ -7193,7 +7103,7 @@
       <c r="AA505" s="4"/>
       <c r="AB505" s="4"/>
     </row>
-    <row r="506" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="506" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q506"/>
       <c r="T506" s="3"/>
       <c r="U506" s="3"/>
@@ -7205,7 +7115,7 @@
       <c r="AA506" s="4"/>
       <c r="AB506" s="4"/>
     </row>
-    <row r="507" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="507" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q507"/>
       <c r="T507" s="3"/>
       <c r="U507" s="3"/>
@@ -7217,9 +7127,8 @@
       <c r="AA507" s="4"/>
       <c r="AB507" s="4"/>
     </row>
-    <row r="508" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="508" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q508"/>
-      <c r="R508" s="12"/>
       <c r="T508" s="3"/>
       <c r="U508" s="3"/>
       <c r="V508" s="3"/>
@@ -7230,7 +7139,7 @@
       <c r="AA508" s="4"/>
       <c r="AB508" s="4"/>
     </row>
-    <row r="509" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="509" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q509"/>
       <c r="T509" s="3"/>
       <c r="U509" s="3"/>
@@ -7242,7 +7151,7 @@
       <c r="AA509" s="4"/>
       <c r="AB509" s="4"/>
     </row>
-    <row r="510" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="510" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q510"/>
       <c r="T510" s="3"/>
       <c r="U510" s="3"/>
@@ -7254,7 +7163,7 @@
       <c r="AA510" s="4"/>
       <c r="AB510" s="4"/>
     </row>
-    <row r="511" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="511" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q511"/>
       <c r="T511" s="3"/>
       <c r="U511" s="3"/>
@@ -7266,7 +7175,7 @@
       <c r="AA511" s="4"/>
       <c r="AB511" s="4"/>
     </row>
-    <row r="512" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="512" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q512"/>
       <c r="T512" s="3"/>
       <c r="U512" s="3"/>
@@ -7316,6 +7225,7 @@
     </row>
     <row r="516" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q516"/>
+      <c r="R516" s="12"/>
       <c r="T516" s="3"/>
       <c r="U516" s="3"/>
       <c r="V516" s="3"/>
@@ -7351,9 +7261,7 @@
       <c r="AB518" s="4"/>
     </row>
     <row r="519" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P519" s="3"/>
       <c r="Q519"/>
-      <c r="R519" s="12"/>
       <c r="T519" s="3"/>
       <c r="U519" s="3"/>
       <c r="V519" s="3"/>
@@ -7449,7 +7357,9 @@
       <c r="AB526" s="4"/>
     </row>
     <row r="527" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P527" s="3"/>
       <c r="Q527"/>
+      <c r="R527" s="12"/>
       <c r="T527" s="3"/>
       <c r="U527" s="3"/>
       <c r="V527" s="3"/>
@@ -7497,9 +7407,7 @@
       <c r="AB530" s="4"/>
     </row>
     <row r="531" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P531" s="3"/>
       <c r="Q531"/>
-      <c r="R531" s="12"/>
       <c r="T531" s="3"/>
       <c r="U531" s="3"/>
       <c r="V531" s="3"/>
@@ -7693,7 +7601,9 @@
       <c r="AB546" s="4"/>
     </row>
     <row r="547" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P547" s="3"/>
       <c r="Q547"/>
+      <c r="R547" s="12"/>
       <c r="T547" s="3"/>
       <c r="U547" s="3"/>
       <c r="V547" s="3"/>
@@ -7801,9 +7711,7 @@
       <c r="AB555" s="4"/>
     </row>
     <row r="556" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P556" s="3"/>
       <c r="Q556"/>
-      <c r="R556" s="12"/>
       <c r="T556" s="3"/>
       <c r="U556" s="3"/>
       <c r="V556" s="3"/>
@@ -7899,7 +7807,9 @@
       <c r="AB563" s="4"/>
     </row>
     <row r="564" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P564" s="3"/>
       <c r="Q564"/>
+      <c r="R564" s="12"/>
       <c r="T564" s="3"/>
       <c r="U564" s="3"/>
       <c r="V564" s="3"/>
@@ -7924,7 +7834,6 @@
     </row>
     <row r="566" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q566"/>
-      <c r="R566" s="12"/>
       <c r="T566" s="3"/>
       <c r="U566" s="3"/>
       <c r="V566" s="3"/>
@@ -7984,9 +7893,7 @@
       <c r="AB570" s="4"/>
     </row>
     <row r="571" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P571" s="3"/>
       <c r="Q571"/>
-      <c r="R571" s="12"/>
       <c r="T571" s="3"/>
       <c r="U571" s="3"/>
       <c r="V571" s="3"/>
@@ -8023,6 +7930,7 @@
     </row>
     <row r="574" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q574"/>
+      <c r="R574" s="12"/>
       <c r="T574" s="3"/>
       <c r="U574" s="3"/>
       <c r="V574" s="3"/>
@@ -8057,7 +7965,7 @@
       <c r="AA576" s="4"/>
       <c r="AB576" s="4"/>
     </row>
-    <row r="577" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="577" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q577"/>
       <c r="T577" s="3"/>
       <c r="U577" s="3"/>
@@ -8069,7 +7977,7 @@
       <c r="AA577" s="4"/>
       <c r="AB577" s="4"/>
     </row>
-    <row r="578" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="578" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q578"/>
       <c r="T578" s="3"/>
       <c r="U578" s="3"/>
@@ -8081,8 +7989,10 @@
       <c r="AA578" s="4"/>
       <c r="AB578" s="4"/>
     </row>
-    <row r="579" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="579" spans="16:28" x14ac:dyDescent="0.2">
+      <c r="P579" s="3"/>
       <c r="Q579"/>
+      <c r="R579" s="12"/>
       <c r="T579" s="3"/>
       <c r="U579" s="3"/>
       <c r="V579" s="3"/>
@@ -8093,7 +8003,7 @@
       <c r="AA579" s="4"/>
       <c r="AB579" s="4"/>
     </row>
-    <row r="580" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="580" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q580"/>
       <c r="T580" s="3"/>
       <c r="U580" s="3"/>
@@ -8105,7 +8015,7 @@
       <c r="AA580" s="4"/>
       <c r="AB580" s="4"/>
     </row>
-    <row r="581" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="581" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q581"/>
       <c r="T581" s="3"/>
       <c r="U581" s="3"/>
@@ -8117,7 +8027,7 @@
       <c r="AA581" s="4"/>
       <c r="AB581" s="4"/>
     </row>
-    <row r="582" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="582" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q582"/>
       <c r="T582" s="3"/>
       <c r="U582" s="3"/>
@@ -8129,7 +8039,7 @@
       <c r="AA582" s="4"/>
       <c r="AB582" s="4"/>
     </row>
-    <row r="583" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="583" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q583"/>
       <c r="T583" s="3"/>
       <c r="U583" s="3"/>
@@ -8141,7 +8051,7 @@
       <c r="AA583" s="4"/>
       <c r="AB583" s="4"/>
     </row>
-    <row r="584" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="584" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q584"/>
       <c r="T584" s="3"/>
       <c r="U584" s="3"/>
@@ -8153,7 +8063,7 @@
       <c r="AA584" s="4"/>
       <c r="AB584" s="4"/>
     </row>
-    <row r="585" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="585" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q585"/>
       <c r="T585" s="3"/>
       <c r="U585" s="3"/>
@@ -8165,7 +8075,7 @@
       <c r="AA585" s="4"/>
       <c r="AB585" s="4"/>
     </row>
-    <row r="586" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="586" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q586"/>
       <c r="T586" s="3"/>
       <c r="U586" s="3"/>
@@ -8177,7 +8087,7 @@
       <c r="AA586" s="4"/>
       <c r="AB586" s="4"/>
     </row>
-    <row r="587" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="587" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q587"/>
       <c r="T587" s="3"/>
       <c r="U587" s="3"/>
@@ -8189,7 +8099,7 @@
       <c r="AA587" s="4"/>
       <c r="AB587" s="4"/>
     </row>
-    <row r="588" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="588" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q588"/>
       <c r="T588" s="3"/>
       <c r="U588" s="3"/>
@@ -8201,7 +8111,7 @@
       <c r="AA588" s="4"/>
       <c r="AB588" s="4"/>
     </row>
-    <row r="589" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="589" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q589"/>
       <c r="T589" s="3"/>
       <c r="U589" s="3"/>
@@ -8213,7 +8123,7 @@
       <c r="AA589" s="4"/>
       <c r="AB589" s="4"/>
     </row>
-    <row r="590" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="590" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q590"/>
       <c r="T590" s="3"/>
       <c r="U590" s="3"/>
@@ -8225,7 +8135,7 @@
       <c r="AA590" s="4"/>
       <c r="AB590" s="4"/>
     </row>
-    <row r="591" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="591" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q591"/>
       <c r="T591" s="3"/>
       <c r="U591" s="3"/>
@@ -8237,7 +8147,7 @@
       <c r="AA591" s="4"/>
       <c r="AB591" s="4"/>
     </row>
-    <row r="592" spans="17:28" x14ac:dyDescent="0.2">
+    <row r="592" spans="16:28" x14ac:dyDescent="0.2">
       <c r="Q592"/>
       <c r="T592" s="3"/>
       <c r="U592" s="3"/>
@@ -8322,36 +8232,100 @@
       <c r="AB598" s="4"/>
     </row>
     <row r="599" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T599" s="6"/>
-      <c r="U599" s="6"/>
+      <c r="Q599"/>
+      <c r="T599" s="3"/>
+      <c r="U599" s="3"/>
+      <c r="V599" s="3"/>
+      <c r="W599"/>
+      <c r="X599" s="10"/>
+      <c r="Y599"/>
+      <c r="Z599"/>
+      <c r="AA599" s="4"/>
+      <c r="AB599" s="4"/>
     </row>
     <row r="600" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T600" s="6"/>
-      <c r="U600" s="6"/>
+      <c r="Q600"/>
+      <c r="T600" s="3"/>
+      <c r="U600" s="3"/>
+      <c r="V600" s="3"/>
+      <c r="W600"/>
+      <c r="X600" s="10"/>
+      <c r="Y600"/>
+      <c r="Z600"/>
+      <c r="AA600" s="4"/>
+      <c r="AB600" s="4"/>
     </row>
     <row r="601" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T601" s="6"/>
-      <c r="U601" s="6"/>
+      <c r="Q601"/>
+      <c r="T601" s="3"/>
+      <c r="U601" s="3"/>
+      <c r="V601" s="3"/>
+      <c r="W601"/>
+      <c r="X601" s="10"/>
+      <c r="Y601"/>
+      <c r="Z601"/>
+      <c r="AA601" s="4"/>
+      <c r="AB601" s="4"/>
     </row>
     <row r="602" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T602" s="6"/>
-      <c r="U602" s="6"/>
+      <c r="Q602"/>
+      <c r="T602" s="3"/>
+      <c r="U602" s="3"/>
+      <c r="V602" s="3"/>
+      <c r="W602"/>
+      <c r="X602" s="10"/>
+      <c r="Y602"/>
+      <c r="Z602"/>
+      <c r="AA602" s="4"/>
+      <c r="AB602" s="4"/>
     </row>
     <row r="603" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T603" s="6"/>
-      <c r="U603" s="6"/>
+      <c r="Q603"/>
+      <c r="T603" s="3"/>
+      <c r="U603" s="3"/>
+      <c r="V603" s="3"/>
+      <c r="W603"/>
+      <c r="X603" s="10"/>
+      <c r="Y603"/>
+      <c r="Z603"/>
+      <c r="AA603" s="4"/>
+      <c r="AB603" s="4"/>
     </row>
     <row r="604" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T604" s="6"/>
-      <c r="U604" s="6"/>
+      <c r="Q604"/>
+      <c r="T604" s="3"/>
+      <c r="U604" s="3"/>
+      <c r="V604" s="3"/>
+      <c r="W604"/>
+      <c r="X604" s="10"/>
+      <c r="Y604"/>
+      <c r="Z604"/>
+      <c r="AA604" s="4"/>
+      <c r="AB604" s="4"/>
     </row>
     <row r="605" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T605" s="6"/>
-      <c r="U605" s="6"/>
+      <c r="Q605"/>
+      <c r="T605" s="3"/>
+      <c r="U605" s="3"/>
+      <c r="V605" s="3"/>
+      <c r="W605"/>
+      <c r="X605" s="10"/>
+      <c r="Y605"/>
+      <c r="Z605"/>
+      <c r="AA605" s="4"/>
+      <c r="AB605" s="4"/>
     </row>
     <row r="606" spans="17:28" x14ac:dyDescent="0.2">
-      <c r="T606" s="6"/>
-      <c r="U606" s="6"/>
+      <c r="Q606"/>
+      <c r="T606" s="3"/>
+      <c r="U606" s="3"/>
+      <c r="V606" s="3"/>
+      <c r="W606"/>
+      <c r="X606" s="10"/>
+      <c r="Y606"/>
+      <c r="Z606"/>
+      <c r="AA606" s="4"/>
+      <c r="AB606" s="4"/>
     </row>
     <row r="607" spans="17:28" x14ac:dyDescent="0.2">
       <c r="T607" s="6"/>
@@ -8440,6 +8414,38 @@
     <row r="628" spans="20:21" x14ac:dyDescent="0.2">
       <c r="T628" s="6"/>
       <c r="U628" s="6"/>
+    </row>
+    <row r="629" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T629" s="6"/>
+      <c r="U629" s="6"/>
+    </row>
+    <row r="630" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T630" s="6"/>
+      <c r="U630" s="6"/>
+    </row>
+    <row r="631" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T631" s="6"/>
+      <c r="U631" s="6"/>
+    </row>
+    <row r="632" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T632" s="6"/>
+      <c r="U632" s="6"/>
+    </row>
+    <row r="633" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T633" s="6"/>
+      <c r="U633" s="6"/>
+    </row>
+    <row r="634" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T634" s="6"/>
+      <c r="U634" s="6"/>
+    </row>
+    <row r="635" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T635" s="6"/>
+      <c r="U635" s="6"/>
+    </row>
+    <row r="636" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T636" s="6"/>
+      <c r="U636" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -8451,12 +8457,9 @@
     <hyperlink ref="F7" r:id="rId5"/>
     <hyperlink ref="F8" r:id="rId6"/>
     <hyperlink ref="F11" r:id="rId7"/>
-    <hyperlink ref="F12" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="5" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>